<commit_message>
working sims + updated example
</commit_message>
<xml_diff>
--- a/inst/extdata/example1.xlsx
+++ b/inst/extdata/example1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/gaelsola/Github-Collabs/mocaredd/inst/extdata/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0187313C-03B8-2844-BB68-86931D34F01F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E047F64E-F354-6E42-95C3-0EC08FD0C6E0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-27320" yWindow="11020" windowWidth="25600" windowHeight="17440" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2920" yWindow="1860" windowWidth="25600" windowHeight="17440" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="user_input_details" sheetId="6" r:id="rId1"/>
@@ -56,7 +56,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="410" uniqueCount="108">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="554" uniqueCount="108">
   <si>
     <t>trans_no</t>
   </si>
@@ -957,10 +957,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:N13"/>
+  <dimension ref="A1:N31"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="127" workbookViewId="0">
-      <selection activeCell="H16" sqref="H16"/>
+    <sheetView tabSelected="1" topLeftCell="A8" zoomScale="127" workbookViewId="0">
+      <selection activeCell="B26" sqref="B26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -1244,232 +1244,862 @@
       <c r="N7" s="2"/>
     </row>
     <row r="8" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A8" s="5">
+      <c r="A8" s="2">
         <v>7</v>
       </c>
-      <c r="B8" s="5" t="s">
+      <c r="B8" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="E8" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="F8" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="G8" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="H8" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="I8">
+        <v>1923.6561915830912</v>
+      </c>
+      <c r="J8">
+        <v>1110.3832615333365</v>
+      </c>
+      <c r="K8" s="2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A9" s="2">
+        <v>8</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="E9" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="F9" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="G9" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="H9" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="I9">
+        <v>0</v>
+      </c>
+      <c r="J9">
+        <v>0</v>
+      </c>
+      <c r="K9" s="2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A10" s="2">
+        <v>9</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="E10" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="F10" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="G10" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="H10" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="I10">
+        <v>0</v>
+      </c>
+      <c r="J10">
+        <v>0</v>
+      </c>
+      <c r="K10" s="2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A11" s="2">
+        <v>10</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="E11" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="F11" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="G11" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="H11" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="I11">
+        <v>0</v>
+      </c>
+      <c r="J11">
+        <v>0</v>
+      </c>
+      <c r="K11" s="2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A12" s="2">
+        <v>11</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="D12" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="E12" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="F12" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="G12" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="H12" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="I12">
+        <v>619.09845559845598</v>
+      </c>
+      <c r="J12">
+        <v>619.09845559845735</v>
+      </c>
+      <c r="K12" s="2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A13" s="2">
+        <v>12</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="E13" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="F13" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="G13" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="H13" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="I13">
+        <v>0</v>
+      </c>
+      <c r="J13">
+        <v>0</v>
+      </c>
+      <c r="K13" s="2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A14" s="2">
+        <v>13</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="D14" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="E14" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="F14" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="G14" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="H14" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="I14">
+        <v>0</v>
+      </c>
+      <c r="J14">
+        <v>0</v>
+      </c>
+      <c r="K14" s="2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="15" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A15" s="2">
+        <v>14</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="C15" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="D15" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="E15" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="F15" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="G15" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="H15" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="I15">
+        <v>0</v>
+      </c>
+      <c r="J15">
+        <v>0</v>
+      </c>
+      <c r="K15" s="2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="16" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A16" s="2">
+        <v>15</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="C16" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="D16" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="E16" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="F16" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="G16" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="H16" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="I16">
+        <v>1270.7069892473119</v>
+      </c>
+      <c r="J16">
+        <v>1272.4172274562584</v>
+      </c>
+      <c r="K16" s="2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="17" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A17" s="2">
+        <v>16</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="C17" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="D17" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="E17" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="F17" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="G17" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="H17" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="I17">
+        <v>640.14165588615788</v>
+      </c>
+      <c r="J17">
+        <v>641.38626053143219</v>
+      </c>
+      <c r="K17" s="2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="18" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A18" s="2">
+        <v>17</v>
+      </c>
+      <c r="B18" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="C18" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="D18" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="E18" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="F18" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="G18" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="H18" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="I18">
+        <v>0</v>
+      </c>
+      <c r="J18">
+        <v>0</v>
+      </c>
+      <c r="K18" s="2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="19" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A19" s="2">
+        <v>18</v>
+      </c>
+      <c r="B19" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="C19" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="D19" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="E19" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="F19" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="G19" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="H19" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="I19">
+        <v>0</v>
+      </c>
+      <c r="J19">
+        <v>0</v>
+      </c>
+      <c r="K19" s="2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="20" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A20" s="2">
+        <v>19</v>
+      </c>
+      <c r="B20" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="C20" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="D20" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="E20" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="F20" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="G20" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="H20" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="I20">
+        <v>637.65851905104239</v>
+      </c>
+      <c r="J20">
+        <v>637.65851905104239</v>
+      </c>
+      <c r="K20" s="2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="21" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A21" s="2">
+        <v>20</v>
+      </c>
+      <c r="B21" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="C21" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="D21" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="E21" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="F21" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="G21" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="H21" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="I21">
+        <v>0</v>
+      </c>
+      <c r="J21">
+        <v>0</v>
+      </c>
+      <c r="K21" s="2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="22" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A22" s="2">
+        <v>21</v>
+      </c>
+      <c r="B22" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="C22" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="D22" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="E22" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="F22" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="G22" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="H22" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="I22">
+        <v>0</v>
+      </c>
+      <c r="J22">
+        <v>0</v>
+      </c>
+      <c r="K22" s="2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="23" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A23" s="2">
+        <v>22</v>
+      </c>
+      <c r="B23" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="C23" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="D23" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="E23" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="F23" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="G23" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="H23" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="I23">
+        <v>640.14165588615788</v>
+      </c>
+      <c r="J23">
+        <v>641.38626053143219</v>
+      </c>
+      <c r="K23" s="2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="24" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A24" s="2">
+        <v>23</v>
+      </c>
+      <c r="B24" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="C24" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="D24" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="E24" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="F24" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="G24" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="H24" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="I24">
+        <v>3093.5016077170417</v>
+      </c>
+      <c r="J24">
+        <v>1385.2330193886739</v>
+      </c>
+      <c r="K24" s="2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="25" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A25" s="2">
+        <v>24</v>
+      </c>
+      <c r="B25" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="C25" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="D25" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="E25" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="F25" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="G25" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="H25" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="I25">
+        <v>159.29007633587787</v>
+      </c>
+      <c r="J25">
+        <v>159.29007633587784</v>
+      </c>
+      <c r="K25" s="2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="26" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A26" s="2">
+        <v>25</v>
+      </c>
+      <c r="B26" s="5" t="s">
         <v>73</v>
       </c>
-      <c r="C8" s="5" t="s">
+      <c r="C26" s="5" t="s">
         <v>59</v>
       </c>
-      <c r="D8" s="5" t="s">
+      <c r="D26" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="E8" s="5" t="s">
+      <c r="E26" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="F8" s="5" t="s">
+      <c r="F26" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="G8" s="5" t="s">
+      <c r="G26" s="5" t="s">
         <v>91</v>
       </c>
-      <c r="H8" s="5" t="s">
+      <c r="H26" s="5" t="s">
         <v>92</v>
       </c>
-      <c r="I8" s="5">
+      <c r="I26" s="5">
         <v>437</v>
       </c>
-      <c r="J8" s="5">
+      <c r="J26" s="5">
         <v>206.91</v>
       </c>
-      <c r="K8" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="L8" s="5"/>
-      <c r="M8" s="5"/>
-      <c r="N8" s="5"/>
-    </row>
-    <row r="9" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A9" s="5">
-        <v>8</v>
-      </c>
-      <c r="B9" s="5" t="s">
+      <c r="K26" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="L26" s="5"/>
+      <c r="M26" s="5"/>
+      <c r="N26" s="5"/>
+    </row>
+    <row r="27" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A27" s="2">
+        <v>26</v>
+      </c>
+      <c r="B27" s="5" t="s">
         <v>74</v>
       </c>
-      <c r="C9" s="5" t="s">
+      <c r="C27" s="5" t="s">
         <v>59</v>
       </c>
-      <c r="D9" s="5" t="s">
+      <c r="D27" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="E9" s="5" t="s">
+      <c r="E27" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="F9" s="5" t="s">
+      <c r="F27" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="G9" s="5" t="s">
+      <c r="G27" s="5" t="s">
         <v>101</v>
       </c>
-      <c r="H9" s="5" t="s">
+      <c r="H27" s="5" t="s">
         <v>93</v>
       </c>
-      <c r="I9" s="5">
+      <c r="I27" s="5">
         <v>303.89</v>
       </c>
-      <c r="J9" s="5">
+      <c r="J27" s="5">
         <v>160.78</v>
       </c>
-      <c r="K9" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="L9" s="5"/>
-      <c r="M9" s="5"/>
-      <c r="N9" s="5"/>
-    </row>
-    <row r="10" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A10" s="5">
-        <v>9</v>
-      </c>
-      <c r="B10" s="5" t="s">
+      <c r="K27" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="L27" s="5"/>
+      <c r="M27" s="5"/>
+      <c r="N27" s="5"/>
+    </row>
+    <row r="28" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A28" s="2">
+        <v>27</v>
+      </c>
+      <c r="B28" s="5" t="s">
         <v>75</v>
       </c>
-      <c r="C10" s="5" t="s">
+      <c r="C28" s="5" t="s">
         <v>59</v>
       </c>
-      <c r="D10" s="5" t="s">
+      <c r="D28" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="E10" s="5" t="s">
+      <c r="E28" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="F10" s="5" t="s">
+      <c r="F28" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="G10" s="5" t="s">
+      <c r="G28" s="5" t="s">
         <v>102</v>
       </c>
-      <c r="H10" s="5" t="s">
+      <c r="H28" s="5" t="s">
         <v>94</v>
       </c>
-      <c r="I10" s="6">
+      <c r="I28" s="6">
         <v>1152.8499999999999</v>
       </c>
-      <c r="J10" s="5">
+      <c r="J28" s="5">
         <v>312.83</v>
       </c>
-      <c r="K10" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="L10" s="5"/>
-      <c r="M10" s="5"/>
-      <c r="N10" s="5"/>
-    </row>
-    <row r="11" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A11" s="5">
-        <v>10</v>
-      </c>
-      <c r="B11" s="5" t="s">
+      <c r="K28" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="L28" s="5"/>
+      <c r="M28" s="5"/>
+      <c r="N28" s="5"/>
+    </row>
+    <row r="29" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A29" s="2">
+        <v>28</v>
+      </c>
+      <c r="B29" s="5" t="s">
         <v>76</v>
       </c>
-      <c r="C11" s="5" t="s">
+      <c r="C29" s="5" t="s">
         <v>59</v>
       </c>
-      <c r="D11" s="5" t="s">
+      <c r="D29" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="E11" s="5" t="s">
+      <c r="E29" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="F11" s="5" t="s">
+      <c r="F29" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="G11" s="5" t="s">
+      <c r="G29" s="5" t="s">
         <v>103</v>
       </c>
-      <c r="H11" s="5" t="s">
+      <c r="H29" s="5" t="s">
         <v>95</v>
       </c>
-      <c r="I11" s="6">
+      <c r="I29" s="6">
         <v>1269.99</v>
       </c>
-      <c r="J11" s="5">
+      <c r="J29" s="5">
         <v>307.97000000000003</v>
       </c>
-      <c r="K11" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="L11" s="5"/>
-      <c r="M11" s="5"/>
-      <c r="N11" s="5"/>
-    </row>
-    <row r="12" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A12" s="5">
-        <v>11</v>
-      </c>
-      <c r="B12" s="5" t="s">
+      <c r="K29" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="L29" s="5"/>
+      <c r="M29" s="5"/>
+      <c r="N29" s="5"/>
+    </row>
+    <row r="30" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A30" s="2">
+        <v>29</v>
+      </c>
+      <c r="B30" s="5" t="s">
         <v>77</v>
       </c>
-      <c r="C12" s="5" t="s">
+      <c r="C30" s="5" t="s">
         <v>59</v>
       </c>
-      <c r="D12" s="5" t="s">
+      <c r="D30" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="E12" s="5" t="s">
+      <c r="E30" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="F12" s="5" t="s">
+      <c r="F30" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="G12" s="5" t="s">
+      <c r="G30" s="5" t="s">
         <v>104</v>
       </c>
-      <c r="H12" s="5" t="s">
+      <c r="H30" s="5" t="s">
         <v>96</v>
       </c>
-      <c r="I12" s="6">
+      <c r="I30" s="6">
         <v>1293</v>
       </c>
-      <c r="J12" s="5">
+      <c r="J30" s="5">
         <v>317.68</v>
       </c>
-      <c r="K12" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="L12" s="5"/>
-      <c r="M12" s="5"/>
-      <c r="N12" s="5"/>
-    </row>
-    <row r="13" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A13" s="5">
-        <v>12</v>
-      </c>
-      <c r="B13" s="5" t="s">
+      <c r="K30" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="L30" s="5"/>
+      <c r="M30" s="5"/>
+      <c r="N30" s="5"/>
+    </row>
+    <row r="31" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A31" s="2">
+        <v>30</v>
+      </c>
+      <c r="B31" s="5" t="s">
         <v>78</v>
       </c>
-      <c r="C13" s="5" t="s">
+      <c r="C31" s="5" t="s">
         <v>59</v>
       </c>
-      <c r="D13" s="5" t="s">
+      <c r="D31" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="E13" s="5" t="s">
+      <c r="E31" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="F13" s="5" t="s">
+      <c r="F31" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="G13" s="5" t="s">
+      <c r="G31" s="5" t="s">
         <v>105</v>
       </c>
-      <c r="H13" s="5" t="s">
+      <c r="H31" s="5" t="s">
         <v>97</v>
       </c>
-      <c r="I13" s="5">
+      <c r="I31" s="5">
         <v>79.849999999999994</v>
       </c>
-      <c r="J13" s="5">
+      <c r="J31" s="5">
         <v>35.53</v>
       </c>
-      <c r="K13" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="L13" s="5"/>
-      <c r="M13" s="5"/>
-      <c r="N13" s="5"/>
+      <c r="K31" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="L31" s="5"/>
+      <c r="M31" s="5"/>
+      <c r="N31" s="5"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1483,7 +2113,7 @@
   </sheetPr>
   <dimension ref="A1:K61"/>
   <sheetViews>
-    <sheetView topLeftCell="A11" zoomScale="109" workbookViewId="0">
+    <sheetView topLeftCell="A32" zoomScale="109" workbookViewId="0">
       <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
re-arranged MCS functions into carbon, emission and period (C, E, P)
</commit_message>
<xml_diff>
--- a/inst/extdata/example1.xlsx
+++ b/inst/extdata/example1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/gaelsola/Github-Collabs/mocaredd/inst/extdata/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2C5F80CD-0349-A944-9AE6-D295B646E9B3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A169BFB3-D7F3-3D4D-98F4-401335B96DF7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2920" yWindow="1860" windowWidth="25600" windowHeight="17440" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2920" yWindow="1860" windowWidth="25600" windowHeight="17440" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="user_input_details" sheetId="6" r:id="rId1"/>
@@ -879,8 +879,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F8C6B7CA-5E2C-284E-A17C-8E0897ACEFB0}">
   <dimension ref="A1:I2"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="186" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView zoomScale="186" workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -3005,8 +3005,8 @@
   </sheetPr>
   <dimension ref="A1:K43"/>
   <sheetViews>
-    <sheetView topLeftCell="A20" zoomScale="109" workbookViewId="0">
-      <selection activeCell="I46" sqref="I46"/>
+    <sheetView tabSelected="1" topLeftCell="A20" zoomScale="109" workbookViewId="0">
+      <selection activeCell="D45" sqref="D45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>

</xml_diff>

<commit_message>
Simplified template and ER calculations
</commit_message>
<xml_diff>
--- a/inst/extdata/example1.xlsx
+++ b/inst/extdata/example1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/gaelsola/Github-Collabs/mocaredd/inst/extdata/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A169BFB3-D7F3-3D4D-98F4-401335B96DF7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1D9B38AF-3742-E64F-8CD7-B8CE274984CC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2920" yWindow="1860" windowWidth="25600" windowHeight="17440" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2920" yWindow="1860" windowWidth="25600" windowHeight="17440" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="user_input_details" sheetId="6" r:id="rId1"/>
@@ -75,7 +75,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="851" uniqueCount="103">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="846" uniqueCount="100">
   <si>
     <t>trans_no</t>
   </si>
@@ -257,30 +257,18 @@
     <t>T1</t>
   </si>
   <si>
-    <t>reference</t>
-  </si>
-  <si>
     <t>T2</t>
   </si>
   <si>
-    <t>monitoring</t>
-  </si>
-  <si>
     <t>T3</t>
   </si>
   <si>
     <t>T4</t>
   </si>
   <si>
-    <t>period_combinations</t>
-  </si>
-  <si>
     <t>trans_period</t>
   </si>
   <si>
-    <t>R1</t>
-  </si>
-  <si>
     <t>M1</t>
   </si>
   <si>
@@ -384,6 +372,9 @@
   </si>
   <si>
     <t>AGB, BGB, DW</t>
+  </si>
+  <si>
+    <t>REF</t>
   </si>
 </sst>
 </file>
@@ -800,34 +791,34 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A1" s="7" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="B1" s="7" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A2" s="7" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="B2" s="7" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A3" s="7" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A4" s="7" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="B4" s="7" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.15">
@@ -835,39 +826,39 @@
         <v>39</v>
       </c>
       <c r="B5" s="7" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
     </row>
     <row r="6" spans="1:2" ht="28" x14ac:dyDescent="0.15">
       <c r="A6" s="7" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
       <c r="B6" s="19" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
     </row>
     <row r="7" spans="1:2" ht="28" x14ac:dyDescent="0.15">
       <c r="A7" s="7" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="B7" s="19" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A8" s="7" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="B8" s="7" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A9" s="7" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="B9" s="7" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
     </row>
   </sheetData>
@@ -894,31 +885,31 @@
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A1" s="7" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="B1" s="7" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="C1" s="7" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="D1" s="7" t="s">
         <v>39</v>
       </c>
       <c r="E1" s="7" t="s">
+        <v>88</v>
+      </c>
+      <c r="F1" s="7" t="s">
+        <v>95</v>
+      </c>
+      <c r="G1" s="7" t="s">
+        <v>94</v>
+      </c>
+      <c r="H1" s="7" t="s">
+        <v>90</v>
+      </c>
+      <c r="I1" s="7" t="s">
         <v>92</v>
-      </c>
-      <c r="F1" s="7" t="s">
-        <v>99</v>
-      </c>
-      <c r="G1" s="7" t="s">
-        <v>98</v>
-      </c>
-      <c r="H1" s="7" t="s">
-        <v>94</v>
-      </c>
-      <c r="I1" s="7" t="s">
-        <v>96</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.15">
@@ -938,7 +929,7 @@
         <v>52</v>
       </c>
       <c r="F2" s="7" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
       <c r="G2" t="b">
         <v>1</v>
@@ -957,18 +948,18 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A7F899DA-46D5-A143-AFBA-1E1D48143306}">
-  <dimension ref="A1:E5"/>
+  <dimension ref="A1:D5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B7" sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="5" max="5" width="17.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A1" s="7" t="s">
         <v>55</v>
       </c>
@@ -981,11 +972,8 @@
       <c r="D1" s="7" t="s">
         <v>58</v>
       </c>
-      <c r="E1" s="7" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.15">
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A2" s="7" t="s">
         <v>59</v>
       </c>
@@ -996,15 +984,12 @@
         <v>2014</v>
       </c>
       <c r="D2" s="7" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A3" s="7" t="s">
         <v>60</v>
-      </c>
-      <c r="E2" s="7" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A3" s="7" t="s">
-        <v>61</v>
       </c>
       <c r="B3" s="7">
         <v>2019</v>
@@ -1013,15 +998,12 @@
         <v>2019</v>
       </c>
       <c r="D3" s="7" t="s">
-        <v>62</v>
-      </c>
-      <c r="E3" s="7" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.15">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A4" s="7" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="B4" s="7">
         <v>2020</v>
@@ -1030,15 +1012,12 @@
         <v>2020</v>
       </c>
       <c r="D4" s="7" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A5" s="7" t="s">
         <v>62</v>
-      </c>
-      <c r="E4" s="7" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A5" s="7" t="s">
-        <v>64</v>
       </c>
       <c r="B5" s="7">
         <v>2021</v>
@@ -1047,10 +1026,7 @@
         <v>2021</v>
       </c>
       <c r="D5" s="7" t="s">
-        <v>62</v>
-      </c>
-      <c r="E5" s="7" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
     </row>
   </sheetData>
@@ -1085,7 +1061,7 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>2</v>
@@ -1364,7 +1340,7 @@
         <v>T2_DF_open</v>
       </c>
       <c r="C8" s="9" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D8" s="9" t="s">
         <v>13</v>
@@ -1403,7 +1379,7 @@
         <v>T2_DF_ev_wet_closed</v>
       </c>
       <c r="C9" s="9" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D9" s="9" t="s">
         <v>13</v>
@@ -1442,7 +1418,7 @@
         <v>T2_DF_ev_moist_closed</v>
       </c>
       <c r="C10" s="9" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D10" s="9" t="s">
         <v>13</v>
@@ -1481,7 +1457,7 @@
         <v>T2_DF_md_moist_closed_se</v>
       </c>
       <c r="C11" s="9" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D11" s="9" t="s">
         <v>13</v>
@@ -1520,7 +1496,7 @@
         <v>T2_DF_md_moist_closed_nw</v>
       </c>
       <c r="C12" s="9" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D12" s="9" t="s">
         <v>13</v>
@@ -1559,7 +1535,7 @@
         <v>T2_DF_ev_upland</v>
       </c>
       <c r="C13" s="9" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D13" s="9" t="s">
         <v>13</v>
@@ -1598,7 +1574,7 @@
         <v>T3_DF_open</v>
       </c>
       <c r="C14" s="12" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="D14" s="12" t="s">
         <v>13</v>
@@ -1637,7 +1613,7 @@
         <v>T3_DF_ev_wet_closed</v>
       </c>
       <c r="C15" s="12" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="D15" s="12" t="s">
         <v>13</v>
@@ -1676,7 +1652,7 @@
         <v>T3_DF_ev_moist_closed</v>
       </c>
       <c r="C16" s="12" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="D16" s="12" t="s">
         <v>13</v>
@@ -1715,7 +1691,7 @@
         <v>T3_DF_md_moist_closed_se</v>
       </c>
       <c r="C17" s="12" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="D17" s="12" t="s">
         <v>13</v>
@@ -1754,7 +1730,7 @@
         <v>T3_DF_md_moist_closed_nw</v>
       </c>
       <c r="C18" s="12" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="D18" s="12" t="s">
         <v>13</v>
@@ -1793,7 +1769,7 @@
         <v>T3_DF_ev_upland</v>
       </c>
       <c r="C19" s="12" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="D19" s="12" t="s">
         <v>13</v>
@@ -1832,7 +1808,7 @@
         <v>T4_DF_open</v>
       </c>
       <c r="C20" s="9" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="D20" s="9" t="s">
         <v>13</v>
@@ -1871,7 +1847,7 @@
         <v>T4_DF_ev_wet_closed</v>
       </c>
       <c r="C21" s="9" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="D21" s="9" t="s">
         <v>13</v>
@@ -1910,7 +1886,7 @@
         <v>T4_DF_ev_moist_closed</v>
       </c>
       <c r="C22" s="9" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="D22" s="9" t="s">
         <v>13</v>
@@ -1949,7 +1925,7 @@
         <v>T4_DF_md_moist_closed_se</v>
       </c>
       <c r="C23" s="9" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="D23" s="9" t="s">
         <v>13</v>
@@ -1988,7 +1964,7 @@
         <v>T4_DF_md_moist_closed_nw</v>
       </c>
       <c r="C24" s="9" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="D24" s="9" t="s">
         <v>13</v>
@@ -2027,7 +2003,7 @@
         <v>T4_DF_ev_upland</v>
       </c>
       <c r="C25" s="9" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="D25" s="9" t="s">
         <v>13</v>
@@ -2078,10 +2054,10 @@
         <v>15</v>
       </c>
       <c r="G26" s="15" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="H26" s="15" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="I26" s="15">
         <v>437</v>
@@ -2117,10 +2093,10 @@
         <v>20</v>
       </c>
       <c r="G27" s="15" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="H27" s="15" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="I27" s="15">
         <v>303.89</v>
@@ -2156,10 +2132,10 @@
         <v>23</v>
       </c>
       <c r="G28" s="15" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="H28" s="15" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="I28" s="16">
         <v>1152.8499999999999</v>
@@ -2195,10 +2171,10 @@
         <v>26</v>
       </c>
       <c r="G29" s="15" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="H29" s="15" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="I29" s="16">
         <v>1269.99</v>
@@ -2234,10 +2210,10 @@
         <v>29</v>
       </c>
       <c r="G30" s="15" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="H30" s="15" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="I30" s="16">
         <v>1293</v>
@@ -2273,10 +2249,10 @@
         <v>32</v>
       </c>
       <c r="G31" s="15" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
       <c r="H31" s="15" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="I31" s="15">
         <v>79.849999999999994</v>
@@ -2300,7 +2276,7 @@
         <v>T2_DG_open</v>
       </c>
       <c r="C32" s="17" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D32" s="17" t="s">
         <v>34</v>
@@ -2312,10 +2288,10 @@
         <v>15</v>
       </c>
       <c r="G32" s="17" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="H32" s="17" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="I32" s="10">
         <v>0</v>
@@ -2339,7 +2315,7 @@
         <v>T2_DG_ev_wet_closed</v>
       </c>
       <c r="C33" s="17" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D33" s="17" t="s">
         <v>34</v>
@@ -2351,10 +2327,10 @@
         <v>20</v>
       </c>
       <c r="G33" s="17" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="H33" s="17" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="I33" s="10">
         <v>607.16865869853905</v>
@@ -2378,7 +2354,7 @@
         <v>T2_DG_ev_moist_closed</v>
       </c>
       <c r="C34" s="17" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D34" s="17" t="s">
         <v>34</v>
@@ -2390,10 +2366,10 @@
         <v>23</v>
       </c>
       <c r="G34" s="17" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="H34" s="17" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="I34" s="10">
         <v>1281.76734104046</v>
@@ -2417,7 +2393,7 @@
         <v>T2_DG_md_moist_closed_se</v>
       </c>
       <c r="C35" s="17" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D35" s="17" t="s">
         <v>34</v>
@@ -2429,10 +2405,10 @@
         <v>26</v>
       </c>
       <c r="G35" s="17" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="H35" s="17" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="I35" s="10">
         <v>4425.8122943927001</v>
@@ -2456,7 +2432,7 @@
         <v>T2_DG_md_moist_closed_nw</v>
       </c>
       <c r="C36" s="17" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D36" s="17" t="s">
         <v>34</v>
@@ -2468,10 +2444,10 @@
         <v>29</v>
       </c>
       <c r="G36" s="17" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="H36" s="17" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="I36" s="10">
         <v>3095.4922779922799</v>
@@ -2495,7 +2471,7 @@
         <v>T2_DG_ev_upland</v>
       </c>
       <c r="C37" s="17" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D37" s="17" t="s">
         <v>34</v>
@@ -2507,10 +2483,10 @@
         <v>32</v>
       </c>
       <c r="G37" s="17" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
       <c r="H37" s="17" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="I37" s="10">
         <v>0</v>
@@ -2534,7 +2510,7 @@
         <v>T3_DG_open</v>
       </c>
       <c r="C38" s="15" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="D38" s="15" t="s">
         <v>34</v>
@@ -2546,10 +2522,10 @@
         <v>15</v>
       </c>
       <c r="G38" s="15" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="H38" s="15" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="I38" s="13">
         <v>0</v>
@@ -2573,7 +2549,7 @@
         <v>T3_DG_ev_wet_closed</v>
       </c>
       <c r="C39" s="15" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="D39" s="15" t="s">
         <v>34</v>
@@ -2585,10 +2561,10 @@
         <v>20</v>
       </c>
       <c r="G39" s="15" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="H39" s="15" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="I39" s="13">
         <v>0</v>
@@ -2612,7 +2588,7 @@
         <v>T3_DG_ev_moist_closed</v>
       </c>
       <c r="C40" s="15" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="D40" s="15" t="s">
         <v>34</v>
@@ -2624,10 +2600,10 @@
         <v>23</v>
       </c>
       <c r="G40" s="15" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="H40" s="15" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="I40" s="13">
         <v>637.65851905104239</v>
@@ -2651,7 +2627,7 @@
         <v>T3_DG_md_moist_closed_se</v>
       </c>
       <c r="C41" s="15" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="D41" s="15" t="s">
         <v>34</v>
@@ -2663,10 +2639,10 @@
         <v>26</v>
       </c>
       <c r="G41" s="15" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="H41" s="15" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="I41" s="13">
         <v>1280.2833117723158</v>
@@ -2690,7 +2666,7 @@
         <v>T3_DG_md_moist_closed_nw</v>
       </c>
       <c r="C42" s="15" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="D42" s="15" t="s">
         <v>34</v>
@@ -2702,10 +2678,10 @@
         <v>29</v>
       </c>
       <c r="G42" s="15" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="H42" s="15" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="I42" s="13">
         <v>618.70032154340834</v>
@@ -2729,7 +2705,7 @@
         <v>T3_DG_ev_upland</v>
       </c>
       <c r="C43" s="15" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="D43" s="15" t="s">
         <v>34</v>
@@ -2741,10 +2717,10 @@
         <v>32</v>
       </c>
       <c r="G43" s="15" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
       <c r="H43" s="15" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="I43" s="13">
         <v>0</v>
@@ -2768,7 +2744,7 @@
         <v>T4_DG_open</v>
       </c>
       <c r="C44" s="17" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="D44" s="17" t="s">
         <v>34</v>
@@ -2780,10 +2756,10 @@
         <v>15</v>
       </c>
       <c r="G44" s="17" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="H44" s="17" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="I44" s="10">
         <v>1280.2833117723158</v>
@@ -2807,7 +2783,7 @@
         <v>T4_DG_ev_wet_closed</v>
       </c>
       <c r="C45" s="17" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="D45" s="17" t="s">
         <v>34</v>
@@ -2819,10 +2795,10 @@
         <v>20</v>
       </c>
       <c r="G45" s="17" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="H45" s="17" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="I45" s="10">
         <v>606.36339522546416</v>
@@ -2846,7 +2822,7 @@
         <v>T4_DG_ev_moist_closed</v>
       </c>
       <c r="C46" s="17" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="D46" s="17" t="s">
         <v>34</v>
@@ -2858,10 +2834,10 @@
         <v>23</v>
       </c>
       <c r="G46" s="17" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="H46" s="17" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="I46" s="10">
         <v>637.65851905104239</v>
@@ -2885,7 +2861,7 @@
         <v>T4_DG_md_moist_closed_se</v>
       </c>
       <c r="C47" s="17" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="D47" s="17" t="s">
         <v>34</v>
@@ -2897,10 +2873,10 @@
         <v>26</v>
       </c>
       <c r="G47" s="17" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="H47" s="17" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="I47" s="10">
         <v>2491.1585170268313</v>
@@ -2924,7 +2900,7 @@
         <v>T4_DG_md_moist_closed_nw</v>
       </c>
       <c r="C48" s="17" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="D48" s="17" t="s">
         <v>34</v>
@@ -2936,10 +2912,10 @@
         <v>29</v>
       </c>
       <c r="G48" s="17" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="H48" s="17" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="I48" s="10">
         <v>3687.6546466624318</v>
@@ -2963,7 +2939,7 @@
         <v>T4_DG_ev_upland</v>
       </c>
       <c r="C49" s="17" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="D49" s="17" t="s">
         <v>34</v>
@@ -2975,10 +2951,10 @@
         <v>32</v>
       </c>
       <c r="G49" s="17" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
       <c r="H49" s="17" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="I49" s="10">
         <v>318.58015267175574</v>
@@ -3005,7 +2981,7 @@
   </sheetPr>
   <dimension ref="A1:K43"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A20" zoomScale="109" workbookViewId="0">
+    <sheetView zoomScale="109" workbookViewId="0">
       <selection activeCell="D45" sqref="D45"/>
     </sheetView>
   </sheetViews>
@@ -4146,13 +4122,13 @@
         <v>DG_ratio_dg_open</v>
       </c>
       <c r="C38" s="18" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="D38" s="18" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="E38" s="18" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="F38" s="18">
         <f>1-0.48</f>
@@ -4162,7 +4138,7 @@
         <v>7.2999999999999995E-2</v>
       </c>
       <c r="H38" s="18" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
       <c r="I38" s="18">
         <f>(F38*(1-F38)/(G38*G38)-1)*F38</f>
@@ -4183,13 +4159,13 @@
         <v>DG_ratio_dg_ev_wet_closed</v>
       </c>
       <c r="C39" s="18" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="D39" s="18" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="E39" s="18" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="F39" s="18">
         <f>1-0.3</f>
@@ -4199,7 +4175,7 @@
         <v>2.5999999999999999E-2</v>
       </c>
       <c r="H39" s="18" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
       <c r="I39" s="18">
         <f t="shared" ref="I39:I43" si="0">(F39*(1-F39)/(G39*G39)-1)*F39</f>
@@ -4220,13 +4196,13 @@
         <v>DG_ratio_dg_ev_moist_closed</v>
       </c>
       <c r="C40" s="18" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="D40" s="18" t="s">
+        <v>78</v>
+      </c>
+      <c r="E40" s="18" t="s">
         <v>82</v>
-      </c>
-      <c r="E40" s="18" t="s">
-        <v>86</v>
       </c>
       <c r="F40" s="18">
         <f t="shared" ref="F40:F43" si="2">1-0.3</f>
@@ -4236,7 +4212,7 @@
         <v>2.5999999999999999E-2</v>
       </c>
       <c r="H40" s="18" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
       <c r="I40" s="18">
         <f t="shared" si="0"/>
@@ -4257,13 +4233,13 @@
         <v>DG_ratio_dg_md_moist_closed_se</v>
       </c>
       <c r="C41" s="18" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="D41" s="18" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="E41" s="18" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="F41" s="18">
         <f t="shared" si="2"/>
@@ -4273,7 +4249,7 @@
         <v>2.5999999999999999E-2</v>
       </c>
       <c r="H41" s="18" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
       <c r="I41" s="18">
         <f t="shared" si="0"/>
@@ -4294,13 +4270,13 @@
         <v>DG_ratio_dg_md_moist_closed_nw</v>
       </c>
       <c r="C42" s="18" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="D42" s="18" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="E42" s="18" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="F42" s="18">
         <f t="shared" si="2"/>
@@ -4310,7 +4286,7 @@
         <v>2.5999999999999999E-2</v>
       </c>
       <c r="H42" s="18" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
       <c r="I42" s="18">
         <f t="shared" si="0"/>
@@ -4331,13 +4307,13 @@
         <v>DG_ratio_dg_ev_upland</v>
       </c>
       <c r="C43" s="18" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
       <c r="D43" s="18" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="E43" s="18" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="F43" s="18">
         <f t="shared" si="2"/>
@@ -4347,7 +4323,7 @@
         <v>2.5999999999999999E-2</v>
       </c>
       <c r="H43" s="18" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
       <c r="I43" s="18">
         <f t="shared" si="0"/>
@@ -5540,10 +5516,10 @@
         <v>AGB_dg_open</v>
       </c>
       <c r="C38" s="5" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="D38" s="5" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="E38" s="5" t="s">
         <v>46</v>
@@ -5570,10 +5546,10 @@
         <v>AGB_dg_ev_wet_closed</v>
       </c>
       <c r="C39" s="5" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="D39" s="5" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="E39" s="5" t="s">
         <v>46</v>
@@ -5600,10 +5576,10 @@
         <v>AGB_dg_ev_moist_closed</v>
       </c>
       <c r="C40" s="5" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="D40" s="5" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="E40" s="5" t="s">
         <v>46</v>
@@ -5630,10 +5606,10 @@
         <v>AGB_dg_md_moist_closed_se</v>
       </c>
       <c r="C41" s="5" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="D41" s="5" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="E41" s="5" t="s">
         <v>46</v>
@@ -5660,10 +5636,10 @@
         <v>AGB_dg_md_moist_closed_nw</v>
       </c>
       <c r="C42" s="5" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="D42" s="5" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="E42" s="5" t="s">
         <v>46</v>
@@ -5690,10 +5666,10 @@
         <v>AGB_dg_ev_upland</v>
       </c>
       <c r="C43" s="5" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
       <c r="D43" s="5" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="E43" s="5" t="s">
         <v>46</v>
@@ -5720,10 +5696,10 @@
         <v>BGB_dg_open</v>
       </c>
       <c r="C44" s="6" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="D44" s="6" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="E44" s="6" t="s">
         <v>48</v>
@@ -5750,10 +5726,10 @@
         <v>BGB_dg_ev_wet_closed</v>
       </c>
       <c r="C45" s="6" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="D45" s="6" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="E45" s="6" t="s">
         <v>48</v>
@@ -5780,10 +5756,10 @@
         <v>BGB_dg_ev_moist_closed</v>
       </c>
       <c r="C46" s="6" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="D46" s="6" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="E46" s="6" t="s">
         <v>48</v>
@@ -5810,10 +5786,10 @@
         <v>BGB_dg_md_moist_closed_se</v>
       </c>
       <c r="C47" s="6" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="D47" s="6" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="E47" s="6" t="s">
         <v>48</v>
@@ -5840,10 +5816,10 @@
         <v>BGB_dg_md_moist_closed_nw</v>
       </c>
       <c r="C48" s="6" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="D48" s="6" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="E48" s="6" t="s">
         <v>48</v>
@@ -5870,10 +5846,10 @@
         <v>BGB_dg_ev_upland</v>
       </c>
       <c r="C49" s="6" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
       <c r="D49" s="6" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="E49" s="6" t="s">
         <v>48</v>
@@ -5900,10 +5876,10 @@
         <v>DW_dg_open</v>
       </c>
       <c r="C50" s="5" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="D50" s="5" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="E50" s="5" t="s">
         <v>49</v>
@@ -5930,10 +5906,10 @@
         <v>DW_dg_ev_wet_closed</v>
       </c>
       <c r="C51" s="5" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="D51" s="5" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="E51" s="5" t="s">
         <v>49</v>
@@ -5960,10 +5936,10 @@
         <v>DW_dg_ev_moist_closed</v>
       </c>
       <c r="C52" s="5" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="D52" s="5" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="E52" s="5" t="s">
         <v>49</v>
@@ -5990,10 +5966,10 @@
         <v>DW_dg_md_moist_closed_se</v>
       </c>
       <c r="C53" s="5" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="D53" s="5" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="E53" s="5" t="s">
         <v>49</v>
@@ -6020,10 +5996,10 @@
         <v>DW_dg_md_moist_closed_nw</v>
       </c>
       <c r="C54" s="5" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="D54" s="5" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="E54" s="5" t="s">
         <v>49</v>
@@ -6050,10 +6026,10 @@
         <v>DW_dg_ev_upland</v>
       </c>
       <c r="C55" s="5" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
       <c r="D55" s="5" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="E55" s="5" t="s">
         <v>49</v>
@@ -6080,18 +6056,18 @@
         <v>DG_ratio_dg_open</v>
       </c>
       <c r="C56" s="6" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="D56" s="6" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="E56" s="6" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="F56" s="6"/>
       <c r="G56" s="6"/>
       <c r="H56" s="6" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
       <c r="I56" s="6">
         <f>1-0.48</f>
@@ -6111,18 +6087,18 @@
         <v>DG_ratio_dg_ev_wet_closed</v>
       </c>
       <c r="C57" s="6" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="D57" s="6" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="E57" s="6" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="F57" s="6"/>
       <c r="G57" s="6"/>
       <c r="H57" s="6" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
       <c r="I57" s="6">
         <f>1-0.3</f>
@@ -6142,18 +6118,18 @@
         <v>DG_ratio_dg_ev_moist_closed</v>
       </c>
       <c r="C58" s="6" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="D58" s="6" t="s">
+        <v>78</v>
+      </c>
+      <c r="E58" s="6" t="s">
         <v>82</v>
-      </c>
-      <c r="E58" s="6" t="s">
-        <v>86</v>
       </c>
       <c r="F58" s="6"/>
       <c r="G58" s="6"/>
       <c r="H58" s="6" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
       <c r="I58" s="6">
         <f t="shared" ref="I58:I61" si="0">1-0.3</f>
@@ -6173,18 +6149,18 @@
         <v>DG_ratio_dg_md_moist_closed_se</v>
       </c>
       <c r="C59" s="6" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="D59" s="6" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="E59" s="6" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="F59" s="6"/>
       <c r="G59" s="6"/>
       <c r="H59" s="6" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
       <c r="I59" s="6">
         <f t="shared" si="0"/>
@@ -6204,18 +6180,18 @@
         <v>DG_ratio_dg_md_moist_closed_nw</v>
       </c>
       <c r="C60" s="6" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="D60" s="6" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="E60" s="6" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="F60" s="6"/>
       <c r="G60" s="6"/>
       <c r="H60" s="6" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
       <c r="I60" s="6">
         <f t="shared" si="0"/>
@@ -6235,18 +6211,18 @@
         <v>DG_ratio_dg_ev_upland</v>
       </c>
       <c r="C61" s="6" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
       <c r="D61" s="6" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="E61" s="6" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="F61" s="6"/>
       <c r="G61" s="6"/>
       <c r="H61" s="6" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
       <c r="I61" s="6">
         <f t="shared" si="0"/>

</xml_diff>

<commit_message>
cleaned functions based on R CMD checks
</commit_message>
<xml_diff>
--- a/inst/extdata/example1.xlsx
+++ b/inst/extdata/example1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/gaelsola/Github-Collabs/mocaredd/inst/extdata/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1D9B38AF-3742-E64F-8CD7-B8CE274984CC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4BAEFECB-49DA-D541-9A48-799527531B36}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2920" yWindow="1860" windowWidth="25600" windowHeight="17440" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2920" yWindow="1860" windowWidth="25600" windowHeight="17440" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="user_input_details" sheetId="6" r:id="rId1"/>
@@ -18,8 +18,7 @@
     <sheet name="time_periods" sheetId="4" r:id="rId3"/>
     <sheet name="AD_lu_transitions" sheetId="1" r:id="rId4"/>
     <sheet name="c_stock" sheetId="2" r:id="rId5"/>
-    <sheet name="C_factors" sheetId="7" r:id="rId6"/>
-    <sheet name="c_stock_old" sheetId="8" r:id="rId7"/>
+    <sheet name="c_stock_old" sheetId="8" r:id="rId6"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -780,7 +779,7 @@
   <dimension ref="A1:B9"/>
   <sheetViews>
     <sheetView zoomScale="190" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -870,7 +869,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F8C6B7CA-5E2C-284E-A17C-8E0897ACEFB0}">
   <dimension ref="A1:I2"/>
   <sheetViews>
-    <sheetView zoomScale="186" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="186" workbookViewId="0">
       <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
@@ -950,8 +949,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A7F899DA-46D5-A143-AFBA-1E1D48143306}">
   <dimension ref="A1:D5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B7" sqref="A1:XFD1048576"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -4347,28 +4346,6 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{310680FF-863C-E441-9495-70029B1244B3}">
-  <dimension ref="A1:B2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I36" sqref="I36"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
-  <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A1" s="7"/>
-      <c r="B1" s="7"/>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A2" s="7"/>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{07289E27-3AAB-8442-B8AB-764F61441691}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>

</xml_diff>

<commit_message>
changed template c_stock to c_stocks for consistency
</commit_message>
<xml_diff>
--- a/inst/extdata/example1.xlsx
+++ b/inst/extdata/example1.xlsx
@@ -8,17 +8,17 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/gaelsola/Github-Collabs/mocaredd/inst/extdata/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4BAEFECB-49DA-D541-9A48-799527531B36}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D5622E29-8D56-B443-9B7F-D6022BC806BA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2920" yWindow="1860" windowWidth="25600" windowHeight="17440" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="620" yWindow="760" windowWidth="29040" windowHeight="18880" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="user_input_details" sheetId="6" r:id="rId1"/>
     <sheet name="user_inputs" sheetId="5" r:id="rId2"/>
     <sheet name="time_periods" sheetId="4" r:id="rId3"/>
     <sheet name="AD_lu_transitions" sheetId="1" r:id="rId4"/>
-    <sheet name="c_stock" sheetId="2" r:id="rId5"/>
-    <sheet name="c_stock_old" sheetId="8" r:id="rId6"/>
+    <sheet name="c_stocks" sheetId="2" r:id="rId5"/>
+    <sheet name="c_stocks_old" sheetId="8" r:id="rId6"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -74,7 +74,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="846" uniqueCount="100">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="846" uniqueCount="101">
   <si>
     <t>trans_no</t>
   </si>
@@ -374,13 +374,16 @@
   </si>
   <si>
     <t>REF</t>
+  </si>
+  <si>
+    <t>s</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -422,12 +425,6 @@
       <name val="Arial"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FF000000"/>
-      <name val="Tahoma"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="12">
@@ -779,7 +776,7 @@
   <dimension ref="A1:B9"/>
   <sheetViews>
     <sheetView zoomScale="190" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -869,8 +866,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F8C6B7CA-5E2C-284E-A17C-8E0897ACEFB0}">
   <dimension ref="A1:I2"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="186" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+    <sheetView zoomScale="186" workbookViewId="0">
+      <selection activeCell="E20" sqref="E20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -950,7 +947,7 @@
   <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -1040,8 +1037,8 @@
   </sheetPr>
   <dimension ref="A1:N49"/>
   <sheetViews>
-    <sheetView topLeftCell="E15" zoomScale="127" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+    <sheetView zoomScale="127" workbookViewId="0">
+      <selection sqref="A1:N1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -2981,7 +2978,7 @@
   <dimension ref="A1:K43"/>
   <sheetViews>
     <sheetView zoomScale="109" workbookViewId="0">
-      <selection activeCell="D45" sqref="D45"/>
+      <selection activeCell="E40" sqref="E40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -3037,7 +3034,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="5" t="str">
-        <f>E2&amp;"_"&amp;C2</f>
+        <f t="shared" ref="B2:B43" si="0">E2&amp;"_"&amp;C2</f>
         <v>AGB_open</v>
       </c>
       <c r="C2" s="5" t="s">
@@ -3067,7 +3064,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="5" t="str">
-        <f>E3&amp;"_"&amp;C3</f>
+        <f t="shared" si="0"/>
         <v>AGB_ev_wet_closed</v>
       </c>
       <c r="C3" s="5" t="s">
@@ -3097,7 +3094,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="5" t="str">
-        <f>E4&amp;"_"&amp;C4</f>
+        <f t="shared" si="0"/>
         <v>AGB_ev_moist_closed</v>
       </c>
       <c r="C4" s="5" t="s">
@@ -3127,7 +3124,7 @@
         <v>4</v>
       </c>
       <c r="B5" s="5" t="str">
-        <f>E5&amp;"_"&amp;C5</f>
+        <f t="shared" si="0"/>
         <v>AGB_md_moist_closed_se</v>
       </c>
       <c r="C5" s="5" t="s">
@@ -3157,7 +3154,7 @@
         <v>5</v>
       </c>
       <c r="B6" s="5" t="str">
-        <f>E6&amp;"_"&amp;C6</f>
+        <f t="shared" si="0"/>
         <v>AGB_md_moist_closed_nw</v>
       </c>
       <c r="C6" s="5" t="s">
@@ -3187,7 +3184,7 @@
         <v>6</v>
       </c>
       <c r="B7" s="5" t="str">
-        <f>E7&amp;"_"&amp;C7</f>
+        <f t="shared" si="0"/>
         <v>AGB_ev_upland</v>
       </c>
       <c r="C7" s="5" t="s">
@@ -3217,7 +3214,7 @@
         <v>7</v>
       </c>
       <c r="B8" s="6" t="str">
-        <f>E8&amp;"_"&amp;C8</f>
+        <f t="shared" si="0"/>
         <v>BGB_open</v>
       </c>
       <c r="C8" s="6" t="s">
@@ -3247,7 +3244,7 @@
         <v>8</v>
       </c>
       <c r="B9" s="6" t="str">
-        <f>E9&amp;"_"&amp;C9</f>
+        <f t="shared" si="0"/>
         <v>BGB_ev_wet_closed</v>
       </c>
       <c r="C9" s="6" t="s">
@@ -3277,7 +3274,7 @@
         <v>9</v>
       </c>
       <c r="B10" s="6" t="str">
-        <f>E10&amp;"_"&amp;C10</f>
+        <f t="shared" si="0"/>
         <v>BGB_ev_moist_closed</v>
       </c>
       <c r="C10" s="6" t="s">
@@ -3307,7 +3304,7 @@
         <v>10</v>
       </c>
       <c r="B11" s="6" t="str">
-        <f>E11&amp;"_"&amp;C11</f>
+        <f t="shared" si="0"/>
         <v>BGB_md_moist_closed_se</v>
       </c>
       <c r="C11" s="6" t="s">
@@ -3337,7 +3334,7 @@
         <v>11</v>
       </c>
       <c r="B12" s="6" t="str">
-        <f>E12&amp;"_"&amp;C12</f>
+        <f t="shared" si="0"/>
         <v>BGB_md_moist_closed_nw</v>
       </c>
       <c r="C12" s="6" t="s">
@@ -3367,7 +3364,7 @@
         <v>12</v>
       </c>
       <c r="B13" s="6" t="str">
-        <f>E13&amp;"_"&amp;C13</f>
+        <f t="shared" si="0"/>
         <v>BGB_ev_upland</v>
       </c>
       <c r="C13" s="6" t="s">
@@ -3397,7 +3394,7 @@
         <v>13</v>
       </c>
       <c r="B14" s="5" t="str">
-        <f>E14&amp;"_"&amp;C14</f>
+        <f t="shared" si="0"/>
         <v>DW_open</v>
       </c>
       <c r="C14" s="5" t="s">
@@ -3427,7 +3424,7 @@
         <v>14</v>
       </c>
       <c r="B15" s="5" t="str">
-        <f>E15&amp;"_"&amp;C15</f>
+        <f t="shared" si="0"/>
         <v>DW_ev_wet_closed</v>
       </c>
       <c r="C15" s="5" t="s">
@@ -3457,7 +3454,7 @@
         <v>15</v>
       </c>
       <c r="B16" s="5" t="str">
-        <f>E16&amp;"_"&amp;C16</f>
+        <f t="shared" si="0"/>
         <v>DW_ev_moist_closed</v>
       </c>
       <c r="C16" s="5" t="s">
@@ -3487,7 +3484,7 @@
         <v>16</v>
       </c>
       <c r="B17" s="5" t="str">
-        <f>E17&amp;"_"&amp;C17</f>
+        <f t="shared" si="0"/>
         <v>DW_md_moist_closed_se</v>
       </c>
       <c r="C17" s="5" t="s">
@@ -3517,7 +3514,7 @@
         <v>17</v>
       </c>
       <c r="B18" s="5" t="str">
-        <f>E18&amp;"_"&amp;C18</f>
+        <f t="shared" si="0"/>
         <v>DW_md_moist_closed_nw</v>
       </c>
       <c r="C18" s="5" t="s">
@@ -3547,7 +3544,7 @@
         <v>18</v>
       </c>
       <c r="B19" s="5" t="str">
-        <f>E19&amp;"_"&amp;C19</f>
+        <f t="shared" si="0"/>
         <v>DW_ev_upland</v>
       </c>
       <c r="C19" s="5" t="s">
@@ -3577,7 +3574,7 @@
         <v>19</v>
       </c>
       <c r="B20" s="6" t="str">
-        <f>E20&amp;"_"&amp;C20</f>
+        <f t="shared" si="0"/>
         <v>LI_open</v>
       </c>
       <c r="C20" s="6" t="s">
@@ -3607,7 +3604,7 @@
         <v>20</v>
       </c>
       <c r="B21" s="6" t="str">
-        <f>E21&amp;"_"&amp;C21</f>
+        <f t="shared" si="0"/>
         <v>LI_ev_wet_closed</v>
       </c>
       <c r="C21" s="6" t="s">
@@ -3637,7 +3634,7 @@
         <v>21</v>
       </c>
       <c r="B22" s="6" t="str">
-        <f>E22&amp;"_"&amp;C22</f>
+        <f t="shared" si="0"/>
         <v>LI_ev_moist_closed</v>
       </c>
       <c r="C22" s="6" t="s">
@@ -3667,7 +3664,7 @@
         <v>22</v>
       </c>
       <c r="B23" s="6" t="str">
-        <f>E23&amp;"_"&amp;C23</f>
+        <f t="shared" si="0"/>
         <v>LI_md_moist_closed_se</v>
       </c>
       <c r="C23" s="6" t="s">
@@ -3697,7 +3694,7 @@
         <v>23</v>
       </c>
       <c r="B24" s="6" t="str">
-        <f>E24&amp;"_"&amp;C24</f>
+        <f t="shared" si="0"/>
         <v>LI_md_moist_closed_nw</v>
       </c>
       <c r="C24" s="6" t="s">
@@ -3727,7 +3724,7 @@
         <v>24</v>
       </c>
       <c r="B25" s="6" t="str">
-        <f>E25&amp;"_"&amp;C25</f>
+        <f t="shared" si="0"/>
         <v>LI_ev_upland</v>
       </c>
       <c r="C25" s="6" t="s">
@@ -3757,7 +3754,7 @@
         <v>25</v>
       </c>
       <c r="B26" s="5" t="str">
-        <f>E26&amp;"_"&amp;C26</f>
+        <f t="shared" si="0"/>
         <v>SOC_open</v>
       </c>
       <c r="C26" s="5" t="s">
@@ -3787,7 +3784,7 @@
         <v>26</v>
       </c>
       <c r="B27" s="5" t="str">
-        <f>E27&amp;"_"&amp;C27</f>
+        <f t="shared" si="0"/>
         <v>SOC_ev_wet_closed</v>
       </c>
       <c r="C27" s="5" t="s">
@@ -3817,7 +3814,7 @@
         <v>27</v>
       </c>
       <c r="B28" s="5" t="str">
-        <f>E28&amp;"_"&amp;C28</f>
+        <f t="shared" si="0"/>
         <v>SOC_ev_moist_closed</v>
       </c>
       <c r="C28" s="5" t="s">
@@ -3847,7 +3844,7 @@
         <v>28</v>
       </c>
       <c r="B29" s="5" t="str">
-        <f>E29&amp;"_"&amp;C29</f>
+        <f t="shared" si="0"/>
         <v>SOC_md_moist_closed_se</v>
       </c>
       <c r="C29" s="5" t="s">
@@ -3877,7 +3874,7 @@
         <v>29</v>
       </c>
       <c r="B30" s="5" t="str">
-        <f>E30&amp;"_"&amp;C30</f>
+        <f t="shared" si="0"/>
         <v>SOC_md_moist_closed_nw</v>
       </c>
       <c r="C30" s="5" t="s">
@@ -3907,7 +3904,7 @@
         <v>30</v>
       </c>
       <c r="B31" s="5" t="str">
-        <f>E31&amp;"_"&amp;C31</f>
+        <f t="shared" si="0"/>
         <v>SOC_ev_upland</v>
       </c>
       <c r="C31" s="5" t="s">
@@ -3937,7 +3934,7 @@
         <v>31</v>
       </c>
       <c r="B32" s="6" t="str">
-        <f>E32&amp;"_"&amp;C32</f>
+        <f t="shared" si="0"/>
         <v>ALL_postdef_open</v>
       </c>
       <c r="C32" s="6" t="s">
@@ -3967,7 +3964,7 @@
         <v>32</v>
       </c>
       <c r="B33" s="6" t="str">
-        <f>E33&amp;"_"&amp;C33</f>
+        <f t="shared" si="0"/>
         <v>ALL_postdef_ev_wet_closed</v>
       </c>
       <c r="C33" s="6" t="s">
@@ -3997,7 +3994,7 @@
         <v>33</v>
       </c>
       <c r="B34" s="6" t="str">
-        <f>E34&amp;"_"&amp;C34</f>
+        <f t="shared" si="0"/>
         <v>ALL_postdef_ev_moist_closed</v>
       </c>
       <c r="C34" s="6" t="s">
@@ -4027,7 +4024,7 @@
         <v>34</v>
       </c>
       <c r="B35" s="6" t="str">
-        <f>E35&amp;"_"&amp;C35</f>
+        <f t="shared" si="0"/>
         <v>ALL_postdef_md_moist_closed_se</v>
       </c>
       <c r="C35" s="6" t="s">
@@ -4057,7 +4054,7 @@
         <v>35</v>
       </c>
       <c r="B36" s="6" t="str">
-        <f>E36&amp;"_"&amp;C36</f>
+        <f t="shared" si="0"/>
         <v>ALL_postdef_md_moist_closed_nw</v>
       </c>
       <c r="C36" s="6" t="s">
@@ -4087,7 +4084,7 @@
         <v>36</v>
       </c>
       <c r="B37" s="6" t="str">
-        <f>E37&amp;"_"&amp;C37</f>
+        <f t="shared" si="0"/>
         <v>ALL_postdef_ev_upland</v>
       </c>
       <c r="C37" s="6" t="s">
@@ -4117,7 +4114,7 @@
         <v>37</v>
       </c>
       <c r="B38" s="18" t="str">
-        <f>E38&amp;"_"&amp;C38</f>
+        <f t="shared" si="0"/>
         <v>DG_ratio_dg_open</v>
       </c>
       <c r="C38" s="18" t="s">
@@ -4154,7 +4151,7 @@
         <v>38</v>
       </c>
       <c r="B39" s="18" t="str">
-        <f>E39&amp;"_"&amp;C39</f>
+        <f t="shared" si="0"/>
         <v>DG_ratio_dg_ev_wet_closed</v>
       </c>
       <c r="C39" s="18" t="s">
@@ -4177,11 +4174,11 @@
         <v>89</v>
       </c>
       <c r="I39" s="18">
-        <f t="shared" ref="I39:I43" si="0">(F39*(1-F39)/(G39*G39)-1)*F39</f>
+        <f t="shared" ref="I39:I43" si="1">(F39*(1-F39)/(G39*G39)-1)*F39</f>
         <v>216.75562130177516</v>
       </c>
       <c r="J39" s="18">
-        <f t="shared" ref="J39:J43" si="1">(F39*(1-F39)/(G39*G39)-1)*(1-F39)</f>
+        <f t="shared" ref="J39:J43" si="2">(F39*(1-F39)/(G39*G39)-1)*(1-F39)</f>
         <v>92.895266272189374</v>
       </c>
       <c r="K39" s="18"/>
@@ -4191,7 +4188,7 @@
         <v>39</v>
       </c>
       <c r="B40" s="18" t="str">
-        <f>E40&amp;"_"&amp;C40</f>
+        <f t="shared" si="0"/>
         <v>DG_ratio_dg_ev_moist_closed</v>
       </c>
       <c r="C40" s="18" t="s">
@@ -4204,7 +4201,7 @@
         <v>82</v>
       </c>
       <c r="F40" s="18">
-        <f t="shared" ref="F40:F43" si="2">1-0.3</f>
+        <f t="shared" ref="F40:F43" si="3">1-0.3</f>
         <v>0.7</v>
       </c>
       <c r="G40" s="18">
@@ -4214,11 +4211,11 @@
         <v>89</v>
       </c>
       <c r="I40" s="18">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>216.75562130177516</v>
       </c>
       <c r="J40" s="18">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>92.895266272189374</v>
       </c>
       <c r="K40" s="18"/>
@@ -4228,7 +4225,7 @@
         <v>40</v>
       </c>
       <c r="B41" s="18" t="str">
-        <f>E41&amp;"_"&amp;C41</f>
+        <f t="shared" si="0"/>
         <v>DG_ratio_dg_md_moist_closed_se</v>
       </c>
       <c r="C41" s="18" t="s">
@@ -4241,7 +4238,7 @@
         <v>82</v>
       </c>
       <c r="F41" s="18">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0.7</v>
       </c>
       <c r="G41" s="18">
@@ -4251,11 +4248,11 @@
         <v>89</v>
       </c>
       <c r="I41" s="18">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>216.75562130177516</v>
       </c>
       <c r="J41" s="18">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>92.895266272189374</v>
       </c>
       <c r="K41" s="18"/>
@@ -4265,7 +4262,7 @@
         <v>41</v>
       </c>
       <c r="B42" s="18" t="str">
-        <f>E42&amp;"_"&amp;C42</f>
+        <f t="shared" si="0"/>
         <v>DG_ratio_dg_md_moist_closed_nw</v>
       </c>
       <c r="C42" s="18" t="s">
@@ -4278,7 +4275,7 @@
         <v>82</v>
       </c>
       <c r="F42" s="18">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0.7</v>
       </c>
       <c r="G42" s="18">
@@ -4288,11 +4285,11 @@
         <v>89</v>
       </c>
       <c r="I42" s="18">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>216.75562130177516</v>
       </c>
       <c r="J42" s="18">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>92.895266272189374</v>
       </c>
       <c r="K42" s="18"/>
@@ -4302,7 +4299,7 @@
         <v>42</v>
       </c>
       <c r="B43" s="18" t="str">
-        <f>E43&amp;"_"&amp;C43</f>
+        <f t="shared" si="0"/>
         <v>DG_ratio_dg_ev_upland</v>
       </c>
       <c r="C43" s="18" t="s">
@@ -4315,7 +4312,7 @@
         <v>82</v>
       </c>
       <c r="F43" s="18">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0.7</v>
       </c>
       <c r="G43" s="18">
@@ -4325,11 +4322,11 @@
         <v>89</v>
       </c>
       <c r="I43" s="18">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>216.75562130177516</v>
       </c>
       <c r="J43" s="18">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>92.895266272189374</v>
       </c>
       <c r="K43" s="18"/>
@@ -4352,8 +4349,8 @@
   </sheetPr>
   <dimension ref="A1:K61"/>
   <sheetViews>
-    <sheetView topLeftCell="A19" zoomScale="109" workbookViewId="0">
-      <selection activeCell="C51" sqref="C51"/>
+    <sheetView tabSelected="1" topLeftCell="A19" zoomScale="109" workbookViewId="0">
+      <selection activeCell="F58" sqref="F58"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -4409,7 +4406,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="5" t="str">
-        <f>E2&amp;"_"&amp;C2</f>
+        <f t="shared" ref="B2:B33" si="0">E2&amp;"_"&amp;C2</f>
         <v>AGB_open</v>
       </c>
       <c r="C2" s="5" t="s">
@@ -4439,7 +4436,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="5" t="str">
-        <f>E3&amp;"_"&amp;C3</f>
+        <f t="shared" si="0"/>
         <v>AGB_ev_wet_closed</v>
       </c>
       <c r="C3" s="5" t="s">
@@ -4469,7 +4466,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="5" t="str">
-        <f>E4&amp;"_"&amp;C4</f>
+        <f t="shared" si="0"/>
         <v>AGB_ev_moist_closed</v>
       </c>
       <c r="C4" s="5" t="s">
@@ -4499,7 +4496,7 @@
         <v>4</v>
       </c>
       <c r="B5" s="5" t="str">
-        <f>E5&amp;"_"&amp;C5</f>
+        <f t="shared" si="0"/>
         <v>AGB_md_moist_closed_se</v>
       </c>
       <c r="C5" s="5" t="s">
@@ -4529,7 +4526,7 @@
         <v>5</v>
       </c>
       <c r="B6" s="5" t="str">
-        <f>E6&amp;"_"&amp;C6</f>
+        <f t="shared" si="0"/>
         <v>AGB_md_moist_closed_nw</v>
       </c>
       <c r="C6" s="5" t="s">
@@ -4559,7 +4556,7 @@
         <v>6</v>
       </c>
       <c r="B7" s="5" t="str">
-        <f>E7&amp;"_"&amp;C7</f>
+        <f t="shared" si="0"/>
         <v>AGB_ev_upland</v>
       </c>
       <c r="C7" s="5" t="s">
@@ -4589,7 +4586,7 @@
         <v>7</v>
       </c>
       <c r="B8" s="6" t="str">
-        <f>E8&amp;"_"&amp;C8</f>
+        <f t="shared" si="0"/>
         <v>BGB_open</v>
       </c>
       <c r="C8" s="6" t="s">
@@ -4619,7 +4616,7 @@
         <v>8</v>
       </c>
       <c r="B9" s="6" t="str">
-        <f>E9&amp;"_"&amp;C9</f>
+        <f t="shared" si="0"/>
         <v>BGB_ev_wet_closed</v>
       </c>
       <c r="C9" s="6" t="s">
@@ -4649,7 +4646,7 @@
         <v>9</v>
       </c>
       <c r="B10" s="6" t="str">
-        <f>E10&amp;"_"&amp;C10</f>
+        <f t="shared" si="0"/>
         <v>BGB_ev_moist_closed</v>
       </c>
       <c r="C10" s="6" t="s">
@@ -4679,7 +4676,7 @@
         <v>10</v>
       </c>
       <c r="B11" s="6" t="str">
-        <f>E11&amp;"_"&amp;C11</f>
+        <f t="shared" si="0"/>
         <v>BGB_md_moist_closed_se</v>
       </c>
       <c r="C11" s="6" t="s">
@@ -4709,7 +4706,7 @@
         <v>11</v>
       </c>
       <c r="B12" s="6" t="str">
-        <f>E12&amp;"_"&amp;C12</f>
+        <f t="shared" si="0"/>
         <v>BGB_md_moist_closed_nw</v>
       </c>
       <c r="C12" s="6" t="s">
@@ -4739,7 +4736,7 @@
         <v>12</v>
       </c>
       <c r="B13" s="6" t="str">
-        <f>E13&amp;"_"&amp;C13</f>
+        <f t="shared" si="0"/>
         <v>BGB_ev_upland</v>
       </c>
       <c r="C13" s="6" t="s">
@@ -4769,7 +4766,7 @@
         <v>13</v>
       </c>
       <c r="B14" s="5" t="str">
-        <f>E14&amp;"_"&amp;C14</f>
+        <f t="shared" si="0"/>
         <v>DW_open</v>
       </c>
       <c r="C14" s="5" t="s">
@@ -4799,7 +4796,7 @@
         <v>14</v>
       </c>
       <c r="B15" s="5" t="str">
-        <f>E15&amp;"_"&amp;C15</f>
+        <f t="shared" si="0"/>
         <v>DW_ev_wet_closed</v>
       </c>
       <c r="C15" s="5" t="s">
@@ -4829,7 +4826,7 @@
         <v>15</v>
       </c>
       <c r="B16" s="5" t="str">
-        <f>E16&amp;"_"&amp;C16</f>
+        <f t="shared" si="0"/>
         <v>DW_ev_moist_closed</v>
       </c>
       <c r="C16" s="5" t="s">
@@ -4859,7 +4856,7 @@
         <v>16</v>
       </c>
       <c r="B17" s="5" t="str">
-        <f>E17&amp;"_"&amp;C17</f>
+        <f t="shared" si="0"/>
         <v>DW_md_moist_closed_se</v>
       </c>
       <c r="C17" s="5" t="s">
@@ -4889,7 +4886,7 @@
         <v>17</v>
       </c>
       <c r="B18" s="5" t="str">
-        <f>E18&amp;"_"&amp;C18</f>
+        <f t="shared" si="0"/>
         <v>DW_md_moist_closed_nw</v>
       </c>
       <c r="C18" s="5" t="s">
@@ -4919,7 +4916,7 @@
         <v>18</v>
       </c>
       <c r="B19" s="5" t="str">
-        <f>E19&amp;"_"&amp;C19</f>
+        <f t="shared" si="0"/>
         <v>DW_ev_upland</v>
       </c>
       <c r="C19" s="5" t="s">
@@ -4949,7 +4946,7 @@
         <v>19</v>
       </c>
       <c r="B20" s="6" t="str">
-        <f>E20&amp;"_"&amp;C20</f>
+        <f t="shared" si="0"/>
         <v>LI_open</v>
       </c>
       <c r="C20" s="6" t="s">
@@ -4979,7 +4976,7 @@
         <v>20</v>
       </c>
       <c r="B21" s="6" t="str">
-        <f>E21&amp;"_"&amp;C21</f>
+        <f t="shared" si="0"/>
         <v>LI_ev_wet_closed</v>
       </c>
       <c r="C21" s="6" t="s">
@@ -5009,7 +5006,7 @@
         <v>21</v>
       </c>
       <c r="B22" s="6" t="str">
-        <f>E22&amp;"_"&amp;C22</f>
+        <f t="shared" si="0"/>
         <v>LI_ev_moist_closed</v>
       </c>
       <c r="C22" s="6" t="s">
@@ -5039,7 +5036,7 @@
         <v>22</v>
       </c>
       <c r="B23" s="6" t="str">
-        <f>E23&amp;"_"&amp;C23</f>
+        <f t="shared" si="0"/>
         <v>LI_md_moist_closed_se</v>
       </c>
       <c r="C23" s="6" t="s">
@@ -5069,7 +5066,7 @@
         <v>23</v>
       </c>
       <c r="B24" s="6" t="str">
-        <f>E24&amp;"_"&amp;C24</f>
+        <f t="shared" si="0"/>
         <v>LI_md_moist_closed_nw</v>
       </c>
       <c r="C24" s="6" t="s">
@@ -5099,7 +5096,7 @@
         <v>24</v>
       </c>
       <c r="B25" s="6" t="str">
-        <f>E25&amp;"_"&amp;C25</f>
+        <f t="shared" si="0"/>
         <v>LI_ev_upland</v>
       </c>
       <c r="C25" s="6" t="s">
@@ -5129,7 +5126,7 @@
         <v>25</v>
       </c>
       <c r="B26" s="5" t="str">
-        <f>E26&amp;"_"&amp;C26</f>
+        <f t="shared" si="0"/>
         <v>SOC_open</v>
       </c>
       <c r="C26" s="5" t="s">
@@ -5159,7 +5156,7 @@
         <v>26</v>
       </c>
       <c r="B27" s="5" t="str">
-        <f>E27&amp;"_"&amp;C27</f>
+        <f t="shared" si="0"/>
         <v>SOC_ev_wet_closed</v>
       </c>
       <c r="C27" s="5" t="s">
@@ -5189,7 +5186,7 @@
         <v>27</v>
       </c>
       <c r="B28" s="5" t="str">
-        <f>E28&amp;"_"&amp;C28</f>
+        <f t="shared" si="0"/>
         <v>SOC_ev_moist_closed</v>
       </c>
       <c r="C28" s="5" t="s">
@@ -5219,7 +5216,7 @@
         <v>28</v>
       </c>
       <c r="B29" s="5" t="str">
-        <f>E29&amp;"_"&amp;C29</f>
+        <f t="shared" si="0"/>
         <v>SOC_md_moist_closed_se</v>
       </c>
       <c r="C29" s="5" t="s">
@@ -5249,7 +5246,7 @@
         <v>29</v>
       </c>
       <c r="B30" s="5" t="str">
-        <f>E30&amp;"_"&amp;C30</f>
+        <f t="shared" si="0"/>
         <v>SOC_md_moist_closed_nw</v>
       </c>
       <c r="C30" s="5" t="s">
@@ -5279,7 +5276,7 @@
         <v>30</v>
       </c>
       <c r="B31" s="5" t="str">
-        <f>E31&amp;"_"&amp;C31</f>
+        <f t="shared" si="0"/>
         <v>SOC_ev_upland</v>
       </c>
       <c r="C31" s="5" t="s">
@@ -5309,7 +5306,7 @@
         <v>31</v>
       </c>
       <c r="B32" s="6" t="str">
-        <f>E32&amp;"_"&amp;C32</f>
+        <f t="shared" si="0"/>
         <v>ALL_postdef_open</v>
       </c>
       <c r="C32" s="6" t="s">
@@ -5339,7 +5336,7 @@
         <v>32</v>
       </c>
       <c r="B33" s="6" t="str">
-        <f>E33&amp;"_"&amp;C33</f>
+        <f t="shared" si="0"/>
         <v>ALL_postdef_ev_wet_closed</v>
       </c>
       <c r="C33" s="6" t="s">
@@ -5369,7 +5366,7 @@
         <v>33</v>
       </c>
       <c r="B34" s="6" t="str">
-        <f>E34&amp;"_"&amp;C34</f>
+        <f t="shared" ref="B34:B65" si="1">E34&amp;"_"&amp;C34</f>
         <v>ALL_postdef_ev_moist_closed</v>
       </c>
       <c r="C34" s="6" t="s">
@@ -5399,7 +5396,7 @@
         <v>34</v>
       </c>
       <c r="B35" s="6" t="str">
-        <f>E35&amp;"_"&amp;C35</f>
+        <f t="shared" si="1"/>
         <v>ALL_postdef_md_moist_closed_se</v>
       </c>
       <c r="C35" s="6" t="s">
@@ -5429,7 +5426,7 @@
         <v>35</v>
       </c>
       <c r="B36" s="6" t="str">
-        <f>E36&amp;"_"&amp;C36</f>
+        <f t="shared" si="1"/>
         <v>ALL_postdef_md_moist_closed_nw</v>
       </c>
       <c r="C36" s="6" t="s">
@@ -5459,7 +5456,7 @@
         <v>36</v>
       </c>
       <c r="B37" s="6" t="str">
-        <f>E37&amp;"_"&amp;C37</f>
+        <f t="shared" si="1"/>
         <v>ALL_postdef_ev_upland</v>
       </c>
       <c r="C37" s="6" t="s">
@@ -5489,7 +5486,7 @@
         <v>37</v>
       </c>
       <c r="B38" s="5" t="str">
-        <f>E38&amp;"_"&amp;C38</f>
+        <f t="shared" si="1"/>
         <v>AGB_dg_open</v>
       </c>
       <c r="C38" s="5" t="s">
@@ -5519,7 +5516,7 @@
         <v>38</v>
       </c>
       <c r="B39" s="5" t="str">
-        <f>E39&amp;"_"&amp;C39</f>
+        <f t="shared" si="1"/>
         <v>AGB_dg_ev_wet_closed</v>
       </c>
       <c r="C39" s="5" t="s">
@@ -5549,7 +5546,7 @@
         <v>39</v>
       </c>
       <c r="B40" s="5" t="str">
-        <f>E40&amp;"_"&amp;C40</f>
+        <f t="shared" si="1"/>
         <v>AGB_dg_ev_moist_closed</v>
       </c>
       <c r="C40" s="5" t="s">
@@ -5579,7 +5576,7 @@
         <v>40</v>
       </c>
       <c r="B41" s="5" t="str">
-        <f>E41&amp;"_"&amp;C41</f>
+        <f t="shared" si="1"/>
         <v>AGB_dg_md_moist_closed_se</v>
       </c>
       <c r="C41" s="5" t="s">
@@ -5609,7 +5606,7 @@
         <v>41</v>
       </c>
       <c r="B42" s="5" t="str">
-        <f>E42&amp;"_"&amp;C42</f>
+        <f t="shared" si="1"/>
         <v>AGB_dg_md_moist_closed_nw</v>
       </c>
       <c r="C42" s="5" t="s">
@@ -5639,7 +5636,7 @@
         <v>42</v>
       </c>
       <c r="B43" s="5" t="str">
-        <f>E43&amp;"_"&amp;C43</f>
+        <f t="shared" si="1"/>
         <v>AGB_dg_ev_upland</v>
       </c>
       <c r="C43" s="5" t="s">
@@ -5669,7 +5666,7 @@
         <v>43</v>
       </c>
       <c r="B44" s="6" t="str">
-        <f>E44&amp;"_"&amp;C44</f>
+        <f t="shared" si="1"/>
         <v>BGB_dg_open</v>
       </c>
       <c r="C44" s="6" t="s">
@@ -5699,7 +5696,7 @@
         <v>44</v>
       </c>
       <c r="B45" s="6" t="str">
-        <f>E45&amp;"_"&amp;C45</f>
+        <f t="shared" si="1"/>
         <v>BGB_dg_ev_wet_closed</v>
       </c>
       <c r="C45" s="6" t="s">
@@ -5729,7 +5726,7 @@
         <v>45</v>
       </c>
       <c r="B46" s="6" t="str">
-        <f>E46&amp;"_"&amp;C46</f>
+        <f t="shared" si="1"/>
         <v>BGB_dg_ev_moist_closed</v>
       </c>
       <c r="C46" s="6" t="s">
@@ -5759,7 +5756,7 @@
         <v>46</v>
       </c>
       <c r="B47" s="6" t="str">
-        <f>E47&amp;"_"&amp;C47</f>
+        <f t="shared" si="1"/>
         <v>BGB_dg_md_moist_closed_se</v>
       </c>
       <c r="C47" s="6" t="s">
@@ -5789,7 +5786,7 @@
         <v>47</v>
       </c>
       <c r="B48" s="6" t="str">
-        <f>E48&amp;"_"&amp;C48</f>
+        <f t="shared" si="1"/>
         <v>BGB_dg_md_moist_closed_nw</v>
       </c>
       <c r="C48" s="6" t="s">
@@ -5819,7 +5816,7 @@
         <v>48</v>
       </c>
       <c r="B49" s="6" t="str">
-        <f>E49&amp;"_"&amp;C49</f>
+        <f t="shared" si="1"/>
         <v>BGB_dg_ev_upland</v>
       </c>
       <c r="C49" s="6" t="s">
@@ -5849,7 +5846,7 @@
         <v>49</v>
       </c>
       <c r="B50" s="5" t="str">
-        <f>E50&amp;"_"&amp;C50</f>
+        <f t="shared" si="1"/>
         <v>DW_dg_open</v>
       </c>
       <c r="C50" s="5" t="s">
@@ -5879,11 +5876,11 @@
         <v>50</v>
       </c>
       <c r="B51" s="5" t="str">
-        <f>E51&amp;"_"&amp;C51</f>
-        <v>DW_dg_ev_wet_closed</v>
+        <f t="shared" si="1"/>
+        <v>DW_s</v>
       </c>
       <c r="C51" s="5" t="s">
-        <v>83</v>
+        <v>100</v>
       </c>
       <c r="D51" s="5" t="s">
         <v>77</v>
@@ -5909,7 +5906,7 @@
         <v>51</v>
       </c>
       <c r="B52" s="5" t="str">
-        <f>E52&amp;"_"&amp;C52</f>
+        <f t="shared" si="1"/>
         <v>DW_dg_ev_moist_closed</v>
       </c>
       <c r="C52" s="5" t="s">
@@ -5939,7 +5936,7 @@
         <v>52</v>
       </c>
       <c r="B53" s="5" t="str">
-        <f>E53&amp;"_"&amp;C53</f>
+        <f t="shared" si="1"/>
         <v>DW_dg_md_moist_closed_se</v>
       </c>
       <c r="C53" s="5" t="s">
@@ -5969,7 +5966,7 @@
         <v>53</v>
       </c>
       <c r="B54" s="5" t="str">
-        <f>E54&amp;"_"&amp;C54</f>
+        <f t="shared" si="1"/>
         <v>DW_dg_md_moist_closed_nw</v>
       </c>
       <c r="C54" s="5" t="s">
@@ -5999,7 +5996,7 @@
         <v>54</v>
       </c>
       <c r="B55" s="5" t="str">
-        <f>E55&amp;"_"&amp;C55</f>
+        <f t="shared" si="1"/>
         <v>DW_dg_ev_upland</v>
       </c>
       <c r="C55" s="5" t="s">
@@ -6029,7 +6026,7 @@
         <v>55</v>
       </c>
       <c r="B56" s="6" t="str">
-        <f>E56&amp;"_"&amp;C56</f>
+        <f t="shared" si="1"/>
         <v>DG_ratio_dg_open</v>
       </c>
       <c r="C56" s="6" t="s">
@@ -6060,7 +6057,7 @@
         <v>56</v>
       </c>
       <c r="B57" s="6" t="str">
-        <f>E57&amp;"_"&amp;C57</f>
+        <f t="shared" si="1"/>
         <v>DG_ratio_dg_ev_wet_closed</v>
       </c>
       <c r="C57" s="6" t="s">
@@ -6091,7 +6088,7 @@
         <v>57</v>
       </c>
       <c r="B58" s="6" t="str">
-        <f>E58&amp;"_"&amp;C58</f>
+        <f t="shared" si="1"/>
         <v>DG_ratio_dg_ev_moist_closed</v>
       </c>
       <c r="C58" s="6" t="s">
@@ -6109,7 +6106,7 @@
         <v>89</v>
       </c>
       <c r="I58" s="6">
-        <f t="shared" ref="I58:I61" si="0">1-0.3</f>
+        <f t="shared" ref="I58:I61" si="2">1-0.3</f>
         <v>0.7</v>
       </c>
       <c r="J58" s="6">
@@ -6122,7 +6119,7 @@
         <v>58</v>
       </c>
       <c r="B59" s="6" t="str">
-        <f>E59&amp;"_"&amp;C59</f>
+        <f t="shared" si="1"/>
         <v>DG_ratio_dg_md_moist_closed_se</v>
       </c>
       <c r="C59" s="6" t="s">
@@ -6140,7 +6137,7 @@
         <v>89</v>
       </c>
       <c r="I59" s="6">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>0.7</v>
       </c>
       <c r="J59" s="6">
@@ -6153,7 +6150,7 @@
         <v>59</v>
       </c>
       <c r="B60" s="6" t="str">
-        <f>E60&amp;"_"&amp;C60</f>
+        <f t="shared" si="1"/>
         <v>DG_ratio_dg_md_moist_closed_nw</v>
       </c>
       <c r="C60" s="6" t="s">
@@ -6171,7 +6168,7 @@
         <v>89</v>
       </c>
       <c r="I60" s="6">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>0.7</v>
       </c>
       <c r="J60" s="6">
@@ -6184,7 +6181,7 @@
         <v>60</v>
       </c>
       <c r="B61" s="6" t="str">
-        <f>E61&amp;"_"&amp;C61</f>
+        <f t="shared" si="1"/>
         <v>DG_ratio_dg_ev_upland</v>
       </c>
       <c r="C61" s="6" t="s">
@@ -6202,7 +6199,7 @@
         <v>89</v>
       </c>
       <c r="I61" s="6">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>0.7</v>
       </c>
       <c r="J61" s="6">

</xml_diff>

<commit_message>
done 4 / 6 checks in function anmd adapted template
</commit_message>
<xml_diff>
--- a/inst/extdata/example1.xlsx
+++ b/inst/extdata/example1.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10811"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11027"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/gaelsola/Github-Collabs/mocaredd/inst/extdata/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D5622E29-8D56-B443-9B7F-D6022BC806BA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0FB44CF1-9D94-5544-A0E5-1C5E9CA5F7BB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="620" yWindow="760" windowWidth="29040" windowHeight="18880" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28860" yWindow="10520" windowWidth="28660" windowHeight="18880" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="user_input_details" sheetId="6" r:id="rId1"/>
@@ -268,12 +268,6 @@
     <t>trans_period</t>
   </si>
   <si>
-    <t>M1</t>
-  </si>
-  <si>
-    <t>M2</t>
-  </si>
-  <si>
     <t>Input_name</t>
   </si>
   <si>
@@ -377,6 +371,12 @@
   </si>
   <si>
     <t>s</t>
+  </si>
+  <si>
+    <t>MON1</t>
+  </si>
+  <si>
+    <t>MON2</t>
   </si>
 </sst>
 </file>
@@ -787,34 +787,34 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A1" s="7" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="B1" s="7" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A2" s="7" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="B2" s="7" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A3" s="7" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A4" s="7" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="B4" s="7" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.15">
@@ -822,39 +822,39 @@
         <v>39</v>
       </c>
       <c r="B5" s="7" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
     </row>
     <row r="6" spans="1:2" ht="28" x14ac:dyDescent="0.15">
       <c r="A6" s="7" t="s">
+        <v>93</v>
+      </c>
+      <c r="B6" s="19" t="s">
         <v>95</v>
-      </c>
-      <c r="B6" s="19" t="s">
-        <v>97</v>
       </c>
     </row>
     <row r="7" spans="1:2" ht="28" x14ac:dyDescent="0.15">
       <c r="A7" s="7" t="s">
+        <v>92</v>
+      </c>
+      <c r="B7" s="19" t="s">
         <v>94</v>
-      </c>
-      <c r="B7" s="19" t="s">
-        <v>96</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A8" s="7" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="B8" s="7" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A9" s="7" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="B9" s="7" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
     </row>
   </sheetData>
@@ -881,31 +881,31 @@
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A1" s="7" t="s">
+        <v>70</v>
+      </c>
+      <c r="B1" s="7" t="s">
+        <v>71</v>
+      </c>
+      <c r="C1" s="7" t="s">
         <v>72</v>
-      </c>
-      <c r="B1" s="7" t="s">
-        <v>73</v>
-      </c>
-      <c r="C1" s="7" t="s">
-        <v>74</v>
       </c>
       <c r="D1" s="7" t="s">
         <v>39</v>
       </c>
       <c r="E1" s="7" t="s">
+        <v>86</v>
+      </c>
+      <c r="F1" s="7" t="s">
+        <v>93</v>
+      </c>
+      <c r="G1" s="7" t="s">
+        <v>92</v>
+      </c>
+      <c r="H1" s="7" t="s">
         <v>88</v>
       </c>
-      <c r="F1" s="7" t="s">
-        <v>95</v>
-      </c>
-      <c r="G1" s="7" t="s">
-        <v>94</v>
-      </c>
-      <c r="H1" s="7" t="s">
+      <c r="I1" s="7" t="s">
         <v>90</v>
-      </c>
-      <c r="I1" s="7" t="s">
-        <v>92</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.15">
@@ -925,7 +925,7 @@
         <v>52</v>
       </c>
       <c r="F2" s="7" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="G2" t="b">
         <v>1</v>
@@ -947,7 +947,7 @@
   <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -980,7 +980,7 @@
         <v>2014</v>
       </c>
       <c r="D2" s="7" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.15">
@@ -994,7 +994,7 @@
         <v>2019</v>
       </c>
       <c r="D3" s="7" t="s">
-        <v>64</v>
+        <v>99</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.15">
@@ -1008,7 +1008,7 @@
         <v>2020</v>
       </c>
       <c r="D4" s="7" t="s">
-        <v>65</v>
+        <v>100</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.15">
@@ -1022,7 +1022,7 @@
         <v>2021</v>
       </c>
       <c r="D5" s="7" t="s">
-        <v>65</v>
+        <v>100</v>
       </c>
     </row>
   </sheetData>
@@ -1037,7 +1037,7 @@
   </sheetPr>
   <dimension ref="A1:N49"/>
   <sheetViews>
-    <sheetView zoomScale="127" workbookViewId="0">
+    <sheetView topLeftCell="D1" zoomScale="127" workbookViewId="0">
       <selection sqref="A1:N1"/>
     </sheetView>
   </sheetViews>
@@ -2050,10 +2050,10 @@
         <v>15</v>
       </c>
       <c r="G26" s="15" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="H26" s="15" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="I26" s="15">
         <v>437</v>
@@ -2089,10 +2089,10 @@
         <v>20</v>
       </c>
       <c r="G27" s="15" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="H27" s="15" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="I27" s="15">
         <v>303.89</v>
@@ -2128,10 +2128,10 @@
         <v>23</v>
       </c>
       <c r="G28" s="15" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="H28" s="15" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="I28" s="16">
         <v>1152.8499999999999</v>
@@ -2167,10 +2167,10 @@
         <v>26</v>
       </c>
       <c r="G29" s="15" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="H29" s="15" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="I29" s="16">
         <v>1269.99</v>
@@ -2206,10 +2206,10 @@
         <v>29</v>
       </c>
       <c r="G30" s="15" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="H30" s="15" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="I30" s="16">
         <v>1293</v>
@@ -2245,10 +2245,10 @@
         <v>32</v>
       </c>
       <c r="G31" s="15" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="H31" s="15" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="I31" s="15">
         <v>79.849999999999994</v>
@@ -2284,10 +2284,10 @@
         <v>15</v>
       </c>
       <c r="G32" s="17" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="H32" s="17" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="I32" s="10">
         <v>0</v>
@@ -2323,10 +2323,10 @@
         <v>20</v>
       </c>
       <c r="G33" s="17" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="H33" s="17" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="I33" s="10">
         <v>607.16865869853905</v>
@@ -2362,10 +2362,10 @@
         <v>23</v>
       </c>
       <c r="G34" s="17" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="H34" s="17" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="I34" s="10">
         <v>1281.76734104046</v>
@@ -2401,10 +2401,10 @@
         <v>26</v>
       </c>
       <c r="G35" s="17" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="H35" s="17" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="I35" s="10">
         <v>4425.8122943927001</v>
@@ -2440,10 +2440,10 @@
         <v>29</v>
       </c>
       <c r="G36" s="17" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="H36" s="17" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="I36" s="10">
         <v>3095.4922779922799</v>
@@ -2479,10 +2479,10 @@
         <v>32</v>
       </c>
       <c r="G37" s="17" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="H37" s="17" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="I37" s="10">
         <v>0</v>
@@ -2518,10 +2518,10 @@
         <v>15</v>
       </c>
       <c r="G38" s="15" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="H38" s="15" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="I38" s="13">
         <v>0</v>
@@ -2557,10 +2557,10 @@
         <v>20</v>
       </c>
       <c r="G39" s="15" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="H39" s="15" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="I39" s="13">
         <v>0</v>
@@ -2596,10 +2596,10 @@
         <v>23</v>
       </c>
       <c r="G40" s="15" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="H40" s="15" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="I40" s="13">
         <v>637.65851905104239</v>
@@ -2635,10 +2635,10 @@
         <v>26</v>
       </c>
       <c r="G41" s="15" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="H41" s="15" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="I41" s="13">
         <v>1280.2833117723158</v>
@@ -2674,10 +2674,10 @@
         <v>29</v>
       </c>
       <c r="G42" s="15" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="H42" s="15" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="I42" s="13">
         <v>618.70032154340834</v>
@@ -2713,10 +2713,10 @@
         <v>32</v>
       </c>
       <c r="G43" s="15" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="H43" s="15" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="I43" s="13">
         <v>0</v>
@@ -2752,10 +2752,10 @@
         <v>15</v>
       </c>
       <c r="G44" s="17" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="H44" s="17" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="I44" s="10">
         <v>1280.2833117723158</v>
@@ -2791,10 +2791,10 @@
         <v>20</v>
       </c>
       <c r="G45" s="17" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="H45" s="17" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="I45" s="10">
         <v>606.36339522546416</v>
@@ -2830,10 +2830,10 @@
         <v>23</v>
       </c>
       <c r="G46" s="17" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="H46" s="17" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="I46" s="10">
         <v>637.65851905104239</v>
@@ -2869,10 +2869,10 @@
         <v>26</v>
       </c>
       <c r="G47" s="17" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="H47" s="17" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="I47" s="10">
         <v>2491.1585170268313</v>
@@ -2908,10 +2908,10 @@
         <v>29</v>
       </c>
       <c r="G48" s="17" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="H48" s="17" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="I48" s="10">
         <v>3687.6546466624318</v>
@@ -2947,10 +2947,10 @@
         <v>32</v>
       </c>
       <c r="G49" s="17" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="H49" s="17" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="I49" s="10">
         <v>318.58015267175574</v>
@@ -2977,8 +2977,8 @@
   </sheetPr>
   <dimension ref="A1:K43"/>
   <sheetViews>
-    <sheetView zoomScale="109" workbookViewId="0">
-      <selection activeCell="E40" sqref="E40"/>
+    <sheetView tabSelected="1" zoomScale="109" workbookViewId="0">
+      <selection activeCell="D36" sqref="D36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -4118,13 +4118,13 @@
         <v>DG_ratio_dg_open</v>
       </c>
       <c r="C38" s="18" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="D38" s="18" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="E38" s="18" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="F38" s="18">
         <f>1-0.48</f>
@@ -4134,7 +4134,7 @@
         <v>7.2999999999999995E-2</v>
       </c>
       <c r="H38" s="18" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="I38" s="18">
         <f>(F38*(1-F38)/(G38*G38)-1)*F38</f>
@@ -4155,13 +4155,13 @@
         <v>DG_ratio_dg_ev_wet_closed</v>
       </c>
       <c r="C39" s="18" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="D39" s="18" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="E39" s="18" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="F39" s="18">
         <f>1-0.3</f>
@@ -4171,7 +4171,7 @@
         <v>2.5999999999999999E-2</v>
       </c>
       <c r="H39" s="18" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="I39" s="18">
         <f t="shared" ref="I39:I43" si="1">(F39*(1-F39)/(G39*G39)-1)*F39</f>
@@ -4192,13 +4192,13 @@
         <v>DG_ratio_dg_ev_moist_closed</v>
       </c>
       <c r="C40" s="18" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="D40" s="18" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="E40" s="18" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="F40" s="18">
         <f t="shared" ref="F40:F43" si="3">1-0.3</f>
@@ -4208,7 +4208,7 @@
         <v>2.5999999999999999E-2</v>
       </c>
       <c r="H40" s="18" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="I40" s="18">
         <f t="shared" si="1"/>
@@ -4229,13 +4229,13 @@
         <v>DG_ratio_dg_md_moist_closed_se</v>
       </c>
       <c r="C41" s="18" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="D41" s="18" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="E41" s="18" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="F41" s="18">
         <f t="shared" si="3"/>
@@ -4245,7 +4245,7 @@
         <v>2.5999999999999999E-2</v>
       </c>
       <c r="H41" s="18" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="I41" s="18">
         <f t="shared" si="1"/>
@@ -4266,13 +4266,13 @@
         <v>DG_ratio_dg_md_moist_closed_nw</v>
       </c>
       <c r="C42" s="18" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="D42" s="18" t="s">
+        <v>78</v>
+      </c>
+      <c r="E42" s="18" t="s">
         <v>80</v>
-      </c>
-      <c r="E42" s="18" t="s">
-        <v>82</v>
       </c>
       <c r="F42" s="18">
         <f t="shared" si="3"/>
@@ -4282,7 +4282,7 @@
         <v>2.5999999999999999E-2</v>
       </c>
       <c r="H42" s="18" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="I42" s="18">
         <f t="shared" si="1"/>
@@ -4303,13 +4303,13 @@
         <v>DG_ratio_dg_ev_upland</v>
       </c>
       <c r="C43" s="18" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="D43" s="18" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="E43" s="18" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="F43" s="18">
         <f t="shared" si="3"/>
@@ -4319,7 +4319,7 @@
         <v>2.5999999999999999E-2</v>
       </c>
       <c r="H43" s="18" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="I43" s="18">
         <f t="shared" si="1"/>
@@ -4349,7 +4349,7 @@
   </sheetPr>
   <dimension ref="A1:K61"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" zoomScale="109" workbookViewId="0">
+    <sheetView topLeftCell="A19" zoomScale="109" workbookViewId="0">
       <selection activeCell="F58" sqref="F58"/>
     </sheetView>
   </sheetViews>
@@ -5366,7 +5366,7 @@
         <v>33</v>
       </c>
       <c r="B34" s="6" t="str">
-        <f t="shared" ref="B34:B65" si="1">E34&amp;"_"&amp;C34</f>
+        <f t="shared" ref="B34:B61" si="1">E34&amp;"_"&amp;C34</f>
         <v>ALL_postdef_ev_moist_closed</v>
       </c>
       <c r="C34" s="6" t="s">
@@ -5490,10 +5490,10 @@
         <v>AGB_dg_open</v>
       </c>
       <c r="C38" s="5" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="D38" s="5" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="E38" s="5" t="s">
         <v>46</v>
@@ -5520,10 +5520,10 @@
         <v>AGB_dg_ev_wet_closed</v>
       </c>
       <c r="C39" s="5" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="D39" s="5" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="E39" s="5" t="s">
         <v>46</v>
@@ -5550,10 +5550,10 @@
         <v>AGB_dg_ev_moist_closed</v>
       </c>
       <c r="C40" s="5" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="D40" s="5" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="E40" s="5" t="s">
         <v>46</v>
@@ -5580,10 +5580,10 @@
         <v>AGB_dg_md_moist_closed_se</v>
       </c>
       <c r="C41" s="5" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="D41" s="5" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="E41" s="5" t="s">
         <v>46</v>
@@ -5610,10 +5610,10 @@
         <v>AGB_dg_md_moist_closed_nw</v>
       </c>
       <c r="C42" s="5" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="D42" s="5" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="E42" s="5" t="s">
         <v>46</v>
@@ -5640,10 +5640,10 @@
         <v>AGB_dg_ev_upland</v>
       </c>
       <c r="C43" s="5" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="D43" s="5" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="E43" s="5" t="s">
         <v>46</v>
@@ -5670,10 +5670,10 @@
         <v>BGB_dg_open</v>
       </c>
       <c r="C44" s="6" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="D44" s="6" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="E44" s="6" t="s">
         <v>48</v>
@@ -5700,10 +5700,10 @@
         <v>BGB_dg_ev_wet_closed</v>
       </c>
       <c r="C45" s="6" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="D45" s="6" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="E45" s="6" t="s">
         <v>48</v>
@@ -5730,10 +5730,10 @@
         <v>BGB_dg_ev_moist_closed</v>
       </c>
       <c r="C46" s="6" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="D46" s="6" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="E46" s="6" t="s">
         <v>48</v>
@@ -5760,10 +5760,10 @@
         <v>BGB_dg_md_moist_closed_se</v>
       </c>
       <c r="C47" s="6" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="D47" s="6" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="E47" s="6" t="s">
         <v>48</v>
@@ -5790,10 +5790,10 @@
         <v>BGB_dg_md_moist_closed_nw</v>
       </c>
       <c r="C48" s="6" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="D48" s="6" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="E48" s="6" t="s">
         <v>48</v>
@@ -5820,10 +5820,10 @@
         <v>BGB_dg_ev_upland</v>
       </c>
       <c r="C49" s="6" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="D49" s="6" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="E49" s="6" t="s">
         <v>48</v>
@@ -5850,10 +5850,10 @@
         <v>DW_dg_open</v>
       </c>
       <c r="C50" s="5" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="D50" s="5" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="E50" s="5" t="s">
         <v>49</v>
@@ -5880,10 +5880,10 @@
         <v>DW_s</v>
       </c>
       <c r="C51" s="5" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="D51" s="5" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="E51" s="5" t="s">
         <v>49</v>
@@ -5910,10 +5910,10 @@
         <v>DW_dg_ev_moist_closed</v>
       </c>
       <c r="C52" s="5" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="D52" s="5" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="E52" s="5" t="s">
         <v>49</v>
@@ -5940,10 +5940,10 @@
         <v>DW_dg_md_moist_closed_se</v>
       </c>
       <c r="C53" s="5" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="D53" s="5" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="E53" s="5" t="s">
         <v>49</v>
@@ -5970,10 +5970,10 @@
         <v>DW_dg_md_moist_closed_nw</v>
       </c>
       <c r="C54" s="5" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="D54" s="5" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="E54" s="5" t="s">
         <v>49</v>
@@ -6000,10 +6000,10 @@
         <v>DW_dg_ev_upland</v>
       </c>
       <c r="C55" s="5" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="D55" s="5" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="E55" s="5" t="s">
         <v>49</v>
@@ -6030,18 +6030,18 @@
         <v>DG_ratio_dg_open</v>
       </c>
       <c r="C56" s="6" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="D56" s="6" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="E56" s="6" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="F56" s="6"/>
       <c r="G56" s="6"/>
       <c r="H56" s="6" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="I56" s="6">
         <f>1-0.48</f>
@@ -6061,18 +6061,18 @@
         <v>DG_ratio_dg_ev_wet_closed</v>
       </c>
       <c r="C57" s="6" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="D57" s="6" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="E57" s="6" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="F57" s="6"/>
       <c r="G57" s="6"/>
       <c r="H57" s="6" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="I57" s="6">
         <f>1-0.3</f>
@@ -6092,18 +6092,18 @@
         <v>DG_ratio_dg_ev_moist_closed</v>
       </c>
       <c r="C58" s="6" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="D58" s="6" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="E58" s="6" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="F58" s="6"/>
       <c r="G58" s="6"/>
       <c r="H58" s="6" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="I58" s="6">
         <f t="shared" ref="I58:I61" si="2">1-0.3</f>
@@ -6123,18 +6123,18 @@
         <v>DG_ratio_dg_md_moist_closed_se</v>
       </c>
       <c r="C59" s="6" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="D59" s="6" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="E59" s="6" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="F59" s="6"/>
       <c r="G59" s="6"/>
       <c r="H59" s="6" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="I59" s="6">
         <f t="shared" si="2"/>
@@ -6154,18 +6154,18 @@
         <v>DG_ratio_dg_md_moist_closed_nw</v>
       </c>
       <c r="C60" s="6" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="D60" s="6" t="s">
+        <v>78</v>
+      </c>
+      <c r="E60" s="6" t="s">
         <v>80</v>
-      </c>
-      <c r="E60" s="6" t="s">
-        <v>82</v>
       </c>
       <c r="F60" s="6"/>
       <c r="G60" s="6"/>
       <c r="H60" s="6" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="I60" s="6">
         <f t="shared" si="2"/>
@@ -6185,18 +6185,18 @@
         <v>DG_ratio_dg_ev_upland</v>
       </c>
       <c r="C61" s="6" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="D61" s="6" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="E61" s="6" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="F61" s="6"/>
       <c r="G61" s="6"/>
       <c r="H61" s="6" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="I61" s="6">
         <f t="shared" si="2"/>

</xml_diff>

<commit_message>
updated checks, only n.6 tbd
</commit_message>
<xml_diff>
--- a/inst/extdata/example1.xlsx
+++ b/inst/extdata/example1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/gaelsola/Github-Collabs/mocaredd/inst/extdata/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0FB44CF1-9D94-5544-A0E5-1C5E9CA5F7BB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{23CADB2F-88A2-AB43-8ED9-2466C694D2C1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28860" yWindow="10520" windowWidth="28660" windowHeight="18880" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-24640" yWindow="4780" windowWidth="22160" windowHeight="16860" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="user_input_details" sheetId="6" r:id="rId1"/>
@@ -43,7 +43,7 @@
     <author>tc={35B02895-20C4-2C4E-BAE2-5B882E755564}</author>
   </authors>
   <commentList>
-    <comment ref="G26" authorId="0" shapeId="0" xr:uid="{35B02895-20C4-2C4E-BAE2-5B882E755564}">
+    <comment ref="H26" authorId="0" shapeId="0" xr:uid="{35B02895-20C4-2C4E-BAE2-5B882E755564}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -74,7 +74,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="846" uniqueCount="101">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="889" uniqueCount="102">
   <si>
     <t>trans_no</t>
   </si>
@@ -377,6 +377,9 @@
   </si>
   <si>
     <t>MON2</t>
+  </si>
+  <si>
+    <t>c_period</t>
   </si>
 </sst>
 </file>
@@ -757,7 +760,7 @@
 
 <file path=xl/threadedComments/threadedComment1.xml><?xml version="1.0" encoding="utf-8"?>
 <ThreadedComments xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <threadedComment ref="G26" dT="2024-10-18T07:06:16.55" personId="{346CA1BB-775C-874F-8397-56904622A61E}" id="{35B02895-20C4-2C4E-BAE2-5B882E755564}">
+  <threadedComment ref="H26" dT="2024-10-18T07:06:16.55" personId="{346CA1BB-775C-874F-8397-56904622A61E}" id="{35B02895-20C4-2C4E-BAE2-5B882E755564}">
     <text>Ghana: placeholder for SOC support in future versions</text>
   </threadedComment>
 </ThreadedComments>
@@ -1037,14 +1040,14 @@
   </sheetPr>
   <dimension ref="A1:N49"/>
   <sheetViews>
-    <sheetView topLeftCell="D1" zoomScale="127" workbookViewId="0">
-      <selection sqref="A1:N1"/>
+    <sheetView tabSelected="1" zoomScale="127" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="2" max="2" width="21.5" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="20.1640625" customWidth="1"/>
+    <col min="3" max="3" width="11.5" bestFit="1" customWidth="1"/>
     <col min="5" max="7" width="25.6640625" customWidth="1"/>
     <col min="8" max="8" width="35.33203125" bestFit="1" customWidth="1"/>
   </cols>
@@ -1098,8 +1101,8 @@
         <v>1</v>
       </c>
       <c r="B2" s="2" t="str">
-        <f>C2&amp;"_"&amp;D2&amp;"_"&amp;E2</f>
-        <v>T1_DF_open</v>
+        <f>C2&amp;"_"&amp;E2&amp;"_"&amp;G2</f>
+        <v>T1_open_postdef_open</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>59</v>
@@ -1137,8 +1140,8 @@
         <v>2</v>
       </c>
       <c r="B3" s="2" t="str">
-        <f t="shared" ref="B3:B49" si="0">C3&amp;"_"&amp;D3&amp;"_"&amp;E3</f>
-        <v>T1_DF_ev_wet_closed</v>
+        <f t="shared" ref="B3:B49" si="0">C3&amp;"_"&amp;E3&amp;"_"&amp;G3</f>
+        <v>T1_ev_wet_closed_postdef_ev_wet_closed</v>
       </c>
       <c r="C3" s="2" t="s">
         <v>59</v>
@@ -1177,7 +1180,7 @@
       </c>
       <c r="B4" s="2" t="str">
         <f t="shared" si="0"/>
-        <v>T1_DF_ev_moist_closed</v>
+        <v>T1_ev_moist_closed_postdef_ev_moist_closed</v>
       </c>
       <c r="C4" s="2" t="s">
         <v>59</v>
@@ -1216,7 +1219,7 @@
       </c>
       <c r="B5" s="2" t="str">
         <f t="shared" si="0"/>
-        <v>T1_DF_md_moist_closed_se</v>
+        <v>T1_md_moist_closed_se_postdef_md_moist_closed_se</v>
       </c>
       <c r="C5" s="2" t="s">
         <v>59</v>
@@ -1255,7 +1258,7 @@
       </c>
       <c r="B6" s="2" t="str">
         <f t="shared" si="0"/>
-        <v>T1_DF_md_moist_closed_nw</v>
+        <v>T1_md_moist_closed_nw_postdef_md_moist_closed_nw</v>
       </c>
       <c r="C6" s="2" t="s">
         <v>59</v>
@@ -1294,7 +1297,7 @@
       </c>
       <c r="B7" s="2" t="str">
         <f t="shared" si="0"/>
-        <v>T1_DF_ev_upland</v>
+        <v>T1_ev_upland_postdef_ev_upland</v>
       </c>
       <c r="C7" s="2" t="s">
         <v>59</v>
@@ -1333,7 +1336,7 @@
       </c>
       <c r="B8" s="9" t="str">
         <f t="shared" si="0"/>
-        <v>T2_DF_open</v>
+        <v>T2_open_postdef_open</v>
       </c>
       <c r="C8" s="9" t="s">
         <v>60</v>
@@ -1372,7 +1375,7 @@
       </c>
       <c r="B9" s="9" t="str">
         <f t="shared" si="0"/>
-        <v>T2_DF_ev_wet_closed</v>
+        <v>T2_ev_wet_closed_postdef_ev_wet_closed</v>
       </c>
       <c r="C9" s="9" t="s">
         <v>60</v>
@@ -1411,7 +1414,7 @@
       </c>
       <c r="B10" s="9" t="str">
         <f t="shared" si="0"/>
-        <v>T2_DF_ev_moist_closed</v>
+        <v>T2_ev_moist_closed_postdef_ev_moist_closed</v>
       </c>
       <c r="C10" s="9" t="s">
         <v>60</v>
@@ -1450,7 +1453,7 @@
       </c>
       <c r="B11" s="9" t="str">
         <f t="shared" si="0"/>
-        <v>T2_DF_md_moist_closed_se</v>
+        <v>T2_md_moist_closed_se_postdef_md_moist_closed_se</v>
       </c>
       <c r="C11" s="9" t="s">
         <v>60</v>
@@ -1489,7 +1492,7 @@
       </c>
       <c r="B12" s="9" t="str">
         <f t="shared" si="0"/>
-        <v>T2_DF_md_moist_closed_nw</v>
+        <v>T2_md_moist_closed_nw_postdef_md_moist_closed_nw</v>
       </c>
       <c r="C12" s="9" t="s">
         <v>60</v>
@@ -1528,7 +1531,7 @@
       </c>
       <c r="B13" s="9" t="str">
         <f t="shared" si="0"/>
-        <v>T2_DF_ev_upland</v>
+        <v>T2_ev_upland_postdef_ev_upland</v>
       </c>
       <c r="C13" s="9" t="s">
         <v>60</v>
@@ -1567,7 +1570,7 @@
       </c>
       <c r="B14" s="12" t="str">
         <f t="shared" si="0"/>
-        <v>T3_DF_open</v>
+        <v>T3_open_postdef_open</v>
       </c>
       <c r="C14" s="12" t="s">
         <v>61</v>
@@ -1606,7 +1609,7 @@
       </c>
       <c r="B15" s="12" t="str">
         <f t="shared" si="0"/>
-        <v>T3_DF_ev_wet_closed</v>
+        <v>T3_ev_wet_closed_postdef_ev_wet_closed</v>
       </c>
       <c r="C15" s="12" t="s">
         <v>61</v>
@@ -1645,7 +1648,7 @@
       </c>
       <c r="B16" s="12" t="str">
         <f t="shared" si="0"/>
-        <v>T3_DF_ev_moist_closed</v>
+        <v>T3_ev_moist_closed_postdef_ev_moist_closed</v>
       </c>
       <c r="C16" s="12" t="s">
         <v>61</v>
@@ -1684,7 +1687,7 @@
       </c>
       <c r="B17" s="12" t="str">
         <f t="shared" si="0"/>
-        <v>T3_DF_md_moist_closed_se</v>
+        <v>T3_md_moist_closed_se_postdef_md_moist_closed_se</v>
       </c>
       <c r="C17" s="12" t="s">
         <v>61</v>
@@ -1723,7 +1726,7 @@
       </c>
       <c r="B18" s="12" t="str">
         <f t="shared" si="0"/>
-        <v>T3_DF_md_moist_closed_nw</v>
+        <v>T3_md_moist_closed_nw_postdef_md_moist_closed_nw</v>
       </c>
       <c r="C18" s="12" t="s">
         <v>61</v>
@@ -1762,7 +1765,7 @@
       </c>
       <c r="B19" s="12" t="str">
         <f t="shared" si="0"/>
-        <v>T3_DF_ev_upland</v>
+        <v>T3_ev_upland_postdef_ev_upland</v>
       </c>
       <c r="C19" s="12" t="s">
         <v>61</v>
@@ -1801,7 +1804,7 @@
       </c>
       <c r="B20" s="9" t="str">
         <f t="shared" si="0"/>
-        <v>T4_DF_open</v>
+        <v>T4_open_postdef_open</v>
       </c>
       <c r="C20" s="9" t="s">
         <v>62</v>
@@ -1840,7 +1843,7 @@
       </c>
       <c r="B21" s="9" t="str">
         <f t="shared" si="0"/>
-        <v>T4_DF_ev_wet_closed</v>
+        <v>T4_ev_wet_closed_postdef_ev_wet_closed</v>
       </c>
       <c r="C21" s="9" t="s">
         <v>62</v>
@@ -1879,7 +1882,7 @@
       </c>
       <c r="B22" s="9" t="str">
         <f t="shared" si="0"/>
-        <v>T4_DF_ev_moist_closed</v>
+        <v>T4_ev_moist_closed_postdef_ev_moist_closed</v>
       </c>
       <c r="C22" s="9" t="s">
         <v>62</v>
@@ -1918,7 +1921,7 @@
       </c>
       <c r="B23" s="9" t="str">
         <f t="shared" si="0"/>
-        <v>T4_DF_md_moist_closed_se</v>
+        <v>T4_md_moist_closed_se_postdef_md_moist_closed_se</v>
       </c>
       <c r="C23" s="9" t="s">
         <v>62</v>
@@ -1957,7 +1960,7 @@
       </c>
       <c r="B24" s="9" t="str">
         <f t="shared" si="0"/>
-        <v>T4_DF_md_moist_closed_nw</v>
+        <v>T4_md_moist_closed_nw_postdef_md_moist_closed_nw</v>
       </c>
       <c r="C24" s="9" t="s">
         <v>62</v>
@@ -1996,7 +1999,7 @@
       </c>
       <c r="B25" s="9" t="str">
         <f t="shared" si="0"/>
-        <v>T4_DF_ev_upland</v>
+        <v>T4_ev_upland_postdef_ev_upland</v>
       </c>
       <c r="C25" s="9" t="s">
         <v>62</v>
@@ -2035,7 +2038,7 @@
       </c>
       <c r="B26" s="15" t="str">
         <f t="shared" si="0"/>
-        <v>T1_DG_open</v>
+        <v>T1_open_dg_open</v>
       </c>
       <c r="C26" s="15" t="s">
         <v>59</v>
@@ -2074,7 +2077,7 @@
       </c>
       <c r="B27" s="15" t="str">
         <f t="shared" si="0"/>
-        <v>T1_DG_ev_wet_closed</v>
+        <v>T1_ev_wet_closed_dg_ev_wet_closed</v>
       </c>
       <c r="C27" s="15" t="s">
         <v>59</v>
@@ -2113,7 +2116,7 @@
       </c>
       <c r="B28" s="15" t="str">
         <f t="shared" si="0"/>
-        <v>T1_DG_ev_moist_closed</v>
+        <v>T1_ev_moist_closed_dg_ev_moist_closed</v>
       </c>
       <c r="C28" s="15" t="s">
         <v>59</v>
@@ -2152,7 +2155,7 @@
       </c>
       <c r="B29" s="15" t="str">
         <f t="shared" si="0"/>
-        <v>T1_DG_md_moist_closed_se</v>
+        <v>T1_md_moist_closed_se_dg_md_moist_closed_se</v>
       </c>
       <c r="C29" s="15" t="s">
         <v>59</v>
@@ -2191,7 +2194,7 @@
       </c>
       <c r="B30" s="15" t="str">
         <f t="shared" si="0"/>
-        <v>T1_DG_md_moist_closed_nw</v>
+        <v>T1_md_moist_closed_nw_dg_md_moist_closed_nw</v>
       </c>
       <c r="C30" s="15" t="s">
         <v>59</v>
@@ -2230,7 +2233,7 @@
       </c>
       <c r="B31" s="15" t="str">
         <f t="shared" si="0"/>
-        <v>T1_DG_ev_upland</v>
+        <v>T1_ev_upland_dg_ev_upland</v>
       </c>
       <c r="C31" s="15" t="s">
         <v>59</v>
@@ -2269,7 +2272,7 @@
       </c>
       <c r="B32" s="17" t="str">
         <f t="shared" si="0"/>
-        <v>T2_DG_open</v>
+        <v>T2_open_dg_open</v>
       </c>
       <c r="C32" s="17" t="s">
         <v>60</v>
@@ -2308,7 +2311,7 @@
       </c>
       <c r="B33" s="17" t="str">
         <f t="shared" si="0"/>
-        <v>T2_DG_ev_wet_closed</v>
+        <v>T2_ev_wet_closed_dg_ev_wet_closed</v>
       </c>
       <c r="C33" s="17" t="s">
         <v>60</v>
@@ -2347,7 +2350,7 @@
       </c>
       <c r="B34" s="17" t="str">
         <f t="shared" si="0"/>
-        <v>T2_DG_ev_moist_closed</v>
+        <v>T2_ev_moist_closed_dg_ev_moist_closed</v>
       </c>
       <c r="C34" s="17" t="s">
         <v>60</v>
@@ -2386,7 +2389,7 @@
       </c>
       <c r="B35" s="17" t="str">
         <f t="shared" si="0"/>
-        <v>T2_DG_md_moist_closed_se</v>
+        <v>T2_md_moist_closed_se_dg_md_moist_closed_se</v>
       </c>
       <c r="C35" s="17" t="s">
         <v>60</v>
@@ -2425,7 +2428,7 @@
       </c>
       <c r="B36" s="17" t="str">
         <f t="shared" si="0"/>
-        <v>T2_DG_md_moist_closed_nw</v>
+        <v>T2_md_moist_closed_nw_dg_md_moist_closed_nw</v>
       </c>
       <c r="C36" s="17" t="s">
         <v>60</v>
@@ -2464,7 +2467,7 @@
       </c>
       <c r="B37" s="17" t="str">
         <f t="shared" si="0"/>
-        <v>T2_DG_ev_upland</v>
+        <v>T2_ev_upland_dg_ev_upland</v>
       </c>
       <c r="C37" s="17" t="s">
         <v>60</v>
@@ -2503,7 +2506,7 @@
       </c>
       <c r="B38" s="15" t="str">
         <f t="shared" si="0"/>
-        <v>T3_DG_open</v>
+        <v>T3_open_dg_open</v>
       </c>
       <c r="C38" s="15" t="s">
         <v>61</v>
@@ -2542,7 +2545,7 @@
       </c>
       <c r="B39" s="15" t="str">
         <f t="shared" si="0"/>
-        <v>T3_DG_ev_wet_closed</v>
+        <v>T3_ev_wet_closed_dg_ev_wet_closed</v>
       </c>
       <c r="C39" s="15" t="s">
         <v>61</v>
@@ -2581,7 +2584,7 @@
       </c>
       <c r="B40" s="15" t="str">
         <f t="shared" si="0"/>
-        <v>T3_DG_ev_moist_closed</v>
+        <v>T3_ev_moist_closed_dg_ev_moist_closed</v>
       </c>
       <c r="C40" s="15" t="s">
         <v>61</v>
@@ -2620,7 +2623,7 @@
       </c>
       <c r="B41" s="15" t="str">
         <f t="shared" si="0"/>
-        <v>T3_DG_md_moist_closed_se</v>
+        <v>T3_md_moist_closed_se_dg_md_moist_closed_se</v>
       </c>
       <c r="C41" s="15" t="s">
         <v>61</v>
@@ -2659,7 +2662,7 @@
       </c>
       <c r="B42" s="15" t="str">
         <f t="shared" si="0"/>
-        <v>T3_DG_md_moist_closed_nw</v>
+        <v>T3_md_moist_closed_nw_dg_md_moist_closed_nw</v>
       </c>
       <c r="C42" s="15" t="s">
         <v>61</v>
@@ -2698,7 +2701,7 @@
       </c>
       <c r="B43" s="15" t="str">
         <f t="shared" si="0"/>
-        <v>T3_DG_ev_upland</v>
+        <v>T3_ev_upland_dg_ev_upland</v>
       </c>
       <c r="C43" s="15" t="s">
         <v>61</v>
@@ -2737,7 +2740,7 @@
       </c>
       <c r="B44" s="17" t="str">
         <f t="shared" si="0"/>
-        <v>T4_DG_open</v>
+        <v>T4_open_dg_open</v>
       </c>
       <c r="C44" s="17" t="s">
         <v>62</v>
@@ -2776,7 +2779,7 @@
       </c>
       <c r="B45" s="17" t="str">
         <f t="shared" si="0"/>
-        <v>T4_DG_ev_wet_closed</v>
+        <v>T4_ev_wet_closed_dg_ev_wet_closed</v>
       </c>
       <c r="C45" s="17" t="s">
         <v>62</v>
@@ -2815,7 +2818,7 @@
       </c>
       <c r="B46" s="17" t="str">
         <f t="shared" si="0"/>
-        <v>T4_DG_ev_moist_closed</v>
+        <v>T4_ev_moist_closed_dg_ev_moist_closed</v>
       </c>
       <c r="C46" s="17" t="s">
         <v>62</v>
@@ -2854,7 +2857,7 @@
       </c>
       <c r="B47" s="17" t="str">
         <f t="shared" si="0"/>
-        <v>T4_DG_md_moist_closed_se</v>
+        <v>T4_md_moist_closed_se_dg_md_moist_closed_se</v>
       </c>
       <c r="C47" s="17" t="s">
         <v>62</v>
@@ -2893,7 +2896,7 @@
       </c>
       <c r="B48" s="17" t="str">
         <f t="shared" si="0"/>
-        <v>T4_DG_md_moist_closed_nw</v>
+        <v>T4_md_moist_closed_nw_dg_md_moist_closed_nw</v>
       </c>
       <c r="C48" s="17" t="s">
         <v>62</v>
@@ -2932,7 +2935,7 @@
       </c>
       <c r="B49" s="17" t="str">
         <f t="shared" si="0"/>
-        <v>T4_DG_ev_upland</v>
+        <v>T4_ev_upland_dg_ev_upland</v>
       </c>
       <c r="C49" s="17" t="s">
         <v>62</v>
@@ -2975,26 +2978,27 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:K43"/>
+  <dimension ref="A1:L43"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="109" workbookViewId="0">
-      <selection activeCell="D36" sqref="D36"/>
+    <sheetView zoomScale="109" workbookViewId="0">
+      <selection activeCell="J2" sqref="J2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="5.83203125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="29.1640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="24.83203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="35.33203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="8" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="8.6640625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="6.1640625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="6.5" bestFit="1" customWidth="1"/>
-    <col min="9" max="11" width="8.83203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.33203125" customWidth="1"/>
+    <col min="4" max="4" width="24.83203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="35.33203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="8" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="8.6640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="6.1640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="6.5" bestFit="1" customWidth="1"/>
+    <col min="10" max="12" width="8.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="8" t="s">
         <v>35</v>
       </c>
@@ -3002,1338 +3006,1467 @@
         <v>36</v>
       </c>
       <c r="C1" s="8" t="s">
+        <v>101</v>
+      </c>
+      <c r="D1" s="8" t="s">
         <v>37</v>
       </c>
-      <c r="D1" s="8" t="s">
+      <c r="E1" s="8" t="s">
         <v>38</v>
       </c>
-      <c r="E1" s="8" t="s">
+      <c r="F1" s="8" t="s">
         <v>54</v>
       </c>
-      <c r="F1" s="8" t="s">
+      <c r="G1" s="8" t="s">
         <v>40</v>
       </c>
-      <c r="G1" s="8" t="s">
+      <c r="H1" s="8" t="s">
         <v>41</v>
       </c>
-      <c r="H1" s="8" t="s">
+      <c r="I1" s="8" t="s">
         <v>42</v>
       </c>
-      <c r="I1" s="8" t="s">
+      <c r="J1" s="8" t="s">
         <v>43</v>
       </c>
-      <c r="J1" s="8" t="s">
+      <c r="K1" s="8" t="s">
         <v>44</v>
       </c>
-      <c r="K1" s="8" t="s">
+      <c r="L1" s="8" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="2" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="5">
         <v>1</v>
       </c>
       <c r="B2" s="5" t="str">
-        <f t="shared" ref="B2:B43" si="0">E2&amp;"_"&amp;C2</f>
-        <v>AGB_open</v>
+        <f>C2&amp;"_"&amp;D2&amp;"_"&amp;F2</f>
+        <v>ALL_open_AGB</v>
       </c>
       <c r="C2" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="D2" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="D2" s="5" t="s">
+      <c r="E2" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="E2" s="5" t="s">
+      <c r="F2" s="5" t="s">
         <v>46</v>
       </c>
-      <c r="F2" s="5">
+      <c r="G2" s="5">
         <v>27.35</v>
       </c>
-      <c r="G2" s="5">
+      <c r="H2" s="5">
         <v>5.35</v>
       </c>
-      <c r="H2" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="I2" s="5"/>
+      <c r="I2" s="5" t="s">
+        <v>18</v>
+      </c>
       <c r="J2" s="5"/>
       <c r="K2" s="5"/>
-    </row>
-    <row r="3" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="L2" s="5"/>
+    </row>
+    <row r="3" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3" s="5">
         <v>2</v>
       </c>
       <c r="B3" s="5" t="str">
-        <f t="shared" si="0"/>
-        <v>AGB_ev_wet_closed</v>
+        <f t="shared" ref="B3:B43" si="0">C3&amp;"_"&amp;D3&amp;"_"&amp;F3</f>
+        <v>ALL_ev_wet_closed_AGB</v>
       </c>
       <c r="C3" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="D3" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="D3" s="5" t="s">
+      <c r="E3" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="E3" s="5" t="s">
+      <c r="F3" s="5" t="s">
         <v>46</v>
       </c>
-      <c r="F3" s="5">
+      <c r="G3" s="5">
         <v>81.28</v>
       </c>
-      <c r="G3" s="5">
+      <c r="H3" s="5">
         <v>43.43</v>
       </c>
-      <c r="H3" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="I3" s="5"/>
+      <c r="I3" s="5" t="s">
+        <v>18</v>
+      </c>
       <c r="J3" s="5"/>
       <c r="K3" s="5"/>
-    </row>
-    <row r="4" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="L3" s="5"/>
+    </row>
+    <row r="4" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A4" s="5">
         <v>3</v>
       </c>
       <c r="B4" s="5" t="str">
         <f t="shared" si="0"/>
-        <v>AGB_ev_moist_closed</v>
+        <v>ALL_ev_moist_closed_AGB</v>
       </c>
       <c r="C4" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="D4" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="D4" s="5" t="s">
+      <c r="E4" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="E4" s="5" t="s">
+      <c r="F4" s="5" t="s">
         <v>46</v>
       </c>
-      <c r="F4" s="5">
+      <c r="G4" s="5">
         <v>202.85</v>
       </c>
-      <c r="G4" s="5">
+      <c r="H4" s="5">
         <v>41.5</v>
       </c>
-      <c r="H4" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="I4" s="5"/>
+      <c r="I4" s="5" t="s">
+        <v>18</v>
+      </c>
       <c r="J4" s="5"/>
       <c r="K4" s="5"/>
-    </row>
-    <row r="5" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="L4" s="5"/>
+    </row>
+    <row r="5" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A5" s="5">
         <v>4</v>
       </c>
       <c r="B5" s="5" t="str">
         <f t="shared" si="0"/>
-        <v>AGB_md_moist_closed_se</v>
+        <v>ALL_md_moist_closed_se_AGB</v>
       </c>
       <c r="C5" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="D5" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="D5" s="5" t="s">
+      <c r="E5" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="E5" s="5" t="s">
+      <c r="F5" s="5" t="s">
         <v>46</v>
       </c>
-      <c r="F5" s="5">
+      <c r="G5" s="5">
         <v>100.46</v>
       </c>
-      <c r="G5" s="5">
+      <c r="H5" s="5">
         <v>35.29</v>
       </c>
-      <c r="H5" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="I5" s="5"/>
+      <c r="I5" s="5" t="s">
+        <v>18</v>
+      </c>
       <c r="J5" s="5"/>
       <c r="K5" s="5"/>
-    </row>
-    <row r="6" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="L5" s="5"/>
+    </row>
+    <row r="6" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A6" s="5">
         <v>5</v>
       </c>
       <c r="B6" s="5" t="str">
         <f t="shared" si="0"/>
-        <v>AGB_md_moist_closed_nw</v>
+        <v>ALL_md_moist_closed_nw_AGB</v>
       </c>
       <c r="C6" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="D6" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="D6" s="5" t="s">
+      <c r="E6" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="E6" s="5" t="s">
+      <c r="F6" s="5" t="s">
         <v>46</v>
       </c>
-      <c r="F6" s="5">
+      <c r="G6" s="5">
         <v>75.91</v>
       </c>
-      <c r="G6" s="5">
+      <c r="H6" s="5">
         <v>11</v>
       </c>
-      <c r="H6" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="I6" s="5"/>
+      <c r="I6" s="5" t="s">
+        <v>18</v>
+      </c>
       <c r="J6" s="5"/>
       <c r="K6" s="5"/>
-    </row>
-    <row r="7" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="L6" s="5"/>
+    </row>
+    <row r="7" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A7" s="5">
         <v>6</v>
       </c>
       <c r="B7" s="5" t="str">
         <f t="shared" si="0"/>
-        <v>AGB_ev_upland</v>
+        <v>ALL_ev_upland_AGB</v>
       </c>
       <c r="C7" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="D7" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="D7" s="5" t="s">
+      <c r="E7" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="E7" s="5" t="s">
+      <c r="F7" s="5" t="s">
         <v>46</v>
       </c>
-      <c r="F7" s="5">
+      <c r="G7" s="5">
         <v>74.599999999999994</v>
       </c>
-      <c r="G7" s="5">
+      <c r="H7" s="5">
         <v>13.87</v>
       </c>
-      <c r="H7" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="I7" s="5"/>
+      <c r="I7" s="5" t="s">
+        <v>18</v>
+      </c>
       <c r="J7" s="5"/>
       <c r="K7" s="5"/>
-    </row>
-    <row r="8" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="L7" s="5"/>
+    </row>
+    <row r="8" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A8" s="6">
         <v>7</v>
       </c>
       <c r="B8" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>BGB_open</v>
+        <v>ALL_open_BGB</v>
       </c>
       <c r="C8" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="D8" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="D8" s="6" t="s">
+      <c r="E8" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="E8" s="6" t="s">
+      <c r="F8" s="6" t="s">
         <v>48</v>
       </c>
-      <c r="F8" s="6">
+      <c r="G8" s="6">
         <v>10.37</v>
       </c>
-      <c r="G8" s="6">
+      <c r="H8" s="6">
         <v>1.85</v>
       </c>
-      <c r="H8" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="I8" s="6"/>
+      <c r="I8" s="6" t="s">
+        <v>18</v>
+      </c>
       <c r="J8" s="6"/>
       <c r="K8" s="6"/>
-    </row>
-    <row r="9" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="L8" s="6"/>
+    </row>
+    <row r="9" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A9" s="6">
         <v>8</v>
       </c>
       <c r="B9" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>BGB_ev_wet_closed</v>
+        <v>ALL_ev_wet_closed_BGB</v>
       </c>
       <c r="C9" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="D9" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="D9" s="6" t="s">
+      <c r="E9" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="E9" s="6" t="s">
+      <c r="F9" s="6" t="s">
         <v>48</v>
       </c>
-      <c r="F9" s="6">
+      <c r="G9" s="6">
         <v>10.5</v>
       </c>
-      <c r="G9" s="6">
+      <c r="H9" s="6">
         <v>4.99</v>
       </c>
-      <c r="H9" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="I9" s="6"/>
+      <c r="I9" s="6" t="s">
+        <v>18</v>
+      </c>
       <c r="J9" s="6"/>
       <c r="K9" s="6"/>
-    </row>
-    <row r="10" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="L9" s="6"/>
+    </row>
+    <row r="10" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A10" s="6">
         <v>9</v>
       </c>
       <c r="B10" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>BGB_ev_moist_closed</v>
+        <v>ALL_ev_moist_closed_BGB</v>
       </c>
       <c r="C10" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="D10" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="D10" s="6" t="s">
+      <c r="E10" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="E10" s="6" t="s">
+      <c r="F10" s="6" t="s">
         <v>48</v>
       </c>
-      <c r="F10" s="6">
+      <c r="G10" s="6">
         <v>26.78</v>
       </c>
-      <c r="G10" s="6">
+      <c r="H10" s="6">
         <v>5.56</v>
       </c>
-      <c r="H10" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="I10" s="6"/>
+      <c r="I10" s="6" t="s">
+        <v>18</v>
+      </c>
       <c r="J10" s="6"/>
       <c r="K10" s="6"/>
-    </row>
-    <row r="11" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="L10" s="6"/>
+    </row>
+    <row r="11" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A11" s="6">
         <v>10</v>
       </c>
       <c r="B11" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>BGB_md_moist_closed_se</v>
+        <v>ALL_md_moist_closed_se_BGB</v>
       </c>
       <c r="C11" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="D11" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="D11" s="6" t="s">
+      <c r="E11" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="E11" s="6" t="s">
+      <c r="F11" s="6" t="s">
         <v>48</v>
       </c>
-      <c r="F11" s="6">
+      <c r="G11" s="6">
         <v>25.85</v>
       </c>
-      <c r="G11" s="6">
+      <c r="H11" s="6">
         <v>3.62</v>
       </c>
-      <c r="H11" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="I11" s="6"/>
+      <c r="I11" s="6" t="s">
+        <v>18</v>
+      </c>
       <c r="J11" s="6"/>
       <c r="K11" s="6"/>
-    </row>
-    <row r="12" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="L11" s="6"/>
+    </row>
+    <row r="12" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A12" s="6">
         <v>11</v>
       </c>
       <c r="B12" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>BGB_md_moist_closed_nw</v>
+        <v>ALL_md_moist_closed_nw_BGB</v>
       </c>
       <c r="C12" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="D12" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="D12" s="6" t="s">
+      <c r="E12" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="E12" s="6" t="s">
+      <c r="F12" s="6" t="s">
         <v>48</v>
       </c>
-      <c r="F12" s="6">
+      <c r="G12" s="6">
         <v>18.989999999999998</v>
       </c>
-      <c r="G12" s="6">
+      <c r="H12" s="6">
         <v>2.13</v>
       </c>
-      <c r="H12" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="I12" s="6"/>
+      <c r="I12" s="6" t="s">
+        <v>18</v>
+      </c>
       <c r="J12" s="6"/>
       <c r="K12" s="6"/>
-    </row>
-    <row r="13" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="L12" s="6"/>
+    </row>
+    <row r="13" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A13" s="6">
         <v>12</v>
       </c>
       <c r="B13" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>BGB_ev_upland</v>
+        <v>ALL_ev_upland_BGB</v>
       </c>
       <c r="C13" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="D13" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="D13" s="6" t="s">
+      <c r="E13" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="E13" s="6" t="s">
+      <c r="F13" s="6" t="s">
         <v>48</v>
       </c>
-      <c r="F13" s="6">
+      <c r="G13" s="6">
         <v>24.09</v>
       </c>
-      <c r="G13" s="6">
+      <c r="H13" s="6">
         <v>2.6</v>
       </c>
-      <c r="H13" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="I13" s="6"/>
+      <c r="I13" s="6" t="s">
+        <v>18</v>
+      </c>
       <c r="J13" s="6"/>
       <c r="K13" s="6"/>
-    </row>
-    <row r="14" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="L13" s="6"/>
+    </row>
+    <row r="14" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A14" s="5">
         <v>13</v>
       </c>
       <c r="B14" s="5" t="str">
         <f t="shared" si="0"/>
-        <v>DW_open</v>
+        <v>ALL_open_DW</v>
       </c>
       <c r="C14" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="D14" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="D14" s="5" t="s">
+      <c r="E14" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="E14" s="5" t="s">
+      <c r="F14" s="5" t="s">
         <v>49</v>
       </c>
-      <c r="F14" s="5">
+      <c r="G14" s="5">
         <v>20.5</v>
       </c>
-      <c r="G14" s="5">
+      <c r="H14" s="5">
         <v>4.68</v>
       </c>
-      <c r="H14" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="I14" s="5"/>
+      <c r="I14" s="5" t="s">
+        <v>18</v>
+      </c>
       <c r="J14" s="5"/>
       <c r="K14" s="5"/>
-    </row>
-    <row r="15" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="L14" s="5"/>
+    </row>
+    <row r="15" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A15" s="5">
         <v>14</v>
       </c>
       <c r="B15" s="5" t="str">
         <f t="shared" si="0"/>
-        <v>DW_ev_wet_closed</v>
+        <v>ALL_ev_wet_closed_DW</v>
       </c>
       <c r="C15" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="D15" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="D15" s="5" t="s">
+      <c r="E15" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="E15" s="5" t="s">
+      <c r="F15" s="5" t="s">
         <v>49</v>
       </c>
-      <c r="F15" s="5">
+      <c r="G15" s="5">
         <v>28.97</v>
       </c>
-      <c r="G15" s="5">
+      <c r="H15" s="5">
         <v>24.34</v>
       </c>
-      <c r="H15" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="I15" s="5"/>
+      <c r="I15" s="5" t="s">
+        <v>18</v>
+      </c>
       <c r="J15" s="5"/>
       <c r="K15" s="5"/>
-    </row>
-    <row r="16" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="L15" s="5"/>
+    </row>
+    <row r="16" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A16" s="5">
         <v>15</v>
       </c>
       <c r="B16" s="5" t="str">
         <f t="shared" si="0"/>
-        <v>DW_ev_moist_closed</v>
+        <v>ALL_ev_moist_closed_DW</v>
       </c>
       <c r="C16" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="D16" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="D16" s="5" t="s">
+      <c r="E16" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="E16" s="5" t="s">
+      <c r="F16" s="5" t="s">
         <v>49</v>
       </c>
-      <c r="F16" s="5">
+      <c r="G16" s="5">
         <v>18.29</v>
       </c>
-      <c r="G16" s="5">
+      <c r="H16" s="5">
         <v>7.1</v>
       </c>
-      <c r="H16" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="I16" s="5"/>
+      <c r="I16" s="5" t="s">
+        <v>18</v>
+      </c>
       <c r="J16" s="5"/>
       <c r="K16" s="5"/>
-    </row>
-    <row r="17" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="L16" s="5"/>
+    </row>
+    <row r="17" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A17" s="5">
         <v>16</v>
       </c>
       <c r="B17" s="5" t="str">
         <f t="shared" si="0"/>
-        <v>DW_md_moist_closed_se</v>
+        <v>ALL_md_moist_closed_se_DW</v>
       </c>
       <c r="C17" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="D17" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="D17" s="5" t="s">
+      <c r="E17" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="E17" s="5" t="s">
+      <c r="F17" s="5" t="s">
         <v>49</v>
       </c>
-      <c r="F17" s="5">
+      <c r="G17" s="5">
         <v>65.83</v>
       </c>
-      <c r="G17" s="5">
+      <c r="H17" s="5">
         <v>24.52</v>
       </c>
-      <c r="H17" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="I17" s="5"/>
+      <c r="I17" s="5" t="s">
+        <v>18</v>
+      </c>
       <c r="J17" s="5"/>
       <c r="K17" s="5"/>
-    </row>
-    <row r="18" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="L17" s="5"/>
+    </row>
+    <row r="18" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A18" s="5">
         <v>17</v>
       </c>
       <c r="B18" s="5" t="str">
         <f t="shared" si="0"/>
-        <v>DW_md_moist_closed_nw</v>
+        <v>ALL_md_moist_closed_nw_DW</v>
       </c>
       <c r="C18" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="D18" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="D18" s="5" t="s">
+      <c r="E18" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="E18" s="5" t="s">
+      <c r="F18" s="5" t="s">
         <v>49</v>
       </c>
-      <c r="F18" s="5">
+      <c r="G18" s="5">
         <v>38.619999999999997</v>
       </c>
-      <c r="G18" s="5">
+      <c r="H18" s="5">
         <v>7.39</v>
       </c>
-      <c r="H18" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="I18" s="5"/>
+      <c r="I18" s="5" t="s">
+        <v>18</v>
+      </c>
       <c r="J18" s="5"/>
       <c r="K18" s="5"/>
-    </row>
-    <row r="19" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="L18" s="5"/>
+    </row>
+    <row r="19" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A19" s="5">
         <v>18</v>
       </c>
       <c r="B19" s="5" t="str">
         <f t="shared" si="0"/>
-        <v>DW_ev_upland</v>
+        <v>ALL_ev_upland_DW</v>
       </c>
       <c r="C19" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="D19" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="D19" s="5" t="s">
+      <c r="E19" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="E19" s="5" t="s">
+      <c r="F19" s="5" t="s">
         <v>49</v>
       </c>
-      <c r="F19" s="5">
+      <c r="G19" s="5">
         <v>41.93</v>
       </c>
-      <c r="G19" s="5">
+      <c r="H19" s="5">
         <v>15.59</v>
       </c>
-      <c r="H19" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="I19" s="5"/>
+      <c r="I19" s="5" t="s">
+        <v>18</v>
+      </c>
       <c r="J19" s="5"/>
       <c r="K19" s="5"/>
-    </row>
-    <row r="20" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="L19" s="5"/>
+    </row>
+    <row r="20" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A20" s="6">
         <v>19</v>
       </c>
       <c r="B20" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>LI_open</v>
+        <v>ALL_open_LI</v>
       </c>
       <c r="C20" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="D20" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="D20" s="6" t="s">
+      <c r="E20" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="E20" s="6" t="s">
+      <c r="F20" s="6" t="s">
         <v>50</v>
       </c>
-      <c r="F20" s="6">
+      <c r="G20" s="6">
         <v>2.6</v>
       </c>
-      <c r="G20" s="6">
+      <c r="H20" s="6">
         <v>0.43</v>
       </c>
-      <c r="H20" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="I20" s="6"/>
+      <c r="I20" s="6" t="s">
+        <v>18</v>
+      </c>
       <c r="J20" s="6"/>
       <c r="K20" s="6"/>
-    </row>
-    <row r="21" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="L20" s="6"/>
+    </row>
+    <row r="21" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A21" s="6">
         <v>20</v>
       </c>
       <c r="B21" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>LI_ev_wet_closed</v>
+        <v>ALL_ev_wet_closed_LI</v>
       </c>
       <c r="C21" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="D21" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="D21" s="6" t="s">
+      <c r="E21" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="E21" s="6" t="s">
+      <c r="F21" s="6" t="s">
         <v>50</v>
       </c>
-      <c r="F21" s="6">
+      <c r="G21" s="6">
         <v>2.98</v>
       </c>
-      <c r="G21" s="6">
+      <c r="H21" s="6">
         <v>0.4</v>
       </c>
-      <c r="H21" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="I21" s="6"/>
+      <c r="I21" s="6" t="s">
+        <v>18</v>
+      </c>
       <c r="J21" s="6"/>
       <c r="K21" s="6"/>
-    </row>
-    <row r="22" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="L21" s="6"/>
+    </row>
+    <row r="22" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A22" s="6">
         <v>21</v>
       </c>
       <c r="B22" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>LI_ev_moist_closed</v>
+        <v>ALL_ev_moist_closed_LI</v>
       </c>
       <c r="C22" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="D22" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="D22" s="6" t="s">
+      <c r="E22" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="E22" s="6" t="s">
+      <c r="F22" s="6" t="s">
         <v>50</v>
       </c>
-      <c r="F22" s="6">
+      <c r="G22" s="6">
         <v>3.31</v>
       </c>
-      <c r="G22" s="6">
+      <c r="H22" s="6">
         <v>1.1299999999999999</v>
       </c>
-      <c r="H22" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="I22" s="6"/>
+      <c r="I22" s="6" t="s">
+        <v>18</v>
+      </c>
       <c r="J22" s="6"/>
       <c r="K22" s="6"/>
-    </row>
-    <row r="23" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="L22" s="6"/>
+    </row>
+    <row r="23" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A23" s="6">
         <v>22</v>
       </c>
       <c r="B23" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>LI_md_moist_closed_se</v>
+        <v>ALL_md_moist_closed_se_LI</v>
       </c>
       <c r="C23" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="D23" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="D23" s="6" t="s">
+      <c r="E23" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="E23" s="6" t="s">
+      <c r="F23" s="6" t="s">
         <v>50</v>
       </c>
-      <c r="F23" s="6">
+      <c r="G23" s="6">
         <v>2.91</v>
       </c>
-      <c r="G23" s="6">
+      <c r="H23" s="6">
         <v>0.49</v>
       </c>
-      <c r="H23" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="I23" s="6"/>
+      <c r="I23" s="6" t="s">
+        <v>18</v>
+      </c>
       <c r="J23" s="6"/>
       <c r="K23" s="6"/>
-    </row>
-    <row r="24" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="L23" s="6"/>
+    </row>
+    <row r="24" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A24" s="6">
         <v>23</v>
       </c>
       <c r="B24" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>LI_md_moist_closed_nw</v>
+        <v>ALL_md_moist_closed_nw_LI</v>
       </c>
       <c r="C24" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="D24" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="D24" s="6" t="s">
+      <c r="E24" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="E24" s="6" t="s">
+      <c r="F24" s="6" t="s">
         <v>50</v>
       </c>
-      <c r="F24" s="6">
+      <c r="G24" s="6">
         <v>2.4</v>
       </c>
-      <c r="G24" s="6">
+      <c r="H24" s="6">
         <v>0.34</v>
       </c>
-      <c r="H24" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="I24" s="6"/>
+      <c r="I24" s="6" t="s">
+        <v>18</v>
+      </c>
       <c r="J24" s="6"/>
       <c r="K24" s="6"/>
-    </row>
-    <row r="25" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="L24" s="6"/>
+    </row>
+    <row r="25" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A25" s="6">
         <v>24</v>
       </c>
       <c r="B25" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>LI_ev_upland</v>
+        <v>ALL_ev_upland_LI</v>
       </c>
       <c r="C25" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="D25" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="D25" s="6" t="s">
+      <c r="E25" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="E25" s="6" t="s">
+      <c r="F25" s="6" t="s">
         <v>50</v>
       </c>
-      <c r="F25" s="6">
+      <c r="G25" s="6">
         <v>1.38</v>
       </c>
-      <c r="G25" s="6">
+      <c r="H25" s="6">
         <v>0.25</v>
       </c>
-      <c r="H25" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="I25" s="6"/>
+      <c r="I25" s="6" t="s">
+        <v>18</v>
+      </c>
       <c r="J25" s="6"/>
       <c r="K25" s="6"/>
-    </row>
-    <row r="26" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="L25" s="6"/>
+    </row>
+    <row r="26" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A26" s="5">
         <v>25</v>
       </c>
       <c r="B26" s="5" t="str">
         <f t="shared" si="0"/>
-        <v>SOC_open</v>
+        <v>ALL_open_SOC</v>
       </c>
       <c r="C26" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="D26" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="D26" s="5" t="s">
+      <c r="E26" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="E26" s="5" t="s">
+      <c r="F26" s="5" t="s">
         <v>51</v>
-      </c>
-      <c r="F26" s="5" t="s">
-        <v>52</v>
       </c>
       <c r="G26" s="5" t="s">
         <v>52</v>
       </c>
       <c r="H26" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="I26" s="5"/>
+        <v>52</v>
+      </c>
+      <c r="I26" s="5" t="s">
+        <v>18</v>
+      </c>
       <c r="J26" s="5"/>
       <c r="K26" s="5"/>
-    </row>
-    <row r="27" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="L26" s="5"/>
+    </row>
+    <row r="27" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A27" s="5">
         <v>26</v>
       </c>
       <c r="B27" s="5" t="str">
         <f t="shared" si="0"/>
-        <v>SOC_ev_wet_closed</v>
+        <v>ALL_ev_wet_closed_SOC</v>
       </c>
       <c r="C27" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="D27" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="D27" s="5" t="s">
+      <c r="E27" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="E27" s="5" t="s">
+      <c r="F27" s="5" t="s">
         <v>51</v>
-      </c>
-      <c r="F27" s="5" t="s">
-        <v>52</v>
       </c>
       <c r="G27" s="5" t="s">
         <v>52</v>
       </c>
       <c r="H27" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="I27" s="5"/>
+        <v>52</v>
+      </c>
+      <c r="I27" s="5" t="s">
+        <v>18</v>
+      </c>
       <c r="J27" s="5"/>
       <c r="K27" s="5"/>
-    </row>
-    <row r="28" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="L27" s="5"/>
+    </row>
+    <row r="28" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A28" s="5">
         <v>27</v>
       </c>
       <c r="B28" s="5" t="str">
         <f t="shared" si="0"/>
-        <v>SOC_ev_moist_closed</v>
+        <v>ALL_ev_moist_closed_SOC</v>
       </c>
       <c r="C28" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="D28" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="D28" s="5" t="s">
+      <c r="E28" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="E28" s="5" t="s">
+      <c r="F28" s="5" t="s">
         <v>51</v>
-      </c>
-      <c r="F28" s="5" t="s">
-        <v>52</v>
       </c>
       <c r="G28" s="5" t="s">
         <v>52</v>
       </c>
       <c r="H28" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="I28" s="5"/>
+        <v>52</v>
+      </c>
+      <c r="I28" s="5" t="s">
+        <v>18</v>
+      </c>
       <c r="J28" s="5"/>
       <c r="K28" s="5"/>
-    </row>
-    <row r="29" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="L28" s="5"/>
+    </row>
+    <row r="29" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A29" s="5">
         <v>28</v>
       </c>
       <c r="B29" s="5" t="str">
         <f t="shared" si="0"/>
-        <v>SOC_md_moist_closed_se</v>
+        <v>ALL_md_moist_closed_se_SOC</v>
       </c>
       <c r="C29" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="D29" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="D29" s="5" t="s">
+      <c r="E29" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="E29" s="5" t="s">
+      <c r="F29" s="5" t="s">
         <v>51</v>
-      </c>
-      <c r="F29" s="5" t="s">
-        <v>52</v>
       </c>
       <c r="G29" s="5" t="s">
         <v>52</v>
       </c>
       <c r="H29" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="I29" s="5"/>
+        <v>52</v>
+      </c>
+      <c r="I29" s="5" t="s">
+        <v>18</v>
+      </c>
       <c r="J29" s="5"/>
       <c r="K29" s="5"/>
-    </row>
-    <row r="30" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="L29" s="5"/>
+    </row>
+    <row r="30" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A30" s="5">
         <v>29</v>
       </c>
       <c r="B30" s="5" t="str">
         <f t="shared" si="0"/>
-        <v>SOC_md_moist_closed_nw</v>
+        <v>ALL_md_moist_closed_nw_SOC</v>
       </c>
       <c r="C30" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="D30" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="D30" s="5" t="s">
+      <c r="E30" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="E30" s="5" t="s">
+      <c r="F30" s="5" t="s">
         <v>51</v>
-      </c>
-      <c r="F30" s="5" t="s">
-        <v>52</v>
       </c>
       <c r="G30" s="5" t="s">
         <v>52</v>
       </c>
       <c r="H30" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="I30" s="5"/>
+        <v>52</v>
+      </c>
+      <c r="I30" s="5" t="s">
+        <v>18</v>
+      </c>
       <c r="J30" s="5"/>
       <c r="K30" s="5"/>
-    </row>
-    <row r="31" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="L30" s="5"/>
+    </row>
+    <row r="31" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A31" s="5">
         <v>30</v>
       </c>
       <c r="B31" s="5" t="str">
         <f t="shared" si="0"/>
-        <v>SOC_ev_upland</v>
+        <v>ALL_ev_upland_SOC</v>
       </c>
       <c r="C31" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="D31" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="D31" s="5" t="s">
+      <c r="E31" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="E31" s="5" t="s">
+      <c r="F31" s="5" t="s">
         <v>51</v>
-      </c>
-      <c r="F31" s="5" t="s">
-        <v>52</v>
       </c>
       <c r="G31" s="5" t="s">
         <v>52</v>
       </c>
       <c r="H31" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="I31" s="5"/>
+        <v>52</v>
+      </c>
+      <c r="I31" s="5" t="s">
+        <v>18</v>
+      </c>
       <c r="J31" s="5"/>
       <c r="K31" s="5"/>
-    </row>
-    <row r="32" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="L31" s="5"/>
+    </row>
+    <row r="32" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A32" s="6">
         <v>31</v>
       </c>
       <c r="B32" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>ALL_postdef_open</v>
+        <v>ALL_postdef_open_ALL</v>
       </c>
       <c r="C32" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="D32" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="D32" s="6" t="s">
+      <c r="E32" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="E32" s="6" t="s">
+      <c r="F32" s="6" t="s">
         <v>53</v>
       </c>
-      <c r="F32" s="6">
+      <c r="G32" s="6">
         <v>14.3</v>
       </c>
-      <c r="G32" s="6">
+      <c r="H32" s="6">
         <v>16.149999999999999</v>
       </c>
-      <c r="H32" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="I32" s="6"/>
+      <c r="I32" s="6" t="s">
+        <v>18</v>
+      </c>
       <c r="J32" s="6"/>
       <c r="K32" s="6"/>
-    </row>
-    <row r="33" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="L32" s="6"/>
+    </row>
+    <row r="33" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A33" s="6">
         <v>32</v>
       </c>
       <c r="B33" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>ALL_postdef_ev_wet_closed</v>
+        <v>ALL_postdef_ev_wet_closed_ALL</v>
       </c>
       <c r="C33" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="D33" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="D33" s="6" t="s">
+      <c r="E33" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="E33" s="6" t="s">
+      <c r="F33" s="6" t="s">
         <v>53</v>
       </c>
-      <c r="F33" s="6">
+      <c r="G33" s="6">
         <v>15.19</v>
       </c>
-      <c r="G33" s="6">
+      <c r="H33" s="6">
         <v>16.149999999999999</v>
       </c>
-      <c r="H33" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="I33" s="6"/>
+      <c r="I33" s="6" t="s">
+        <v>18</v>
+      </c>
       <c r="J33" s="6"/>
       <c r="K33" s="6"/>
-    </row>
-    <row r="34" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="L33" s="6"/>
+    </row>
+    <row r="34" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A34" s="6">
         <v>33</v>
       </c>
       <c r="B34" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>ALL_postdef_ev_moist_closed</v>
+        <v>ALL_postdef_ev_moist_closed_ALL</v>
       </c>
       <c r="C34" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="D34" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="D34" s="6" t="s">
+      <c r="E34" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="E34" s="6" t="s">
+      <c r="F34" s="6" t="s">
         <v>53</v>
       </c>
-      <c r="F34" s="6">
+      <c r="G34" s="6">
         <v>16.96</v>
       </c>
-      <c r="G34" s="6">
+      <c r="H34" s="6">
         <v>8.69</v>
       </c>
-      <c r="H34" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="I34" s="6"/>
+      <c r="I34" s="6" t="s">
+        <v>18</v>
+      </c>
       <c r="J34" s="6"/>
       <c r="K34" s="6"/>
-    </row>
-    <row r="35" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="L34" s="6"/>
+    </row>
+    <row r="35" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A35" s="6">
         <v>34</v>
       </c>
       <c r="B35" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>ALL_postdef_md_moist_closed_se</v>
+        <v>ALL_postdef_md_moist_closed_se_ALL</v>
       </c>
       <c r="C35" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="D35" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="D35" s="6" t="s">
+      <c r="E35" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="E35" s="6" t="s">
+      <c r="F35" s="6" t="s">
         <v>53</v>
       </c>
-      <c r="F35" s="6">
+      <c r="G35" s="6">
         <v>13.83</v>
       </c>
-      <c r="G35" s="6">
+      <c r="H35" s="6">
         <v>6.46</v>
       </c>
-      <c r="H35" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="I35" s="6"/>
+      <c r="I35" s="6" t="s">
+        <v>18</v>
+      </c>
       <c r="J35" s="6"/>
       <c r="K35" s="6"/>
-    </row>
-    <row r="36" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="L35" s="6"/>
+    </row>
+    <row r="36" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A36" s="6">
         <v>35</v>
       </c>
       <c r="B36" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>ALL_postdef_md_moist_closed_nw</v>
+        <v>ALL_postdef_md_moist_closed_nw_ALL</v>
       </c>
       <c r="C36" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="D36" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="D36" s="6" t="s">
+      <c r="E36" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="E36" s="6" t="s">
+      <c r="F36" s="6" t="s">
         <v>53</v>
       </c>
-      <c r="F36" s="6">
+      <c r="G36" s="6">
         <v>17.62</v>
       </c>
-      <c r="G36" s="6">
+      <c r="H36" s="6">
         <v>7.66</v>
       </c>
-      <c r="H36" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="I36" s="6"/>
+      <c r="I36" s="6" t="s">
+        <v>18</v>
+      </c>
       <c r="J36" s="6"/>
       <c r="K36" s="6"/>
-    </row>
-    <row r="37" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="L36" s="6"/>
+    </row>
+    <row r="37" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A37" s="6">
         <v>36</v>
       </c>
       <c r="B37" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>ALL_postdef_ev_upland</v>
+        <v>ALL_postdef_ev_upland_ALL</v>
       </c>
       <c r="C37" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="D37" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="D37" s="6" t="s">
+      <c r="E37" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="E37" s="6" t="s">
+      <c r="F37" s="6" t="s">
         <v>53</v>
       </c>
-      <c r="F37" s="6">
+      <c r="G37" s="6">
         <v>7.9</v>
       </c>
-      <c r="G37" s="6">
+      <c r="H37" s="6">
         <v>8.33</v>
       </c>
-      <c r="H37" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="I37" s="6"/>
+      <c r="I37" s="6" t="s">
+        <v>18</v>
+      </c>
       <c r="J37" s="6"/>
       <c r="K37" s="6"/>
-    </row>
-    <row r="38" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="L37" s="6"/>
+    </row>
+    <row r="38" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A38" s="18">
         <v>37</v>
       </c>
       <c r="B38" s="18" t="str">
         <f t="shared" si="0"/>
-        <v>DG_ratio_dg_open</v>
+        <v>ALL_dg_open_DG_ratio</v>
       </c>
       <c r="C38" s="18" t="s">
+        <v>53</v>
+      </c>
+      <c r="D38" s="18" t="s">
         <v>73</v>
       </c>
-      <c r="D38" s="18" t="s">
+      <c r="E38" s="18" t="s">
         <v>74</v>
       </c>
-      <c r="E38" s="18" t="s">
+      <c r="F38" s="18" t="s">
         <v>80</v>
       </c>
-      <c r="F38" s="18">
+      <c r="G38" s="18">
         <f>1-0.48</f>
         <v>0.52</v>
       </c>
-      <c r="G38" s="18">
+      <c r="H38" s="18">
         <v>7.2999999999999995E-2</v>
       </c>
-      <c r="H38" s="18" t="s">
+      <c r="I38" s="18" t="s">
         <v>87</v>
       </c>
-      <c r="I38" s="18">
-        <f>(F38*(1-F38)/(G38*G38)-1)*F38</f>
+      <c r="J38" s="18">
+        <f>(G38*(1-G38)/(H38*H38)-1)*G38</f>
         <v>23.835789078626387</v>
       </c>
-      <c r="J38" s="18">
-        <f>(F38*(1-F38)/(G38*G38)-1)*(1-F38)</f>
+      <c r="K38" s="18">
+        <f>(G38*(1-G38)/(H38*H38)-1)*(1-G38)</f>
         <v>22.002266841808972</v>
       </c>
-      <c r="K38" s="18"/>
-    </row>
-    <row r="39" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="L38" s="18"/>
+    </row>
+    <row r="39" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A39" s="18">
         <v>38</v>
       </c>
       <c r="B39" s="18" t="str">
         <f t="shared" si="0"/>
-        <v>DG_ratio_dg_ev_wet_closed</v>
+        <v>ALL_dg_ev_wet_closed_DG_ratio</v>
       </c>
       <c r="C39" s="18" t="s">
+        <v>53</v>
+      </c>
+      <c r="D39" s="18" t="s">
         <v>81</v>
       </c>
-      <c r="D39" s="18" t="s">
+      <c r="E39" s="18" t="s">
         <v>75</v>
       </c>
-      <c r="E39" s="18" t="s">
+      <c r="F39" s="18" t="s">
         <v>80</v>
       </c>
-      <c r="F39" s="18">
+      <c r="G39" s="18">
         <f>1-0.3</f>
         <v>0.7</v>
       </c>
-      <c r="G39" s="18">
+      <c r="H39" s="18">
         <v>2.5999999999999999E-2</v>
       </c>
-      <c r="H39" s="18" t="s">
+      <c r="I39" s="18" t="s">
         <v>87</v>
       </c>
-      <c r="I39" s="18">
-        <f t="shared" ref="I39:I43" si="1">(F39*(1-F39)/(G39*G39)-1)*F39</f>
+      <c r="J39" s="18">
+        <f t="shared" ref="J39:J43" si="1">(G39*(1-G39)/(H39*H39)-1)*G39</f>
         <v>216.75562130177516</v>
       </c>
-      <c r="J39" s="18">
-        <f t="shared" ref="J39:J43" si="2">(F39*(1-F39)/(G39*G39)-1)*(1-F39)</f>
+      <c r="K39" s="18">
+        <f t="shared" ref="K39:K43" si="2">(G39*(1-G39)/(H39*H39)-1)*(1-G39)</f>
         <v>92.895266272189374</v>
       </c>
-      <c r="K39" s="18"/>
-    </row>
-    <row r="40" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="L39" s="18"/>
+    </row>
+    <row r="40" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A40" s="18">
         <v>39</v>
       </c>
       <c r="B40" s="18" t="str">
         <f t="shared" si="0"/>
-        <v>DG_ratio_dg_ev_moist_closed</v>
+        <v>ALL_dg_ev_moist_closed_DG_ratio</v>
       </c>
       <c r="C40" s="18" t="s">
+        <v>53</v>
+      </c>
+      <c r="D40" s="18" t="s">
         <v>82</v>
       </c>
-      <c r="D40" s="18" t="s">
+      <c r="E40" s="18" t="s">
         <v>76</v>
       </c>
-      <c r="E40" s="18" t="s">
+      <c r="F40" s="18" t="s">
         <v>80</v>
       </c>
-      <c r="F40" s="18">
-        <f t="shared" ref="F40:F43" si="3">1-0.3</f>
+      <c r="G40" s="18">
+        <f t="shared" ref="G40:G43" si="3">1-0.3</f>
         <v>0.7</v>
       </c>
-      <c r="G40" s="18">
+      <c r="H40" s="18">
         <v>2.5999999999999999E-2</v>
       </c>
-      <c r="H40" s="18" t="s">
+      <c r="I40" s="18" t="s">
         <v>87</v>
       </c>
-      <c r="I40" s="18">
+      <c r="J40" s="18">
         <f t="shared" si="1"/>
         <v>216.75562130177516</v>
       </c>
-      <c r="J40" s="18">
+      <c r="K40" s="18">
         <f t="shared" si="2"/>
         <v>92.895266272189374</v>
       </c>
-      <c r="K40" s="18"/>
-    </row>
-    <row r="41" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="L40" s="18"/>
+    </row>
+    <row r="41" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A41" s="18">
         <v>40</v>
       </c>
       <c r="B41" s="18" t="str">
         <f t="shared" si="0"/>
-        <v>DG_ratio_dg_md_moist_closed_se</v>
+        <v>ALL_dg_md_moist_closed_se_DG_ratio</v>
       </c>
       <c r="C41" s="18" t="s">
+        <v>53</v>
+      </c>
+      <c r="D41" s="18" t="s">
         <v>83</v>
       </c>
-      <c r="D41" s="18" t="s">
+      <c r="E41" s="18" t="s">
         <v>77</v>
       </c>
-      <c r="E41" s="18" t="s">
+      <c r="F41" s="18" t="s">
         <v>80</v>
       </c>
-      <c r="F41" s="18">
+      <c r="G41" s="18">
         <f t="shared" si="3"/>
         <v>0.7</v>
       </c>
-      <c r="G41" s="18">
+      <c r="H41" s="18">
         <v>2.5999999999999999E-2</v>
       </c>
-      <c r="H41" s="18" t="s">
+      <c r="I41" s="18" t="s">
         <v>87</v>
       </c>
-      <c r="I41" s="18">
+      <c r="J41" s="18">
         <f t="shared" si="1"/>
         <v>216.75562130177516</v>
       </c>
-      <c r="J41" s="18">
+      <c r="K41" s="18">
         <f t="shared" si="2"/>
         <v>92.895266272189374</v>
       </c>
-      <c r="K41" s="18"/>
-    </row>
-    <row r="42" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="L41" s="18"/>
+    </row>
+    <row r="42" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A42" s="18">
         <v>41</v>
       </c>
       <c r="B42" s="18" t="str">
         <f t="shared" si="0"/>
-        <v>DG_ratio_dg_md_moist_closed_nw</v>
+        <v>ALL_dg_md_moist_closed_nw_DG_ratio</v>
       </c>
       <c r="C42" s="18" t="s">
+        <v>53</v>
+      </c>
+      <c r="D42" s="18" t="s">
         <v>84</v>
       </c>
-      <c r="D42" s="18" t="s">
+      <c r="E42" s="18" t="s">
         <v>78</v>
       </c>
-      <c r="E42" s="18" t="s">
+      <c r="F42" s="18" t="s">
         <v>80</v>
       </c>
-      <c r="F42" s="18">
+      <c r="G42" s="18">
         <f t="shared" si="3"/>
         <v>0.7</v>
       </c>
-      <c r="G42" s="18">
+      <c r="H42" s="18">
         <v>2.5999999999999999E-2</v>
       </c>
-      <c r="H42" s="18" t="s">
+      <c r="I42" s="18" t="s">
         <v>87</v>
       </c>
-      <c r="I42" s="18">
+      <c r="J42" s="18">
         <f t="shared" si="1"/>
         <v>216.75562130177516</v>
       </c>
-      <c r="J42" s="18">
+      <c r="K42" s="18">
         <f t="shared" si="2"/>
         <v>92.895266272189374</v>
       </c>
-      <c r="K42" s="18"/>
-    </row>
-    <row r="43" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="L42" s="18"/>
+    </row>
+    <row r="43" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A43" s="18">
         <v>42</v>
       </c>
       <c r="B43" s="18" t="str">
         <f t="shared" si="0"/>
-        <v>DG_ratio_dg_ev_upland</v>
+        <v>ALL_dg_ev_upland_DG_ratio</v>
       </c>
       <c r="C43" s="18" t="s">
+        <v>53</v>
+      </c>
+      <c r="D43" s="18" t="s">
         <v>85</v>
       </c>
-      <c r="D43" s="18" t="s">
+      <c r="E43" s="18" t="s">
         <v>79</v>
       </c>
-      <c r="E43" s="18" t="s">
+      <c r="F43" s="18" t="s">
         <v>80</v>
       </c>
-      <c r="F43" s="18">
+      <c r="G43" s="18">
         <f t="shared" si="3"/>
         <v>0.7</v>
       </c>
-      <c r="G43" s="18">
+      <c r="H43" s="18">
         <v>2.5999999999999999E-2</v>
       </c>
-      <c r="H43" s="18" t="s">
+      <c r="I43" s="18" t="s">
         <v>87</v>
       </c>
-      <c r="I43" s="18">
+      <c r="J43" s="18">
         <f t="shared" si="1"/>
         <v>216.75562130177516</v>
       </c>
-      <c r="J43" s="18">
+      <c r="K43" s="18">
         <f t="shared" si="2"/>
         <v>92.895266272189374</v>
       </c>
-      <c r="K43" s="18"/>
+      <c r="L43" s="18"/>
     </row>
   </sheetData>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="E2:E37" xr:uid="{00000000-0002-0000-0100-000003000000}">
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="F2:F37" xr:uid="{00000000-0002-0000-0100-000003000000}">
       <formula1>"AGB,BGB,DW,LI,SOC,ALL"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
solved UI pb when changing input file
</commit_message>
<xml_diff>
--- a/inst/extdata/example1.xlsx
+++ b/inst/extdata/example1.xlsx
@@ -8,17 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/gaelsola/Github-Collabs/mocaredd/inst/extdata/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{23CADB2F-88A2-AB43-8ED9-2466C694D2C1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DE622DAE-D5B5-9649-83F0-538B4EB112B7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-24640" yWindow="4780" windowWidth="22160" windowHeight="16860" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-24640" yWindow="4740" windowWidth="22160" windowHeight="16860" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="user_input_details" sheetId="6" r:id="rId1"/>
     <sheet name="user_inputs" sheetId="5" r:id="rId2"/>
     <sheet name="time_periods" sheetId="4" r:id="rId3"/>
-    <sheet name="AD_lu_transitions" sheetId="1" r:id="rId4"/>
-    <sheet name="c_stocks" sheetId="2" r:id="rId5"/>
-    <sheet name="c_stocks_old" sheetId="8" r:id="rId6"/>
+    <sheet name="AD_lu_transitions" sheetId="10" r:id="rId4"/>
+    <sheet name="c_stocks" sheetId="9" r:id="rId5"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -40,28 +39,10 @@
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
-    <author>tc={35B02895-20C4-2C4E-BAE2-5B882E755564}</author>
+    <author>tc={06DDC166-B212-EC49-A2FA-47E5D6BB99FE}</author>
   </authors>
   <commentList>
-    <comment ref="H26" authorId="0" shapeId="0" xr:uid="{35B02895-20C4-2C4E-BAE2-5B882E755564}">
-      <text>
-        <t>[Threaded comment]
-Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
-Comment:
-    Ghana: placeholder for SOC support in future versions</t>
-      </text>
-    </comment>
-  </commentList>
-</comments>
-</file>
-
-<file path=xl/comments2.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
-  <authors>
-    <author>tc={6F402312-6687-204C-BC4B-C8641010B8EF}</author>
-  </authors>
-  <commentList>
-    <comment ref="G26" authorId="0" shapeId="0" xr:uid="{6F402312-6687-204C-BC4B-C8641010B8EF}">
+    <comment ref="H26" authorId="0" shapeId="0" xr:uid="{06DDC166-B212-EC49-A2FA-47E5D6BB99FE}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -74,7 +55,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="889" uniqueCount="102">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="626" uniqueCount="101">
   <si>
     <t>trans_no</t>
   </si>
@@ -368,9 +349,6 @@
   </si>
   <si>
     <t>REF</t>
-  </si>
-  <si>
-    <t>s</t>
   </si>
   <si>
     <t>MON1</t>
@@ -760,15 +738,7 @@
 
 <file path=xl/threadedComments/threadedComment1.xml><?xml version="1.0" encoding="utf-8"?>
 <ThreadedComments xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <threadedComment ref="H26" dT="2024-10-18T07:06:16.55" personId="{346CA1BB-775C-874F-8397-56904622A61E}" id="{35B02895-20C4-2C4E-BAE2-5B882E755564}">
-    <text>Ghana: placeholder for SOC support in future versions</text>
-  </threadedComment>
-</ThreadedComments>
-</file>
-
-<file path=xl/threadedComments/threadedComment2.xml><?xml version="1.0" encoding="utf-8"?>
-<ThreadedComments xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <threadedComment ref="G26" dT="2024-10-18T07:06:16.55" personId="{346CA1BB-775C-874F-8397-56904622A61E}" id="{6F402312-6687-204C-BC4B-C8641010B8EF}">
+  <threadedComment ref="H26" dT="2024-10-18T07:06:16.55" personId="{346CA1BB-775C-874F-8397-56904622A61E}" id="{06DDC166-B212-EC49-A2FA-47E5D6BB99FE}">
     <text>Ghana: placeholder for SOC support in future versions</text>
   </threadedComment>
 </ThreadedComments>
@@ -950,7 +920,7 @@
   <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -997,7 +967,7 @@
         <v>2019</v>
       </c>
       <c r="D3" s="7" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.15">
@@ -1011,7 +981,7 @@
         <v>2020</v>
       </c>
       <c r="D4" s="7" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.15">
@@ -1025,7 +995,7 @@
         <v>2021</v>
       </c>
       <c r="D5" s="7" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
   </sheetData>
@@ -1034,14 +1004,14 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4FBD584A-3C50-2A48-B2AD-AFCD6F08F4C8}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
   <dimension ref="A1:N49"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="127" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+    <sheetView topLeftCell="A33" zoomScale="127" workbookViewId="0">
+      <selection activeCell="F60" sqref="F60"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -2974,14 +2944,14 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8D402F9E-AC0E-614F-ACB5-63E242DFE6FF}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
   <dimension ref="A1:L43"/>
   <sheetViews>
-    <sheetView zoomScale="109" workbookViewId="0">
-      <selection activeCell="J2" sqref="J2"/>
+    <sheetView tabSelected="1" zoomScale="109" workbookViewId="0">
+      <selection activeCell="B32" sqref="B32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -3006,7 +2976,7 @@
         <v>36</v>
       </c>
       <c r="C1" s="8" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="D1" s="8" t="s">
         <v>37</v>
@@ -4466,1883 +4436,7 @@
     </row>
   </sheetData>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="F2:F37" xr:uid="{00000000-0002-0000-0100-000003000000}">
-      <formula1>"AGB,BGB,DW,LI,SOC,ALL"</formula1>
-    </dataValidation>
-  </dataValidations>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <legacyDrawing r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{07289E27-3AAB-8442-B8AB-764F61441691}">
-  <sheetPr>
-    <outlinePr summaryBelow="0" summaryRight="0"/>
-  </sheetPr>
-  <dimension ref="A1:K61"/>
-  <sheetViews>
-    <sheetView topLeftCell="A19" zoomScale="109" workbookViewId="0">
-      <selection activeCell="F58" sqref="F58"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-  <cols>
-    <col min="1" max="1" width="5.83203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="29.1640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="24.83203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="35.33203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="8" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="8.6640625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="6.1640625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="6.5" bestFit="1" customWidth="1"/>
-    <col min="9" max="11" width="8.83203125" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="8" t="s">
-        <v>35</v>
-      </c>
-      <c r="B1" s="8" t="s">
-        <v>36</v>
-      </c>
-      <c r="C1" s="8" t="s">
-        <v>37</v>
-      </c>
-      <c r="D1" s="8" t="s">
-        <v>38</v>
-      </c>
-      <c r="E1" s="8" t="s">
-        <v>54</v>
-      </c>
-      <c r="F1" s="8" t="s">
-        <v>40</v>
-      </c>
-      <c r="G1" s="8" t="s">
-        <v>41</v>
-      </c>
-      <c r="H1" s="8" t="s">
-        <v>42</v>
-      </c>
-      <c r="I1" s="8" t="s">
-        <v>43</v>
-      </c>
-      <c r="J1" s="8" t="s">
-        <v>44</v>
-      </c>
-      <c r="K1" s="8" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="2" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A2" s="5">
-        <v>1</v>
-      </c>
-      <c r="B2" s="5" t="str">
-        <f t="shared" ref="B2:B33" si="0">E2&amp;"_"&amp;C2</f>
-        <v>AGB_open</v>
-      </c>
-      <c r="C2" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="D2" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="E2" s="5" t="s">
-        <v>46</v>
-      </c>
-      <c r="F2" s="5">
-        <v>27.35</v>
-      </c>
-      <c r="G2" s="5">
-        <v>5.35</v>
-      </c>
-      <c r="H2" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="I2" s="5"/>
-      <c r="J2" s="5"/>
-      <c r="K2" s="5"/>
-    </row>
-    <row r="3" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A3" s="5">
-        <v>2</v>
-      </c>
-      <c r="B3" s="5" t="str">
-        <f t="shared" si="0"/>
-        <v>AGB_ev_wet_closed</v>
-      </c>
-      <c r="C3" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="D3" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="E3" s="5" t="s">
-        <v>46</v>
-      </c>
-      <c r="F3" s="5">
-        <v>81.28</v>
-      </c>
-      <c r="G3" s="5">
-        <v>43.43</v>
-      </c>
-      <c r="H3" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="I3" s="5"/>
-      <c r="J3" s="5"/>
-      <c r="K3" s="5"/>
-    </row>
-    <row r="4" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A4" s="5">
-        <v>3</v>
-      </c>
-      <c r="B4" s="5" t="str">
-        <f t="shared" si="0"/>
-        <v>AGB_ev_moist_closed</v>
-      </c>
-      <c r="C4" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="D4" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="E4" s="5" t="s">
-        <v>46</v>
-      </c>
-      <c r="F4" s="5">
-        <v>202.85</v>
-      </c>
-      <c r="G4" s="5">
-        <v>41.5</v>
-      </c>
-      <c r="H4" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="I4" s="5"/>
-      <c r="J4" s="5"/>
-      <c r="K4" s="5"/>
-    </row>
-    <row r="5" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A5" s="5">
-        <v>4</v>
-      </c>
-      <c r="B5" s="5" t="str">
-        <f t="shared" si="0"/>
-        <v>AGB_md_moist_closed_se</v>
-      </c>
-      <c r="C5" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="D5" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="E5" s="5" t="s">
-        <v>46</v>
-      </c>
-      <c r="F5" s="5">
-        <v>100.46</v>
-      </c>
-      <c r="G5" s="5">
-        <v>35.29</v>
-      </c>
-      <c r="H5" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="I5" s="5"/>
-      <c r="J5" s="5"/>
-      <c r="K5" s="5"/>
-    </row>
-    <row r="6" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A6" s="5">
-        <v>5</v>
-      </c>
-      <c r="B6" s="5" t="str">
-        <f t="shared" si="0"/>
-        <v>AGB_md_moist_closed_nw</v>
-      </c>
-      <c r="C6" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="D6" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="E6" s="5" t="s">
-        <v>46</v>
-      </c>
-      <c r="F6" s="5">
-        <v>75.91</v>
-      </c>
-      <c r="G6" s="5">
-        <v>11</v>
-      </c>
-      <c r="H6" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="I6" s="5"/>
-      <c r="J6" s="5"/>
-      <c r="K6" s="5"/>
-    </row>
-    <row r="7" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A7" s="5">
-        <v>6</v>
-      </c>
-      <c r="B7" s="5" t="str">
-        <f t="shared" si="0"/>
-        <v>AGB_ev_upland</v>
-      </c>
-      <c r="C7" s="5" t="s">
-        <v>31</v>
-      </c>
-      <c r="D7" s="5" t="s">
-        <v>32</v>
-      </c>
-      <c r="E7" s="5" t="s">
-        <v>46</v>
-      </c>
-      <c r="F7" s="5">
-        <v>74.599999999999994</v>
-      </c>
-      <c r="G7" s="5">
-        <v>13.87</v>
-      </c>
-      <c r="H7" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="I7" s="5"/>
-      <c r="J7" s="5"/>
-      <c r="K7" s="5"/>
-    </row>
-    <row r="8" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A8" s="6">
-        <v>7</v>
-      </c>
-      <c r="B8" s="6" t="str">
-        <f t="shared" si="0"/>
-        <v>BGB_open</v>
-      </c>
-      <c r="C8" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="D8" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="E8" s="6" t="s">
-        <v>48</v>
-      </c>
-      <c r="F8" s="6">
-        <v>10.37</v>
-      </c>
-      <c r="G8" s="6">
-        <v>1.85</v>
-      </c>
-      <c r="H8" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="I8" s="6"/>
-      <c r="J8" s="6"/>
-      <c r="K8" s="6"/>
-    </row>
-    <row r="9" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A9" s="6">
-        <v>8</v>
-      </c>
-      <c r="B9" s="6" t="str">
-        <f t="shared" si="0"/>
-        <v>BGB_ev_wet_closed</v>
-      </c>
-      <c r="C9" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="D9" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="E9" s="6" t="s">
-        <v>48</v>
-      </c>
-      <c r="F9" s="6">
-        <v>10.5</v>
-      </c>
-      <c r="G9" s="6">
-        <v>4.99</v>
-      </c>
-      <c r="H9" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="I9" s="6"/>
-      <c r="J9" s="6"/>
-      <c r="K9" s="6"/>
-    </row>
-    <row r="10" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A10" s="6">
-        <v>9</v>
-      </c>
-      <c r="B10" s="6" t="str">
-        <f t="shared" si="0"/>
-        <v>BGB_ev_moist_closed</v>
-      </c>
-      <c r="C10" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="D10" s="6" t="s">
-        <v>23</v>
-      </c>
-      <c r="E10" s="6" t="s">
-        <v>48</v>
-      </c>
-      <c r="F10" s="6">
-        <v>26.78</v>
-      </c>
-      <c r="G10" s="6">
-        <v>5.56</v>
-      </c>
-      <c r="H10" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="I10" s="6"/>
-      <c r="J10" s="6"/>
-      <c r="K10" s="6"/>
-    </row>
-    <row r="11" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A11" s="6">
-        <v>10</v>
-      </c>
-      <c r="B11" s="6" t="str">
-        <f t="shared" si="0"/>
-        <v>BGB_md_moist_closed_se</v>
-      </c>
-      <c r="C11" s="6" t="s">
-        <v>25</v>
-      </c>
-      <c r="D11" s="6" t="s">
-        <v>26</v>
-      </c>
-      <c r="E11" s="6" t="s">
-        <v>48</v>
-      </c>
-      <c r="F11" s="6">
-        <v>25.85</v>
-      </c>
-      <c r="G11" s="6">
-        <v>3.62</v>
-      </c>
-      <c r="H11" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="I11" s="6"/>
-      <c r="J11" s="6"/>
-      <c r="K11" s="6"/>
-    </row>
-    <row r="12" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A12" s="6">
-        <v>11</v>
-      </c>
-      <c r="B12" s="6" t="str">
-        <f t="shared" si="0"/>
-        <v>BGB_md_moist_closed_nw</v>
-      </c>
-      <c r="C12" s="6" t="s">
-        <v>28</v>
-      </c>
-      <c r="D12" s="6" t="s">
-        <v>29</v>
-      </c>
-      <c r="E12" s="6" t="s">
-        <v>48</v>
-      </c>
-      <c r="F12" s="6">
-        <v>18.989999999999998</v>
-      </c>
-      <c r="G12" s="6">
-        <v>2.13</v>
-      </c>
-      <c r="H12" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="I12" s="6"/>
-      <c r="J12" s="6"/>
-      <c r="K12" s="6"/>
-    </row>
-    <row r="13" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A13" s="6">
-        <v>12</v>
-      </c>
-      <c r="B13" s="6" t="str">
-        <f t="shared" si="0"/>
-        <v>BGB_ev_upland</v>
-      </c>
-      <c r="C13" s="6" t="s">
-        <v>31</v>
-      </c>
-      <c r="D13" s="6" t="s">
-        <v>32</v>
-      </c>
-      <c r="E13" s="6" t="s">
-        <v>48</v>
-      </c>
-      <c r="F13" s="6">
-        <v>24.09</v>
-      </c>
-      <c r="G13" s="6">
-        <v>2.6</v>
-      </c>
-      <c r="H13" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="I13" s="6"/>
-      <c r="J13" s="6"/>
-      <c r="K13" s="6"/>
-    </row>
-    <row r="14" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A14" s="5">
-        <v>13</v>
-      </c>
-      <c r="B14" s="5" t="str">
-        <f t="shared" si="0"/>
-        <v>DW_open</v>
-      </c>
-      <c r="C14" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="D14" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="E14" s="5" t="s">
-        <v>49</v>
-      </c>
-      <c r="F14" s="5">
-        <v>20.5</v>
-      </c>
-      <c r="G14" s="5">
-        <v>4.68</v>
-      </c>
-      <c r="H14" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="I14" s="5"/>
-      <c r="J14" s="5"/>
-      <c r="K14" s="5"/>
-    </row>
-    <row r="15" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A15" s="5">
-        <v>14</v>
-      </c>
-      <c r="B15" s="5" t="str">
-        <f t="shared" si="0"/>
-        <v>DW_ev_wet_closed</v>
-      </c>
-      <c r="C15" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="D15" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="E15" s="5" t="s">
-        <v>49</v>
-      </c>
-      <c r="F15" s="5">
-        <v>28.97</v>
-      </c>
-      <c r="G15" s="5">
-        <v>24.34</v>
-      </c>
-      <c r="H15" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="I15" s="5"/>
-      <c r="J15" s="5"/>
-      <c r="K15" s="5"/>
-    </row>
-    <row r="16" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A16" s="5">
-        <v>15</v>
-      </c>
-      <c r="B16" s="5" t="str">
-        <f t="shared" si="0"/>
-        <v>DW_ev_moist_closed</v>
-      </c>
-      <c r="C16" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="D16" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="E16" s="5" t="s">
-        <v>49</v>
-      </c>
-      <c r="F16" s="5">
-        <v>18.29</v>
-      </c>
-      <c r="G16" s="5">
-        <v>7.1</v>
-      </c>
-      <c r="H16" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="I16" s="5"/>
-      <c r="J16" s="5"/>
-      <c r="K16" s="5"/>
-    </row>
-    <row r="17" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A17" s="5">
-        <v>16</v>
-      </c>
-      <c r="B17" s="5" t="str">
-        <f t="shared" si="0"/>
-        <v>DW_md_moist_closed_se</v>
-      </c>
-      <c r="C17" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="D17" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="E17" s="5" t="s">
-        <v>49</v>
-      </c>
-      <c r="F17" s="5">
-        <v>65.83</v>
-      </c>
-      <c r="G17" s="5">
-        <v>24.52</v>
-      </c>
-      <c r="H17" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="I17" s="5"/>
-      <c r="J17" s="5"/>
-      <c r="K17" s="5"/>
-    </row>
-    <row r="18" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A18" s="5">
-        <v>17</v>
-      </c>
-      <c r="B18" s="5" t="str">
-        <f t="shared" si="0"/>
-        <v>DW_md_moist_closed_nw</v>
-      </c>
-      <c r="C18" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="D18" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="E18" s="5" t="s">
-        <v>49</v>
-      </c>
-      <c r="F18" s="5">
-        <v>38.619999999999997</v>
-      </c>
-      <c r="G18" s="5">
-        <v>7.39</v>
-      </c>
-      <c r="H18" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="I18" s="5"/>
-      <c r="J18" s="5"/>
-      <c r="K18" s="5"/>
-    </row>
-    <row r="19" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A19" s="5">
-        <v>18</v>
-      </c>
-      <c r="B19" s="5" t="str">
-        <f t="shared" si="0"/>
-        <v>DW_ev_upland</v>
-      </c>
-      <c r="C19" s="5" t="s">
-        <v>31</v>
-      </c>
-      <c r="D19" s="5" t="s">
-        <v>32</v>
-      </c>
-      <c r="E19" s="5" t="s">
-        <v>49</v>
-      </c>
-      <c r="F19" s="5">
-        <v>41.93</v>
-      </c>
-      <c r="G19" s="5">
-        <v>15.59</v>
-      </c>
-      <c r="H19" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="I19" s="5"/>
-      <c r="J19" s="5"/>
-      <c r="K19" s="5"/>
-    </row>
-    <row r="20" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A20" s="6">
-        <v>19</v>
-      </c>
-      <c r="B20" s="6" t="str">
-        <f t="shared" si="0"/>
-        <v>LI_open</v>
-      </c>
-      <c r="C20" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="D20" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="E20" s="6" t="s">
-        <v>50</v>
-      </c>
-      <c r="F20" s="6">
-        <v>2.6</v>
-      </c>
-      <c r="G20" s="6">
-        <v>0.43</v>
-      </c>
-      <c r="H20" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="I20" s="6"/>
-      <c r="J20" s="6"/>
-      <c r="K20" s="6"/>
-    </row>
-    <row r="21" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A21" s="6">
-        <v>20</v>
-      </c>
-      <c r="B21" s="6" t="str">
-        <f t="shared" si="0"/>
-        <v>LI_ev_wet_closed</v>
-      </c>
-      <c r="C21" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="D21" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="E21" s="6" t="s">
-        <v>50</v>
-      </c>
-      <c r="F21" s="6">
-        <v>2.98</v>
-      </c>
-      <c r="G21" s="6">
-        <v>0.4</v>
-      </c>
-      <c r="H21" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="I21" s="6"/>
-      <c r="J21" s="6"/>
-      <c r="K21" s="6"/>
-    </row>
-    <row r="22" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A22" s="6">
-        <v>21</v>
-      </c>
-      <c r="B22" s="6" t="str">
-        <f t="shared" si="0"/>
-        <v>LI_ev_moist_closed</v>
-      </c>
-      <c r="C22" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="D22" s="6" t="s">
-        <v>23</v>
-      </c>
-      <c r="E22" s="6" t="s">
-        <v>50</v>
-      </c>
-      <c r="F22" s="6">
-        <v>3.31</v>
-      </c>
-      <c r="G22" s="6">
-        <v>1.1299999999999999</v>
-      </c>
-      <c r="H22" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="I22" s="6"/>
-      <c r="J22" s="6"/>
-      <c r="K22" s="6"/>
-    </row>
-    <row r="23" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A23" s="6">
-        <v>22</v>
-      </c>
-      <c r="B23" s="6" t="str">
-        <f t="shared" si="0"/>
-        <v>LI_md_moist_closed_se</v>
-      </c>
-      <c r="C23" s="6" t="s">
-        <v>25</v>
-      </c>
-      <c r="D23" s="6" t="s">
-        <v>26</v>
-      </c>
-      <c r="E23" s="6" t="s">
-        <v>50</v>
-      </c>
-      <c r="F23" s="6">
-        <v>2.91</v>
-      </c>
-      <c r="G23" s="6">
-        <v>0.49</v>
-      </c>
-      <c r="H23" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="I23" s="6"/>
-      <c r="J23" s="6"/>
-      <c r="K23" s="6"/>
-    </row>
-    <row r="24" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A24" s="6">
-        <v>23</v>
-      </c>
-      <c r="B24" s="6" t="str">
-        <f t="shared" si="0"/>
-        <v>LI_md_moist_closed_nw</v>
-      </c>
-      <c r="C24" s="6" t="s">
-        <v>28</v>
-      </c>
-      <c r="D24" s="6" t="s">
-        <v>29</v>
-      </c>
-      <c r="E24" s="6" t="s">
-        <v>50</v>
-      </c>
-      <c r="F24" s="6">
-        <v>2.4</v>
-      </c>
-      <c r="G24" s="6">
-        <v>0.34</v>
-      </c>
-      <c r="H24" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="I24" s="6"/>
-      <c r="J24" s="6"/>
-      <c r="K24" s="6"/>
-    </row>
-    <row r="25" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A25" s="6">
-        <v>24</v>
-      </c>
-      <c r="B25" s="6" t="str">
-        <f t="shared" si="0"/>
-        <v>LI_ev_upland</v>
-      </c>
-      <c r="C25" s="6" t="s">
-        <v>31</v>
-      </c>
-      <c r="D25" s="6" t="s">
-        <v>32</v>
-      </c>
-      <c r="E25" s="6" t="s">
-        <v>50</v>
-      </c>
-      <c r="F25" s="6">
-        <v>1.38</v>
-      </c>
-      <c r="G25" s="6">
-        <v>0.25</v>
-      </c>
-      <c r="H25" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="I25" s="6"/>
-      <c r="J25" s="6"/>
-      <c r="K25" s="6"/>
-    </row>
-    <row r="26" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A26" s="5">
-        <v>25</v>
-      </c>
-      <c r="B26" s="5" t="str">
-        <f t="shared" si="0"/>
-        <v>SOC_open</v>
-      </c>
-      <c r="C26" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="D26" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="E26" s="5" t="s">
-        <v>51</v>
-      </c>
-      <c r="F26" s="5" t="s">
-        <v>52</v>
-      </c>
-      <c r="G26" s="5" t="s">
-        <v>52</v>
-      </c>
-      <c r="H26" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="I26" s="5"/>
-      <c r="J26" s="5"/>
-      <c r="K26" s="5"/>
-    </row>
-    <row r="27" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A27" s="5">
-        <v>26</v>
-      </c>
-      <c r="B27" s="5" t="str">
-        <f t="shared" si="0"/>
-        <v>SOC_ev_wet_closed</v>
-      </c>
-      <c r="C27" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="D27" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="E27" s="5" t="s">
-        <v>51</v>
-      </c>
-      <c r="F27" s="5" t="s">
-        <v>52</v>
-      </c>
-      <c r="G27" s="5" t="s">
-        <v>52</v>
-      </c>
-      <c r="H27" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="I27" s="5"/>
-      <c r="J27" s="5"/>
-      <c r="K27" s="5"/>
-    </row>
-    <row r="28" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A28" s="5">
-        <v>27</v>
-      </c>
-      <c r="B28" s="5" t="str">
-        <f t="shared" si="0"/>
-        <v>SOC_ev_moist_closed</v>
-      </c>
-      <c r="C28" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="D28" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="E28" s="5" t="s">
-        <v>51</v>
-      </c>
-      <c r="F28" s="5" t="s">
-        <v>52</v>
-      </c>
-      <c r="G28" s="5" t="s">
-        <v>52</v>
-      </c>
-      <c r="H28" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="I28" s="5"/>
-      <c r="J28" s="5"/>
-      <c r="K28" s="5"/>
-    </row>
-    <row r="29" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A29" s="5">
-        <v>28</v>
-      </c>
-      <c r="B29" s="5" t="str">
-        <f t="shared" si="0"/>
-        <v>SOC_md_moist_closed_se</v>
-      </c>
-      <c r="C29" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="D29" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="E29" s="5" t="s">
-        <v>51</v>
-      </c>
-      <c r="F29" s="5" t="s">
-        <v>52</v>
-      </c>
-      <c r="G29" s="5" t="s">
-        <v>52</v>
-      </c>
-      <c r="H29" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="I29" s="5"/>
-      <c r="J29" s="5"/>
-      <c r="K29" s="5"/>
-    </row>
-    <row r="30" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A30" s="5">
-        <v>29</v>
-      </c>
-      <c r="B30" s="5" t="str">
-        <f t="shared" si="0"/>
-        <v>SOC_md_moist_closed_nw</v>
-      </c>
-      <c r="C30" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="D30" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="E30" s="5" t="s">
-        <v>51</v>
-      </c>
-      <c r="F30" s="5" t="s">
-        <v>52</v>
-      </c>
-      <c r="G30" s="5" t="s">
-        <v>52</v>
-      </c>
-      <c r="H30" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="I30" s="5"/>
-      <c r="J30" s="5"/>
-      <c r="K30" s="5"/>
-    </row>
-    <row r="31" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A31" s="5">
-        <v>30</v>
-      </c>
-      <c r="B31" s="5" t="str">
-        <f t="shared" si="0"/>
-        <v>SOC_ev_upland</v>
-      </c>
-      <c r="C31" s="5" t="s">
-        <v>31</v>
-      </c>
-      <c r="D31" s="5" t="s">
-        <v>32</v>
-      </c>
-      <c r="E31" s="5" t="s">
-        <v>51</v>
-      </c>
-      <c r="F31" s="5" t="s">
-        <v>52</v>
-      </c>
-      <c r="G31" s="5" t="s">
-        <v>52</v>
-      </c>
-      <c r="H31" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="I31" s="5"/>
-      <c r="J31" s="5"/>
-      <c r="K31" s="5"/>
-    </row>
-    <row r="32" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A32" s="6">
-        <v>31</v>
-      </c>
-      <c r="B32" s="6" t="str">
-        <f t="shared" si="0"/>
-        <v>ALL_postdef_open</v>
-      </c>
-      <c r="C32" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="D32" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="E32" s="6" t="s">
-        <v>53</v>
-      </c>
-      <c r="F32" s="6">
-        <v>14.3</v>
-      </c>
-      <c r="G32" s="6">
-        <v>16.149999999999999</v>
-      </c>
-      <c r="H32" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="I32" s="6"/>
-      <c r="J32" s="6"/>
-      <c r="K32" s="6"/>
-    </row>
-    <row r="33" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A33" s="6">
-        <v>32</v>
-      </c>
-      <c r="B33" s="6" t="str">
-        <f t="shared" si="0"/>
-        <v>ALL_postdef_ev_wet_closed</v>
-      </c>
-      <c r="C33" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="D33" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="E33" s="6" t="s">
-        <v>53</v>
-      </c>
-      <c r="F33" s="6">
-        <v>15.19</v>
-      </c>
-      <c r="G33" s="6">
-        <v>16.149999999999999</v>
-      </c>
-      <c r="H33" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="I33" s="6"/>
-      <c r="J33" s="6"/>
-      <c r="K33" s="6"/>
-    </row>
-    <row r="34" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A34" s="6">
-        <v>33</v>
-      </c>
-      <c r="B34" s="6" t="str">
-        <f t="shared" ref="B34:B61" si="1">E34&amp;"_"&amp;C34</f>
-        <v>ALL_postdef_ev_moist_closed</v>
-      </c>
-      <c r="C34" s="6" t="s">
-        <v>24</v>
-      </c>
-      <c r="D34" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="E34" s="6" t="s">
-        <v>53</v>
-      </c>
-      <c r="F34" s="6">
-        <v>16.96</v>
-      </c>
-      <c r="G34" s="6">
-        <v>8.69</v>
-      </c>
-      <c r="H34" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="I34" s="6"/>
-      <c r="J34" s="6"/>
-      <c r="K34" s="6"/>
-    </row>
-    <row r="35" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A35" s="6">
-        <v>34</v>
-      </c>
-      <c r="B35" s="6" t="str">
-        <f t="shared" si="1"/>
-        <v>ALL_postdef_md_moist_closed_se</v>
-      </c>
-      <c r="C35" s="6" t="s">
-        <v>27</v>
-      </c>
-      <c r="D35" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="E35" s="6" t="s">
-        <v>53</v>
-      </c>
-      <c r="F35" s="6">
-        <v>13.83</v>
-      </c>
-      <c r="G35" s="6">
-        <v>6.46</v>
-      </c>
-      <c r="H35" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="I35" s="6"/>
-      <c r="J35" s="6"/>
-      <c r="K35" s="6"/>
-    </row>
-    <row r="36" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A36" s="6">
-        <v>35</v>
-      </c>
-      <c r="B36" s="6" t="str">
-        <f t="shared" si="1"/>
-        <v>ALL_postdef_md_moist_closed_nw</v>
-      </c>
-      <c r="C36" s="6" t="s">
-        <v>30</v>
-      </c>
-      <c r="D36" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="E36" s="6" t="s">
-        <v>53</v>
-      </c>
-      <c r="F36" s="6">
-        <v>17.62</v>
-      </c>
-      <c r="G36" s="6">
-        <v>7.66</v>
-      </c>
-      <c r="H36" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="I36" s="6"/>
-      <c r="J36" s="6"/>
-      <c r="K36" s="6"/>
-    </row>
-    <row r="37" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A37" s="6">
-        <v>36</v>
-      </c>
-      <c r="B37" s="6" t="str">
-        <f t="shared" si="1"/>
-        <v>ALL_postdef_ev_upland</v>
-      </c>
-      <c r="C37" s="6" t="s">
-        <v>33</v>
-      </c>
-      <c r="D37" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="E37" s="6" t="s">
-        <v>53</v>
-      </c>
-      <c r="F37" s="6">
-        <v>7.9</v>
-      </c>
-      <c r="G37" s="6">
-        <v>8.33</v>
-      </c>
-      <c r="H37" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="I37" s="6"/>
-      <c r="J37" s="6"/>
-      <c r="K37" s="6"/>
-    </row>
-    <row r="38" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A38" s="5">
-        <v>37</v>
-      </c>
-      <c r="B38" s="5" t="str">
-        <f t="shared" si="1"/>
-        <v>AGB_dg_open</v>
-      </c>
-      <c r="C38" s="5" t="s">
-        <v>73</v>
-      </c>
-      <c r="D38" s="5" t="s">
-        <v>74</v>
-      </c>
-      <c r="E38" s="5" t="s">
-        <v>46</v>
-      </c>
-      <c r="F38" s="5">
-        <v>27.35</v>
-      </c>
-      <c r="G38" s="5">
-        <v>5.35</v>
-      </c>
-      <c r="H38" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="I38" s="5"/>
-      <c r="J38" s="5"/>
-      <c r="K38" s="5"/>
-    </row>
-    <row r="39" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A39" s="5">
-        <v>38</v>
-      </c>
-      <c r="B39" s="5" t="str">
-        <f t="shared" si="1"/>
-        <v>AGB_dg_ev_wet_closed</v>
-      </c>
-      <c r="C39" s="5" t="s">
-        <v>81</v>
-      </c>
-      <c r="D39" s="5" t="s">
-        <v>75</v>
-      </c>
-      <c r="E39" s="5" t="s">
-        <v>46</v>
-      </c>
-      <c r="F39" s="5">
-        <v>81.28</v>
-      </c>
-      <c r="G39" s="5">
-        <v>43.43</v>
-      </c>
-      <c r="H39" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="I39" s="5"/>
-      <c r="J39" s="5"/>
-      <c r="K39" s="5"/>
-    </row>
-    <row r="40" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A40" s="5">
-        <v>39</v>
-      </c>
-      <c r="B40" s="5" t="str">
-        <f t="shared" si="1"/>
-        <v>AGB_dg_ev_moist_closed</v>
-      </c>
-      <c r="C40" s="5" t="s">
-        <v>82</v>
-      </c>
-      <c r="D40" s="5" t="s">
-        <v>76</v>
-      </c>
-      <c r="E40" s="5" t="s">
-        <v>46</v>
-      </c>
-      <c r="F40" s="5">
-        <v>202.85</v>
-      </c>
-      <c r="G40" s="5">
-        <v>41.5</v>
-      </c>
-      <c r="H40" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="I40" s="5"/>
-      <c r="J40" s="5"/>
-      <c r="K40" s="5"/>
-    </row>
-    <row r="41" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A41" s="5">
-        <v>40</v>
-      </c>
-      <c r="B41" s="5" t="str">
-        <f t="shared" si="1"/>
-        <v>AGB_dg_md_moist_closed_se</v>
-      </c>
-      <c r="C41" s="5" t="s">
-        <v>83</v>
-      </c>
-      <c r="D41" s="5" t="s">
-        <v>77</v>
-      </c>
-      <c r="E41" s="5" t="s">
-        <v>46</v>
-      </c>
-      <c r="F41" s="5">
-        <v>100.46</v>
-      </c>
-      <c r="G41" s="5">
-        <v>35.29</v>
-      </c>
-      <c r="H41" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="I41" s="5"/>
-      <c r="J41" s="5"/>
-      <c r="K41" s="5"/>
-    </row>
-    <row r="42" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A42" s="5">
-        <v>41</v>
-      </c>
-      <c r="B42" s="5" t="str">
-        <f t="shared" si="1"/>
-        <v>AGB_dg_md_moist_closed_nw</v>
-      </c>
-      <c r="C42" s="5" t="s">
-        <v>84</v>
-      </c>
-      <c r="D42" s="5" t="s">
-        <v>78</v>
-      </c>
-      <c r="E42" s="5" t="s">
-        <v>46</v>
-      </c>
-      <c r="F42" s="5">
-        <v>75.91</v>
-      </c>
-      <c r="G42" s="5">
-        <v>11</v>
-      </c>
-      <c r="H42" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="I42" s="5"/>
-      <c r="J42" s="5"/>
-      <c r="K42" s="5"/>
-    </row>
-    <row r="43" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A43" s="5">
-        <v>42</v>
-      </c>
-      <c r="B43" s="5" t="str">
-        <f t="shared" si="1"/>
-        <v>AGB_dg_ev_upland</v>
-      </c>
-      <c r="C43" s="5" t="s">
-        <v>85</v>
-      </c>
-      <c r="D43" s="5" t="s">
-        <v>79</v>
-      </c>
-      <c r="E43" s="5" t="s">
-        <v>46</v>
-      </c>
-      <c r="F43" s="5">
-        <v>74.599999999999994</v>
-      </c>
-      <c r="G43" s="5">
-        <v>13.87</v>
-      </c>
-      <c r="H43" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="I43" s="5"/>
-      <c r="J43" s="5"/>
-      <c r="K43" s="5"/>
-    </row>
-    <row r="44" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A44" s="6">
-        <v>43</v>
-      </c>
-      <c r="B44" s="6" t="str">
-        <f t="shared" si="1"/>
-        <v>BGB_dg_open</v>
-      </c>
-      <c r="C44" s="6" t="s">
-        <v>73</v>
-      </c>
-      <c r="D44" s="6" t="s">
-        <v>74</v>
-      </c>
-      <c r="E44" s="6" t="s">
-        <v>48</v>
-      </c>
-      <c r="F44" s="6">
-        <v>10.37</v>
-      </c>
-      <c r="G44" s="6">
-        <v>1.85</v>
-      </c>
-      <c r="H44" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="I44" s="6"/>
-      <c r="J44" s="6"/>
-      <c r="K44" s="6"/>
-    </row>
-    <row r="45" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A45" s="6">
-        <v>44</v>
-      </c>
-      <c r="B45" s="6" t="str">
-        <f t="shared" si="1"/>
-        <v>BGB_dg_ev_wet_closed</v>
-      </c>
-      <c r="C45" s="6" t="s">
-        <v>81</v>
-      </c>
-      <c r="D45" s="6" t="s">
-        <v>75</v>
-      </c>
-      <c r="E45" s="6" t="s">
-        <v>48</v>
-      </c>
-      <c r="F45" s="6">
-        <v>10.5</v>
-      </c>
-      <c r="G45" s="6">
-        <v>4.99</v>
-      </c>
-      <c r="H45" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="I45" s="6"/>
-      <c r="J45" s="6"/>
-      <c r="K45" s="6"/>
-    </row>
-    <row r="46" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A46" s="6">
-        <v>45</v>
-      </c>
-      <c r="B46" s="6" t="str">
-        <f t="shared" si="1"/>
-        <v>BGB_dg_ev_moist_closed</v>
-      </c>
-      <c r="C46" s="6" t="s">
-        <v>82</v>
-      </c>
-      <c r="D46" s="6" t="s">
-        <v>76</v>
-      </c>
-      <c r="E46" s="6" t="s">
-        <v>48</v>
-      </c>
-      <c r="F46" s="6">
-        <v>26.78</v>
-      </c>
-      <c r="G46" s="6">
-        <v>5.56</v>
-      </c>
-      <c r="H46" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="I46" s="6"/>
-      <c r="J46" s="6"/>
-      <c r="K46" s="6"/>
-    </row>
-    <row r="47" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A47" s="6">
-        <v>46</v>
-      </c>
-      <c r="B47" s="6" t="str">
-        <f t="shared" si="1"/>
-        <v>BGB_dg_md_moist_closed_se</v>
-      </c>
-      <c r="C47" s="6" t="s">
-        <v>83</v>
-      </c>
-      <c r="D47" s="6" t="s">
-        <v>77</v>
-      </c>
-      <c r="E47" s="6" t="s">
-        <v>48</v>
-      </c>
-      <c r="F47" s="6">
-        <v>25.85</v>
-      </c>
-      <c r="G47" s="6">
-        <v>3.62</v>
-      </c>
-      <c r="H47" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="I47" s="6"/>
-      <c r="J47" s="6"/>
-      <c r="K47" s="6"/>
-    </row>
-    <row r="48" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A48" s="6">
-        <v>47</v>
-      </c>
-      <c r="B48" s="6" t="str">
-        <f t="shared" si="1"/>
-        <v>BGB_dg_md_moist_closed_nw</v>
-      </c>
-      <c r="C48" s="6" t="s">
-        <v>84</v>
-      </c>
-      <c r="D48" s="6" t="s">
-        <v>78</v>
-      </c>
-      <c r="E48" s="6" t="s">
-        <v>48</v>
-      </c>
-      <c r="F48" s="6">
-        <v>18.989999999999998</v>
-      </c>
-      <c r="G48" s="6">
-        <v>2.13</v>
-      </c>
-      <c r="H48" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="I48" s="6"/>
-      <c r="J48" s="6"/>
-      <c r="K48" s="6"/>
-    </row>
-    <row r="49" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A49" s="6">
-        <v>48</v>
-      </c>
-      <c r="B49" s="6" t="str">
-        <f t="shared" si="1"/>
-        <v>BGB_dg_ev_upland</v>
-      </c>
-      <c r="C49" s="6" t="s">
-        <v>85</v>
-      </c>
-      <c r="D49" s="6" t="s">
-        <v>79</v>
-      </c>
-      <c r="E49" s="6" t="s">
-        <v>48</v>
-      </c>
-      <c r="F49" s="6">
-        <v>24.09</v>
-      </c>
-      <c r="G49" s="6">
-        <v>2.6</v>
-      </c>
-      <c r="H49" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="I49" s="6"/>
-      <c r="J49" s="6"/>
-      <c r="K49" s="6"/>
-    </row>
-    <row r="50" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A50" s="5">
-        <v>49</v>
-      </c>
-      <c r="B50" s="5" t="str">
-        <f t="shared" si="1"/>
-        <v>DW_dg_open</v>
-      </c>
-      <c r="C50" s="5" t="s">
-        <v>73</v>
-      </c>
-      <c r="D50" s="5" t="s">
-        <v>74</v>
-      </c>
-      <c r="E50" s="5" t="s">
-        <v>49</v>
-      </c>
-      <c r="F50" s="5">
-        <v>20.5</v>
-      </c>
-      <c r="G50" s="5">
-        <v>4.68</v>
-      </c>
-      <c r="H50" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="I50" s="5"/>
-      <c r="J50" s="5"/>
-      <c r="K50" s="5"/>
-    </row>
-    <row r="51" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A51" s="5">
-        <v>50</v>
-      </c>
-      <c r="B51" s="5" t="str">
-        <f t="shared" si="1"/>
-        <v>DW_s</v>
-      </c>
-      <c r="C51" s="5" t="s">
-        <v>98</v>
-      </c>
-      <c r="D51" s="5" t="s">
-        <v>75</v>
-      </c>
-      <c r="E51" s="5" t="s">
-        <v>49</v>
-      </c>
-      <c r="F51" s="5">
-        <v>28.97</v>
-      </c>
-      <c r="G51" s="5">
-        <v>24.34</v>
-      </c>
-      <c r="H51" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="I51" s="5"/>
-      <c r="J51" s="5"/>
-      <c r="K51" s="5"/>
-    </row>
-    <row r="52" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A52" s="5">
-        <v>51</v>
-      </c>
-      <c r="B52" s="5" t="str">
-        <f t="shared" si="1"/>
-        <v>DW_dg_ev_moist_closed</v>
-      </c>
-      <c r="C52" s="5" t="s">
-        <v>82</v>
-      </c>
-      <c r="D52" s="5" t="s">
-        <v>76</v>
-      </c>
-      <c r="E52" s="5" t="s">
-        <v>49</v>
-      </c>
-      <c r="F52" s="5">
-        <v>18.29</v>
-      </c>
-      <c r="G52" s="5">
-        <v>7.1</v>
-      </c>
-      <c r="H52" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="I52" s="5"/>
-      <c r="J52" s="5"/>
-      <c r="K52" s="5"/>
-    </row>
-    <row r="53" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A53" s="5">
-        <v>52</v>
-      </c>
-      <c r="B53" s="5" t="str">
-        <f t="shared" si="1"/>
-        <v>DW_dg_md_moist_closed_se</v>
-      </c>
-      <c r="C53" s="5" t="s">
-        <v>83</v>
-      </c>
-      <c r="D53" s="5" t="s">
-        <v>77</v>
-      </c>
-      <c r="E53" s="5" t="s">
-        <v>49</v>
-      </c>
-      <c r="F53" s="5">
-        <v>65.83</v>
-      </c>
-      <c r="G53" s="5">
-        <v>24.52</v>
-      </c>
-      <c r="H53" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="I53" s="5"/>
-      <c r="J53" s="5"/>
-      <c r="K53" s="5"/>
-    </row>
-    <row r="54" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A54" s="5">
-        <v>53</v>
-      </c>
-      <c r="B54" s="5" t="str">
-        <f t="shared" si="1"/>
-        <v>DW_dg_md_moist_closed_nw</v>
-      </c>
-      <c r="C54" s="5" t="s">
-        <v>84</v>
-      </c>
-      <c r="D54" s="5" t="s">
-        <v>78</v>
-      </c>
-      <c r="E54" s="5" t="s">
-        <v>49</v>
-      </c>
-      <c r="F54" s="5">
-        <v>38.619999999999997</v>
-      </c>
-      <c r="G54" s="5">
-        <v>7.39</v>
-      </c>
-      <c r="H54" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="I54" s="5"/>
-      <c r="J54" s="5"/>
-      <c r="K54" s="5"/>
-    </row>
-    <row r="55" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A55" s="5">
-        <v>54</v>
-      </c>
-      <c r="B55" s="5" t="str">
-        <f t="shared" si="1"/>
-        <v>DW_dg_ev_upland</v>
-      </c>
-      <c r="C55" s="5" t="s">
-        <v>85</v>
-      </c>
-      <c r="D55" s="5" t="s">
-        <v>79</v>
-      </c>
-      <c r="E55" s="5" t="s">
-        <v>49</v>
-      </c>
-      <c r="F55" s="5">
-        <v>41.93</v>
-      </c>
-      <c r="G55" s="5">
-        <v>15.59</v>
-      </c>
-      <c r="H55" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="I55" s="5"/>
-      <c r="J55" s="5"/>
-      <c r="K55" s="5"/>
-    </row>
-    <row r="56" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A56" s="6">
-        <v>55</v>
-      </c>
-      <c r="B56" s="6" t="str">
-        <f t="shared" si="1"/>
-        <v>DG_ratio_dg_open</v>
-      </c>
-      <c r="C56" s="6" t="s">
-        <v>73</v>
-      </c>
-      <c r="D56" s="6" t="s">
-        <v>74</v>
-      </c>
-      <c r="E56" s="6" t="s">
-        <v>80</v>
-      </c>
-      <c r="F56" s="6"/>
-      <c r="G56" s="6"/>
-      <c r="H56" s="6" t="s">
-        <v>87</v>
-      </c>
-      <c r="I56" s="6">
-        <f>1-0.48</f>
-        <v>0.52</v>
-      </c>
-      <c r="J56" s="6">
-        <v>7.2999999999999995E-2</v>
-      </c>
-      <c r="K56" s="6"/>
-    </row>
-    <row r="57" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A57" s="6">
-        <v>56</v>
-      </c>
-      <c r="B57" s="6" t="str">
-        <f t="shared" si="1"/>
-        <v>DG_ratio_dg_ev_wet_closed</v>
-      </c>
-      <c r="C57" s="6" t="s">
-        <v>81</v>
-      </c>
-      <c r="D57" s="6" t="s">
-        <v>75</v>
-      </c>
-      <c r="E57" s="6" t="s">
-        <v>80</v>
-      </c>
-      <c r="F57" s="6"/>
-      <c r="G57" s="6"/>
-      <c r="H57" s="6" t="s">
-        <v>87</v>
-      </c>
-      <c r="I57" s="6">
-        <f>1-0.3</f>
-        <v>0.7</v>
-      </c>
-      <c r="J57" s="6">
-        <v>2.5999999999999999E-2</v>
-      </c>
-      <c r="K57" s="6"/>
-    </row>
-    <row r="58" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A58" s="6">
-        <v>57</v>
-      </c>
-      <c r="B58" s="6" t="str">
-        <f t="shared" si="1"/>
-        <v>DG_ratio_dg_ev_moist_closed</v>
-      </c>
-      <c r="C58" s="6" t="s">
-        <v>82</v>
-      </c>
-      <c r="D58" s="6" t="s">
-        <v>76</v>
-      </c>
-      <c r="E58" s="6" t="s">
-        <v>80</v>
-      </c>
-      <c r="F58" s="6"/>
-      <c r="G58" s="6"/>
-      <c r="H58" s="6" t="s">
-        <v>87</v>
-      </c>
-      <c r="I58" s="6">
-        <f t="shared" ref="I58:I61" si="2">1-0.3</f>
-        <v>0.7</v>
-      </c>
-      <c r="J58" s="6">
-        <v>2.5999999999999999E-2</v>
-      </c>
-      <c r="K58" s="6"/>
-    </row>
-    <row r="59" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A59" s="6">
-        <v>58</v>
-      </c>
-      <c r="B59" s="6" t="str">
-        <f t="shared" si="1"/>
-        <v>DG_ratio_dg_md_moist_closed_se</v>
-      </c>
-      <c r="C59" s="6" t="s">
-        <v>83</v>
-      </c>
-      <c r="D59" s="6" t="s">
-        <v>77</v>
-      </c>
-      <c r="E59" s="6" t="s">
-        <v>80</v>
-      </c>
-      <c r="F59" s="6"/>
-      <c r="G59" s="6"/>
-      <c r="H59" s="6" t="s">
-        <v>87</v>
-      </c>
-      <c r="I59" s="6">
-        <f t="shared" si="2"/>
-        <v>0.7</v>
-      </c>
-      <c r="J59" s="6">
-        <v>2.5999999999999999E-2</v>
-      </c>
-      <c r="K59" s="6"/>
-    </row>
-    <row r="60" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A60" s="6">
-        <v>59</v>
-      </c>
-      <c r="B60" s="6" t="str">
-        <f t="shared" si="1"/>
-        <v>DG_ratio_dg_md_moist_closed_nw</v>
-      </c>
-      <c r="C60" s="6" t="s">
-        <v>84</v>
-      </c>
-      <c r="D60" s="6" t="s">
-        <v>78</v>
-      </c>
-      <c r="E60" s="6" t="s">
-        <v>80</v>
-      </c>
-      <c r="F60" s="6"/>
-      <c r="G60" s="6"/>
-      <c r="H60" s="6" t="s">
-        <v>87</v>
-      </c>
-      <c r="I60" s="6">
-        <f t="shared" si="2"/>
-        <v>0.7</v>
-      </c>
-      <c r="J60" s="6">
-        <v>2.5999999999999999E-2</v>
-      </c>
-      <c r="K60" s="6"/>
-    </row>
-    <row r="61" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A61" s="6">
-        <v>60</v>
-      </c>
-      <c r="B61" s="6" t="str">
-        <f t="shared" si="1"/>
-        <v>DG_ratio_dg_ev_upland</v>
-      </c>
-      <c r="C61" s="6" t="s">
-        <v>85</v>
-      </c>
-      <c r="D61" s="6" t="s">
-        <v>79</v>
-      </c>
-      <c r="E61" s="6" t="s">
-        <v>80</v>
-      </c>
-      <c r="F61" s="6"/>
-      <c r="G61" s="6"/>
-      <c r="H61" s="6" t="s">
-        <v>87</v>
-      </c>
-      <c r="I61" s="6">
-        <f t="shared" si="2"/>
-        <v>0.7</v>
-      </c>
-      <c r="J61" s="6">
-        <v>2.5999999999999999E-2</v>
-      </c>
-      <c r="K61" s="6"/>
-    </row>
-  </sheetData>
-  <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="E2:E55" xr:uid="{C8AAE3E1-51FC-6E43-8297-A59F04991BBC}">
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="F2:F37" xr:uid="{3D7EF7D9-A43C-A04A-950F-6332D8AE5CD1}">
       <formula1>"AGB,BGB,DW,LI,SOC,ALL"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
Added forest to LU and first draft of LU matrix done
</commit_message>
<xml_diff>
--- a/inst/extdata/example1.xlsx
+++ b/inst/extdata/example1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/gaelsola/Github-Collabs/mocaredd/inst/extdata/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DE622DAE-D5B5-9649-83F0-538B4EB112B7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{63A626F1-E594-E54F-8B30-3EFB05C72C4D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-24640" yWindow="4740" windowWidth="22160" windowHeight="16860" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -55,7 +55,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="626" uniqueCount="101">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="626" uniqueCount="111">
   <si>
     <t>trans_no</t>
   </si>
@@ -358,6 +358,36 @@
   </si>
   <si>
     <t>c_period</t>
+  </si>
+  <si>
+    <t>Closed Wet Evergreen Forest</t>
+  </si>
+  <si>
+    <t>Closed Moist Evergreen Forest</t>
+  </si>
+  <si>
+    <t>Closed Moist Semideciduous SE Forest</t>
+  </si>
+  <si>
+    <t>Closed Moist Semideciduous NW Forest</t>
+  </si>
+  <si>
+    <t>Closed Upland Evergreen Forest</t>
+  </si>
+  <si>
+    <t>Degraded Closed Wet Evergreen Forest</t>
+  </si>
+  <si>
+    <t>Degraded Closed Moist Evergreen Forest</t>
+  </si>
+  <si>
+    <t>Degraded Closed Moist Semideciduous SE Forest</t>
+  </si>
+  <si>
+    <t>Degraded Closed Moist Semideciduous NW Forest</t>
+  </si>
+  <si>
+    <t>Degraded Closed Upland Evergreen Forest</t>
   </si>
 </sst>
 </file>
@@ -2950,8 +2980,8 @@
   </sheetPr>
   <dimension ref="A1:L43"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="109" workbookViewId="0">
-      <selection activeCell="B32" sqref="B32"/>
+    <sheetView tabSelected="1" topLeftCell="A11" zoomScale="109" workbookViewId="0">
+      <selection activeCell="E45" sqref="E45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -3054,7 +3084,7 @@
         <v>19</v>
       </c>
       <c r="E3" s="5" t="s">
-        <v>20</v>
+        <v>101</v>
       </c>
       <c r="F3" s="5" t="s">
         <v>46</v>
@@ -3087,7 +3117,7 @@
         <v>22</v>
       </c>
       <c r="E4" s="5" t="s">
-        <v>23</v>
+        <v>102</v>
       </c>
       <c r="F4" s="5" t="s">
         <v>46</v>
@@ -3120,7 +3150,7 @@
         <v>25</v>
       </c>
       <c r="E5" s="5" t="s">
-        <v>26</v>
+        <v>103</v>
       </c>
       <c r="F5" s="5" t="s">
         <v>46</v>
@@ -3153,7 +3183,7 @@
         <v>28</v>
       </c>
       <c r="E6" s="5" t="s">
-        <v>29</v>
+        <v>104</v>
       </c>
       <c r="F6" s="5" t="s">
         <v>46</v>
@@ -3186,7 +3216,7 @@
         <v>31</v>
       </c>
       <c r="E7" s="5" t="s">
-        <v>32</v>
+        <v>105</v>
       </c>
       <c r="F7" s="5" t="s">
         <v>46</v>
@@ -3252,7 +3282,7 @@
         <v>19</v>
       </c>
       <c r="E9" s="6" t="s">
-        <v>20</v>
+        <v>101</v>
       </c>
       <c r="F9" s="6" t="s">
         <v>48</v>
@@ -3285,7 +3315,7 @@
         <v>22</v>
       </c>
       <c r="E10" s="6" t="s">
-        <v>23</v>
+        <v>102</v>
       </c>
       <c r="F10" s="6" t="s">
         <v>48</v>
@@ -3318,7 +3348,7 @@
         <v>25</v>
       </c>
       <c r="E11" s="6" t="s">
-        <v>26</v>
+        <v>103</v>
       </c>
       <c r="F11" s="6" t="s">
         <v>48</v>
@@ -3351,7 +3381,7 @@
         <v>28</v>
       </c>
       <c r="E12" s="6" t="s">
-        <v>29</v>
+        <v>104</v>
       </c>
       <c r="F12" s="6" t="s">
         <v>48</v>
@@ -3384,7 +3414,7 @@
         <v>31</v>
       </c>
       <c r="E13" s="6" t="s">
-        <v>32</v>
+        <v>105</v>
       </c>
       <c r="F13" s="6" t="s">
         <v>48</v>
@@ -3450,7 +3480,7 @@
         <v>19</v>
       </c>
       <c r="E15" s="5" t="s">
-        <v>20</v>
+        <v>101</v>
       </c>
       <c r="F15" s="5" t="s">
         <v>49</v>
@@ -3483,7 +3513,7 @@
         <v>22</v>
       </c>
       <c r="E16" s="5" t="s">
-        <v>23</v>
+        <v>102</v>
       </c>
       <c r="F16" s="5" t="s">
         <v>49</v>
@@ -3516,7 +3546,7 @@
         <v>25</v>
       </c>
       <c r="E17" s="5" t="s">
-        <v>26</v>
+        <v>103</v>
       </c>
       <c r="F17" s="5" t="s">
         <v>49</v>
@@ -3549,7 +3579,7 @@
         <v>28</v>
       </c>
       <c r="E18" s="5" t="s">
-        <v>29</v>
+        <v>104</v>
       </c>
       <c r="F18" s="5" t="s">
         <v>49</v>
@@ -3582,7 +3612,7 @@
         <v>31</v>
       </c>
       <c r="E19" s="5" t="s">
-        <v>32</v>
+        <v>105</v>
       </c>
       <c r="F19" s="5" t="s">
         <v>49</v>
@@ -3648,7 +3678,7 @@
         <v>19</v>
       </c>
       <c r="E21" s="6" t="s">
-        <v>20</v>
+        <v>101</v>
       </c>
       <c r="F21" s="6" t="s">
         <v>50</v>
@@ -3681,7 +3711,7 @@
         <v>22</v>
       </c>
       <c r="E22" s="6" t="s">
-        <v>23</v>
+        <v>102</v>
       </c>
       <c r="F22" s="6" t="s">
         <v>50</v>
@@ -3714,7 +3744,7 @@
         <v>25</v>
       </c>
       <c r="E23" s="6" t="s">
-        <v>26</v>
+        <v>103</v>
       </c>
       <c r="F23" s="6" t="s">
         <v>50</v>
@@ -3747,7 +3777,7 @@
         <v>28</v>
       </c>
       <c r="E24" s="6" t="s">
-        <v>29</v>
+        <v>104</v>
       </c>
       <c r="F24" s="6" t="s">
         <v>50</v>
@@ -3780,7 +3810,7 @@
         <v>31</v>
       </c>
       <c r="E25" s="6" t="s">
-        <v>32</v>
+        <v>105</v>
       </c>
       <c r="F25" s="6" t="s">
         <v>50</v>
@@ -3846,7 +3876,7 @@
         <v>19</v>
       </c>
       <c r="E27" s="5" t="s">
-        <v>20</v>
+        <v>101</v>
       </c>
       <c r="F27" s="5" t="s">
         <v>51</v>
@@ -3879,7 +3909,7 @@
         <v>22</v>
       </c>
       <c r="E28" s="5" t="s">
-        <v>23</v>
+        <v>102</v>
       </c>
       <c r="F28" s="5" t="s">
         <v>51</v>
@@ -3912,7 +3942,7 @@
         <v>25</v>
       </c>
       <c r="E29" s="5" t="s">
-        <v>26</v>
+        <v>103</v>
       </c>
       <c r="F29" s="5" t="s">
         <v>51</v>
@@ -3945,7 +3975,7 @@
         <v>28</v>
       </c>
       <c r="E30" s="5" t="s">
-        <v>29</v>
+        <v>104</v>
       </c>
       <c r="F30" s="5" t="s">
         <v>51</v>
@@ -3978,7 +4008,7 @@
         <v>31</v>
       </c>
       <c r="E31" s="5" t="s">
-        <v>32</v>
+        <v>105</v>
       </c>
       <c r="F31" s="5" t="s">
         <v>51</v>
@@ -4249,7 +4279,7 @@
         <v>81</v>
       </c>
       <c r="E39" s="18" t="s">
-        <v>75</v>
+        <v>106</v>
       </c>
       <c r="F39" s="18" t="s">
         <v>80</v>
@@ -4289,7 +4319,7 @@
         <v>82</v>
       </c>
       <c r="E40" s="18" t="s">
-        <v>76</v>
+        <v>107</v>
       </c>
       <c r="F40" s="18" t="s">
         <v>80</v>
@@ -4329,7 +4359,7 @@
         <v>83</v>
       </c>
       <c r="E41" s="18" t="s">
-        <v>77</v>
+        <v>108</v>
       </c>
       <c r="F41" s="18" t="s">
         <v>80</v>
@@ -4369,7 +4399,7 @@
         <v>84</v>
       </c>
       <c r="E42" s="18" t="s">
-        <v>78</v>
+        <v>109</v>
       </c>
       <c r="F42" s="18" t="s">
         <v>80</v>
@@ -4409,7 +4439,7 @@
         <v>85</v>
       </c>
       <c r="E43" s="18" t="s">
-        <v>79</v>
+        <v>110</v>
       </c>
       <c r="F43" s="18" t="s">
         <v>80</v>

</xml_diff>

<commit_message>
added initial simulation results
</commit_message>
<xml_diff>
--- a/inst/extdata/example1.xlsx
+++ b/inst/extdata/example1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/gaelsola/Github-Collabs/mocaredd/inst/extdata/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{63A626F1-E594-E54F-8B30-3EFB05C72C4D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F7B3AABF-C4FE-624D-8D57-D3EAE3A867C2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-24640" yWindow="4740" windowWidth="22160" windowHeight="16860" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3980" yWindow="1760" windowWidth="22160" windowHeight="16860" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="user_input_details" sheetId="6" r:id="rId1"/>
@@ -1040,8 +1040,8 @@
   </sheetPr>
   <dimension ref="A1:N49"/>
   <sheetViews>
-    <sheetView topLeftCell="A33" zoomScale="127" workbookViewId="0">
-      <selection activeCell="F60" sqref="F60"/>
+    <sheetView tabSelected="1" zoomScale="127" workbookViewId="0">
+      <selection activeCell="E38" sqref="E38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -2980,7 +2980,7 @@
   </sheetPr>
   <dimension ref="A1:L43"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A11" zoomScale="109" workbookViewId="0">
+    <sheetView topLeftCell="A11" zoomScale="109" workbookViewId="0">
       <selection activeCell="E45" sqref="E45"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
split mcs_C function into mcs_cpools and msc_cstock plus integrate with mcs_E. Remove dg_expool from usr, now systematic
</commit_message>
<xml_diff>
--- a/inst/extdata/example1.xlsx
+++ b/inst/extdata/example1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/gaelsola/Github-Collabs/mocaredd/inst/extdata/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F7B3AABF-C4FE-624D-8D57-D3EAE3A867C2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{555DCE12-2679-D942-B1A8-198BAD468BE5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3980" yWindow="1760" windowWidth="22160" windowHeight="16860" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-26260" yWindow="10920" windowWidth="26260" windowHeight="16860" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="user_input_details" sheetId="6" r:id="rId1"/>
@@ -342,9 +342,6 @@
     <t>Excluded pools from degradation (TRUE or FALSE). If TRUE the pools not listed in dg_pool will be excluded when calculating the initial vs final Cstocks</t>
   </si>
   <si>
-    <t>If degradation is a ratio of intact forest Cstock, list of pools separated by coma. Any combination of AGB, BGB, DW, LI, SOC</t>
-  </si>
-  <si>
     <t>AGB, BGB, DW</t>
   </si>
   <si>
@@ -388,13 +385,16 @@
   </si>
   <si>
     <t>Degraded Closed Upland Evergreen Forest</t>
+  </si>
+  <si>
+    <t>If degradation is a ratio of intact forest Cstock, list of pools separated by coma. Any combination of AGB, BGB, DW, LI, SOC or NA if not applicable. Note: the pools not listed in dg_pool will be excluded when calculating the initial vs final Cstocks</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -433,6 +433,14 @@
       <b/>
       <sz val="12"/>
       <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="10"/>
+      <color theme="0" tint="-0.14999847407452621"/>
       <name val="Arial"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -518,7 +526,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -545,6 +553,10 @@
     <xf numFmtId="0" fontId="2" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -778,8 +790,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{71C5FFA2-A875-134F-9BDA-F112D638328C}">
   <dimension ref="A1:B9"/>
   <sheetViews>
-    <sheetView zoomScale="190" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+    <sheetView tabSelected="1" zoomScale="190" workbookViewId="0">
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -828,19 +840,19 @@
         <v>69</v>
       </c>
     </row>
-    <row r="6" spans="1:2" ht="28" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:2" ht="42" x14ac:dyDescent="0.15">
       <c r="A6" s="7" t="s">
         <v>93</v>
       </c>
       <c r="B6" s="19" t="s">
-        <v>95</v>
+        <v>110</v>
       </c>
     </row>
     <row r="7" spans="1:2" ht="28" x14ac:dyDescent="0.15">
-      <c r="A7" s="7" t="s">
+      <c r="A7" s="20" t="s">
         <v>92</v>
       </c>
-      <c r="B7" s="19" t="s">
+      <c r="B7" s="21" t="s">
         <v>94</v>
       </c>
     </row>
@@ -928,7 +940,7 @@
         <v>52</v>
       </c>
       <c r="F2" s="7" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="G2" t="b">
         <v>1</v>
@@ -983,7 +995,7 @@
         <v>2014</v>
       </c>
       <c r="D2" s="7" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.15">
@@ -997,7 +1009,7 @@
         <v>2019</v>
       </c>
       <c r="D3" s="7" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.15">
@@ -1011,7 +1023,7 @@
         <v>2020</v>
       </c>
       <c r="D4" s="7" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.15">
@@ -1025,7 +1037,7 @@
         <v>2021</v>
       </c>
       <c r="D5" s="7" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
   </sheetData>
@@ -1040,7 +1052,7 @@
   </sheetPr>
   <dimension ref="A1:N49"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="127" workbookViewId="0">
+    <sheetView topLeftCell="A24" zoomScale="127" workbookViewId="0">
       <selection activeCell="E38" sqref="E38"/>
     </sheetView>
   </sheetViews>
@@ -3006,7 +3018,7 @@
         <v>36</v>
       </c>
       <c r="C1" s="8" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="D1" s="8" t="s">
         <v>37</v>
@@ -3084,7 +3096,7 @@
         <v>19</v>
       </c>
       <c r="E3" s="5" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="F3" s="5" t="s">
         <v>46</v>
@@ -3117,7 +3129,7 @@
         <v>22</v>
       </c>
       <c r="E4" s="5" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="F4" s="5" t="s">
         <v>46</v>
@@ -3150,7 +3162,7 @@
         <v>25</v>
       </c>
       <c r="E5" s="5" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="F5" s="5" t="s">
         <v>46</v>
@@ -3183,7 +3195,7 @@
         <v>28</v>
       </c>
       <c r="E6" s="5" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="F6" s="5" t="s">
         <v>46</v>
@@ -3216,7 +3228,7 @@
         <v>31</v>
       </c>
       <c r="E7" s="5" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="F7" s="5" t="s">
         <v>46</v>
@@ -3282,7 +3294,7 @@
         <v>19</v>
       </c>
       <c r="E9" s="6" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="F9" s="6" t="s">
         <v>48</v>
@@ -3315,7 +3327,7 @@
         <v>22</v>
       </c>
       <c r="E10" s="6" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="F10" s="6" t="s">
         <v>48</v>
@@ -3348,7 +3360,7 @@
         <v>25</v>
       </c>
       <c r="E11" s="6" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="F11" s="6" t="s">
         <v>48</v>
@@ -3381,7 +3393,7 @@
         <v>28</v>
       </c>
       <c r="E12" s="6" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="F12" s="6" t="s">
         <v>48</v>
@@ -3414,7 +3426,7 @@
         <v>31</v>
       </c>
       <c r="E13" s="6" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="F13" s="6" t="s">
         <v>48</v>
@@ -3480,7 +3492,7 @@
         <v>19</v>
       </c>
       <c r="E15" s="5" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="F15" s="5" t="s">
         <v>49</v>
@@ -3513,7 +3525,7 @@
         <v>22</v>
       </c>
       <c r="E16" s="5" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="F16" s="5" t="s">
         <v>49</v>
@@ -3546,7 +3558,7 @@
         <v>25</v>
       </c>
       <c r="E17" s="5" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="F17" s="5" t="s">
         <v>49</v>
@@ -3579,7 +3591,7 @@
         <v>28</v>
       </c>
       <c r="E18" s="5" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="F18" s="5" t="s">
         <v>49</v>
@@ -3612,7 +3624,7 @@
         <v>31</v>
       </c>
       <c r="E19" s="5" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="F19" s="5" t="s">
         <v>49</v>
@@ -3678,7 +3690,7 @@
         <v>19</v>
       </c>
       <c r="E21" s="6" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="F21" s="6" t="s">
         <v>50</v>
@@ -3711,7 +3723,7 @@
         <v>22</v>
       </c>
       <c r="E22" s="6" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="F22" s="6" t="s">
         <v>50</v>
@@ -3744,7 +3756,7 @@
         <v>25</v>
       </c>
       <c r="E23" s="6" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="F23" s="6" t="s">
         <v>50</v>
@@ -3777,7 +3789,7 @@
         <v>28</v>
       </c>
       <c r="E24" s="6" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="F24" s="6" t="s">
         <v>50</v>
@@ -3810,7 +3822,7 @@
         <v>31</v>
       </c>
       <c r="E25" s="6" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="F25" s="6" t="s">
         <v>50</v>
@@ -3876,7 +3888,7 @@
         <v>19</v>
       </c>
       <c r="E27" s="5" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="F27" s="5" t="s">
         <v>51</v>
@@ -3909,7 +3921,7 @@
         <v>22</v>
       </c>
       <c r="E28" s="5" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="F28" s="5" t="s">
         <v>51</v>
@@ -3942,7 +3954,7 @@
         <v>25</v>
       </c>
       <c r="E29" s="5" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="F29" s="5" t="s">
         <v>51</v>
@@ -3975,7 +3987,7 @@
         <v>28</v>
       </c>
       <c r="E30" s="5" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="F30" s="5" t="s">
         <v>51</v>
@@ -4008,7 +4020,7 @@
         <v>31</v>
       </c>
       <c r="E31" s="5" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="F31" s="5" t="s">
         <v>51</v>
@@ -4279,7 +4291,7 @@
         <v>81</v>
       </c>
       <c r="E39" s="18" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="F39" s="18" t="s">
         <v>80</v>
@@ -4319,7 +4331,7 @@
         <v>82</v>
       </c>
       <c r="E40" s="18" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="F40" s="18" t="s">
         <v>80</v>
@@ -4359,7 +4371,7 @@
         <v>83</v>
       </c>
       <c r="E41" s="18" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="F41" s="18" t="s">
         <v>80</v>
@@ -4399,7 +4411,7 @@
         <v>84</v>
       </c>
       <c r="E42" s="18" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="F42" s="18" t="s">
         <v>80</v>
@@ -4439,7 +4451,7 @@
         <v>85</v>
       </c>
       <c r="E43" s="18" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="F43" s="18" t="s">
         <v>80</v>

</xml_diff>